<commit_message>
new predictions, sheet messed up due to incomplete changes to make_predictions.py
</commit_message>
<xml_diff>
--- a/data/predictions.xlsx
+++ b/data/predictions.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T18"/>
+  <dimension ref="A1:Y33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -505,42 +505,69 @@
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
+          <t>home_score</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>away_score</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>winning_pitcher</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>losing_pitcher</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
           <t>prediction_value</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>venue</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>series_status</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>national_broadcasts</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>odds_retrieval_time</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>datetime</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>game_id</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>summary</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr"/>
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
       <c r="B2" t="inlineStr">
         <is>
           <t>2023-07-15</t>
@@ -581,20 +608,16 @@
           <t>San Diego Padres</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>+128</t>
-        </is>
+      <c r="J2" t="n">
+        <v>128</v>
       </c>
       <c r="K2" t="inlineStr">
         <is>
           <t>LowVig.ag</t>
         </is>
       </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>-133</t>
-        </is>
+      <c r="L2" t="n">
+        <v>-133</v>
       </c>
       <c r="M2" t="inlineStr">
         <is>
@@ -602,32 +625,43 @@
         </is>
       </c>
       <c r="N2" t="n">
+        <v>6</v>
+      </c>
+      <c r="O2" t="n">
+        <v>4</v>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>Matt Strahm</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>Tim Hill</t>
+        </is>
+      </c>
+      <c r="R2" t="n">
         <v>0.9884720883230922</v>
       </c>
-      <c r="O2" t="inlineStr">
+      <c r="S2" t="inlineStr">
         <is>
           <t>Citizens Bank Park</t>
         </is>
       </c>
-      <c r="P2" t="inlineStr"/>
-      <c r="Q2" t="inlineStr">
+      <c r="T2" t="inlineStr"/>
+      <c r="U2" t="inlineStr">
         <is>
           <t>['MLBN (out-of-market only)']</t>
         </is>
       </c>
-      <c r="R2" s="2" t="n">
-        <v>45122.40607709075</v>
-      </c>
-      <c r="S2" t="inlineStr">
-        <is>
-          <t>2023-07-15T17:05:00Z</t>
-        </is>
-      </c>
-      <c r="T2" t="inlineStr">
-        <is>
-          <t>2023-07-15 - San Diego Padres @ Philadelphia Phillies (Scheduled)</t>
-        </is>
-      </c>
+      <c r="V2" s="2" t="n">
+        <v>45122.40607709491</v>
+      </c>
+      <c r="W2" s="2" t="n">
+        <v>45122.71180555555</v>
+      </c>
+      <c r="X2" t="inlineStr"/>
+      <c r="Y2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr"/>
@@ -671,56 +705,51 @@
           <t>Tampa Bay Rays</t>
         </is>
       </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>+245</t>
-        </is>
+      <c r="J3" t="n">
+        <v>245</v>
       </c>
       <c r="K3" t="inlineStr">
         <is>
           <t>FanDuel</t>
         </is>
       </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>-263</t>
-        </is>
+      <c r="L3" t="n">
+        <v>-263</v>
       </c>
       <c r="M3" t="inlineStr">
         <is>
           <t>WynnBET</t>
         </is>
       </c>
-      <c r="N3" t="n">
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr"/>
+      <c r="P3" t="inlineStr"/>
+      <c r="Q3" t="inlineStr"/>
+      <c r="R3" t="n">
         <v>0.01030191366295862</v>
       </c>
-      <c r="O3" t="inlineStr">
+      <c r="S3" t="inlineStr">
         <is>
           <t>Kauffman Stadium</t>
         </is>
       </c>
-      <c r="P3" t="inlineStr"/>
-      <c r="Q3" t="inlineStr">
+      <c r="T3" t="inlineStr"/>
+      <c r="U3" t="inlineStr">
         <is>
           <t>[]</t>
         </is>
       </c>
-      <c r="R3" s="2" t="n">
-        <v>45122.40607709075</v>
-      </c>
-      <c r="S3" t="inlineStr">
-        <is>
-          <t>2023-07-15T00:10:00Z</t>
-        </is>
-      </c>
-      <c r="T3" t="inlineStr">
-        <is>
-          <t>2023-07-14 - Tampa Bay Rays @ Kansas City Royals (Postponed)</t>
-        </is>
-      </c>
+      <c r="V3" s="2" t="n">
+        <v>45122.40607709491</v>
+      </c>
+      <c r="W3" t="inlineStr"/>
+      <c r="X3" t="inlineStr"/>
+      <c r="Y3" t="inlineStr"/>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr"/>
+      <c r="A4" t="n">
+        <v>0</v>
+      </c>
       <c r="B4" t="inlineStr">
         <is>
           <t>2023-07-15</t>
@@ -761,20 +790,16 @@
           <t>Boston Red Sox</t>
         </is>
       </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>-105</t>
-        </is>
+      <c r="J4" t="n">
+        <v>-105</v>
       </c>
       <c r="K4" t="inlineStr">
         <is>
           <t>LowVig.ag</t>
         </is>
       </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>-103</t>
-        </is>
+      <c r="L4" t="n">
+        <v>-103</v>
       </c>
       <c r="M4" t="inlineStr">
         <is>
@@ -782,35 +807,46 @@
         </is>
       </c>
       <c r="N4" t="n">
+        <v>10</v>
+      </c>
+      <c r="O4" t="n">
+        <v>4</v>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>Marcus Stroman</t>
+        </is>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>James Paxton</t>
+        </is>
+      </c>
+      <c r="R4" t="n">
         <v>0.003209165968602913</v>
       </c>
-      <c r="O4" t="inlineStr">
+      <c r="S4" t="inlineStr">
         <is>
           <t>Wrigley Field</t>
         </is>
       </c>
-      <c r="P4" t="inlineStr"/>
-      <c r="Q4" t="inlineStr">
+      <c r="T4" t="inlineStr"/>
+      <c r="U4" t="inlineStr">
         <is>
           <t>[]</t>
         </is>
       </c>
-      <c r="R4" s="2" t="n">
-        <v>45122.40607709075</v>
-      </c>
-      <c r="S4" t="inlineStr">
-        <is>
-          <t>2023-07-15T18:20:00Z</t>
-        </is>
-      </c>
-      <c r="T4" t="inlineStr">
-        <is>
-          <t>2023-07-15 - Boston Red Sox @ Chicago Cubs (Scheduled)</t>
-        </is>
-      </c>
+      <c r="V4" s="2" t="n">
+        <v>45122.40607709491</v>
+      </c>
+      <c r="W4" t="inlineStr"/>
+      <c r="X4" t="inlineStr"/>
+      <c r="Y4" t="inlineStr"/>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr"/>
+      <c r="A5" t="n">
+        <v>0</v>
+      </c>
       <c r="B5" t="inlineStr">
         <is>
           <t>2023-07-15</t>
@@ -851,20 +887,16 @@
           <t>Toronto Blue Jays</t>
         </is>
       </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>-123</t>
-        </is>
+      <c r="J5" t="n">
+        <v>-123</v>
       </c>
       <c r="K5" t="inlineStr">
         <is>
           <t>BetOnline.ag</t>
         </is>
       </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>+118</t>
-        </is>
+      <c r="L5" t="n">
+        <v>118</v>
       </c>
       <c r="M5" t="inlineStr">
         <is>
@@ -872,39 +904,50 @@
         </is>
       </c>
       <c r="N5" t="n">
+        <v>5</v>
+      </c>
+      <c r="O5" t="n">
+        <v>2</v>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>Chris Bassitt</t>
+        </is>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>Zac Gallen</t>
+        </is>
+      </c>
+      <c r="R5" t="n">
         <v>4.910299968765712e-05</v>
       </c>
-      <c r="O5" t="inlineStr">
+      <c r="S5" t="inlineStr">
         <is>
           <t>Rogers Centre</t>
         </is>
       </c>
-      <c r="P5" t="inlineStr">
+      <c r="T5" t="inlineStr">
         <is>
           <t>TOR leads 1-0</t>
         </is>
       </c>
-      <c r="Q5" t="inlineStr">
+      <c r="U5" t="inlineStr">
         <is>
           <t>[]</t>
         </is>
       </c>
-      <c r="R5" s="2" t="n">
-        <v>45122.40607709075</v>
-      </c>
-      <c r="S5" t="inlineStr">
-        <is>
-          <t>2023-07-15T19:07:00Z</t>
-        </is>
-      </c>
-      <c r="T5" t="inlineStr">
-        <is>
-          <t>2023-07-15 - Arizona Diamondbacks @ Toronto Blue Jays (Scheduled)</t>
-        </is>
-      </c>
+      <c r="V5" s="2" t="n">
+        <v>45122.40607709491</v>
+      </c>
+      <c r="W5" t="inlineStr"/>
+      <c r="X5" t="inlineStr"/>
+      <c r="Y5" t="inlineStr"/>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr"/>
+      <c r="A6" t="n">
+        <v>0</v>
+      </c>
       <c r="B6" t="inlineStr">
         <is>
           <t>2023-07-15</t>
@@ -945,20 +988,16 @@
           <t>Texas Rangers</t>
         </is>
       </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>-145</t>
-        </is>
+      <c r="J6" t="n">
+        <v>-145</v>
       </c>
       <c r="K6" t="inlineStr">
         <is>
           <t>WynnBET</t>
         </is>
       </c>
-      <c r="L6" t="inlineStr">
-        <is>
-          <t>+140</t>
-        </is>
+      <c r="L6" t="n">
+        <v>140</v>
       </c>
       <c r="M6" t="inlineStr">
         <is>
@@ -966,35 +1005,46 @@
         </is>
       </c>
       <c r="N6" t="n">
+        <v>2</v>
+      </c>
+      <c r="O6" t="n">
+        <v>0</v>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>Andrew Heaney</t>
+        </is>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>Gavin Williams</t>
+        </is>
+      </c>
+      <c r="R6" t="n">
         <v>0.1089422418040507</v>
       </c>
-      <c r="O6" t="inlineStr">
+      <c r="S6" t="inlineStr">
         <is>
           <t>Globe Life Field</t>
         </is>
       </c>
-      <c r="P6" t="inlineStr"/>
-      <c r="Q6" t="inlineStr">
+      <c r="T6" t="inlineStr"/>
+      <c r="U6" t="inlineStr">
         <is>
           <t>['FS1']</t>
         </is>
       </c>
-      <c r="R6" s="2" t="n">
-        <v>45122.40607709075</v>
-      </c>
-      <c r="S6" t="inlineStr">
-        <is>
-          <t>2023-07-15T20:05:00Z</t>
-        </is>
-      </c>
-      <c r="T6" t="inlineStr">
-        <is>
-          <t>2023-07-15 - Cleveland Guardians @ Texas Rangers (Scheduled)</t>
-        </is>
-      </c>
+      <c r="V6" s="2" t="n">
+        <v>45122.40607709491</v>
+      </c>
+      <c r="W6" t="inlineStr"/>
+      <c r="X6" t="inlineStr"/>
+      <c r="Y6" t="inlineStr"/>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr"/>
+      <c r="A7" t="n">
+        <v>0</v>
+      </c>
       <c r="B7" t="inlineStr">
         <is>
           <t>2023-07-15</t>
@@ -1035,20 +1085,16 @@
           <t>Baltimore Orioles</t>
         </is>
       </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>-112</t>
-        </is>
+      <c r="J7" t="n">
+        <v>-112</v>
       </c>
       <c r="K7" t="inlineStr">
         <is>
           <t>WynnBET</t>
         </is>
       </c>
-      <c r="L7" t="inlineStr">
-        <is>
-          <t>+104</t>
-        </is>
+      <c r="L7" t="n">
+        <v>104</v>
       </c>
       <c r="M7" t="inlineStr">
         <is>
@@ -1056,35 +1102,46 @@
         </is>
       </c>
       <c r="N7" t="n">
+        <v>6</v>
+      </c>
+      <c r="O7" t="n">
+        <v>5</v>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>Mike Baumann</t>
+        </is>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>Huascar Brazoban</t>
+        </is>
+      </c>
+      <c r="R7" t="n">
         <v>1.884601924724619e-08</v>
       </c>
-      <c r="O7" t="inlineStr">
+      <c r="S7" t="inlineStr">
         <is>
           <t>Oriole Park at Camden Yards</t>
         </is>
       </c>
-      <c r="P7" t="inlineStr"/>
-      <c r="Q7" t="inlineStr">
+      <c r="T7" t="inlineStr"/>
+      <c r="U7" t="inlineStr">
         <is>
           <t>[]</t>
         </is>
       </c>
-      <c r="R7" s="2" t="n">
-        <v>45122.40607709075</v>
-      </c>
-      <c r="S7" t="inlineStr">
-        <is>
-          <t>2023-07-15T23:05:00Z</t>
-        </is>
-      </c>
-      <c r="T7" t="inlineStr">
-        <is>
-          <t>2023-07-15 - Miami Marlins @ Baltimore Orioles (Scheduled)</t>
-        </is>
-      </c>
+      <c r="V7" s="2" t="n">
+        <v>45122.40607709491</v>
+      </c>
+      <c r="W7" t="inlineStr"/>
+      <c r="X7" t="inlineStr"/>
+      <c r="Y7" t="inlineStr"/>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr"/>
+      <c r="A8" t="n">
+        <v>1</v>
+      </c>
       <c r="B8" t="inlineStr">
         <is>
           <t>2023-07-15</t>
@@ -1125,20 +1182,16 @@
           <t>Philadelphia Phillies</t>
         </is>
       </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>-143</t>
-        </is>
+      <c r="J8" t="n">
+        <v>-143</v>
       </c>
       <c r="K8" t="inlineStr">
         <is>
           <t>LowVig.ag</t>
         </is>
       </c>
-      <c r="L8" t="inlineStr">
-        <is>
-          <t>+133</t>
-        </is>
+      <c r="L8" t="n">
+        <v>133</v>
       </c>
       <c r="M8" t="inlineStr">
         <is>
@@ -1146,35 +1199,46 @@
         </is>
       </c>
       <c r="N8" t="n">
+        <v>9</v>
+      </c>
+      <c r="O8" t="n">
+        <v>4</v>
+      </c>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>Taijuan Walker</t>
+        </is>
+      </c>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>Ryan Weathers</t>
+        </is>
+      </c>
+      <c r="R8" t="n">
         <v>0.9884720883230922</v>
       </c>
-      <c r="O8" t="inlineStr">
+      <c r="S8" t="inlineStr">
         <is>
           <t>Citizens Bank Park</t>
         </is>
       </c>
-      <c r="P8" t="inlineStr"/>
-      <c r="Q8" t="inlineStr">
+      <c r="T8" t="inlineStr"/>
+      <c r="U8" t="inlineStr">
         <is>
           <t>['MLBN (out-of-market only)']</t>
         </is>
       </c>
-      <c r="R8" s="2" t="n">
-        <v>45122.40607709075</v>
-      </c>
-      <c r="S8" t="inlineStr">
-        <is>
-          <t>2023-07-15T17:05:00Z</t>
-        </is>
-      </c>
-      <c r="T8" t="inlineStr">
-        <is>
-          <t>2023-07-15 - San Diego Padres @ Philadelphia Phillies (Scheduled)</t>
-        </is>
-      </c>
+      <c r="V8" s="2" t="n">
+        <v>45122.40607709491</v>
+      </c>
+      <c r="W8" t="inlineStr"/>
+      <c r="X8" t="inlineStr"/>
+      <c r="Y8" t="inlineStr"/>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr"/>
+      <c r="A9" t="n">
+        <v>1</v>
+      </c>
       <c r="B9" t="inlineStr">
         <is>
           <t>2023-07-15</t>
@@ -1215,20 +1279,16 @@
           <t>San Francisco Giants</t>
         </is>
       </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>+139</t>
-        </is>
+      <c r="J9" t="n">
+        <v>139</v>
       </c>
       <c r="K9" t="inlineStr">
         <is>
           <t>LowVig.ag</t>
         </is>
       </c>
-      <c r="L9" t="inlineStr">
-        <is>
-          <t>-145</t>
-        </is>
+      <c r="L9" t="n">
+        <v>-145</v>
       </c>
       <c r="M9" t="inlineStr">
         <is>
@@ -1236,35 +1296,46 @@
         </is>
       </c>
       <c r="N9" t="n">
+        <v>1</v>
+      </c>
+      <c r="O9" t="n">
+        <v>3</v>
+      </c>
+      <c r="P9" t="inlineStr">
+        <is>
+          <t>Taylor Rogers</t>
+        </is>
+      </c>
+      <c r="Q9" t="inlineStr">
+        <is>
+          <t>Carmen Mlodzinski</t>
+        </is>
+      </c>
+      <c r="R9" t="n">
         <v>0.004972930915199898</v>
       </c>
-      <c r="O9" t="inlineStr">
+      <c r="S9" t="inlineStr">
         <is>
           <t>PNC Park</t>
         </is>
       </c>
-      <c r="P9" t="inlineStr"/>
-      <c r="Q9" t="inlineStr">
+      <c r="T9" t="inlineStr"/>
+      <c r="U9" t="inlineStr">
         <is>
           <t>[]</t>
         </is>
       </c>
-      <c r="R9" s="2" t="n">
-        <v>45122.40607709075</v>
-      </c>
-      <c r="S9" t="inlineStr">
-        <is>
-          <t>2023-07-15T23:05:00Z</t>
-        </is>
-      </c>
-      <c r="T9" t="inlineStr">
-        <is>
-          <t>2023-07-15 - San Francisco Giants @ Pittsburgh Pirates (Scheduled)</t>
-        </is>
-      </c>
+      <c r="V9" s="2" t="n">
+        <v>45122.40607709491</v>
+      </c>
+      <c r="W9" t="inlineStr"/>
+      <c r="X9" t="inlineStr"/>
+      <c r="Y9" t="inlineStr"/>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr"/>
+      <c r="A10" t="n">
+        <v>1</v>
+      </c>
       <c r="B10" t="inlineStr">
         <is>
           <t>2023-07-15</t>
@@ -1305,20 +1376,16 @@
           <t>Minnesota Twins</t>
         </is>
       </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>+198</t>
-        </is>
+      <c r="J10" t="n">
+        <v>198</v>
       </c>
       <c r="K10" t="inlineStr">
         <is>
           <t>LowVig.ag</t>
         </is>
       </c>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t>-217</t>
-        </is>
+      <c r="L10" t="n">
+        <v>-217</v>
       </c>
       <c r="M10" t="inlineStr">
         <is>
@@ -1326,35 +1393,46 @@
         </is>
       </c>
       <c r="N10" t="n">
+        <v>7</v>
+      </c>
+      <c r="O10" t="n">
+        <v>10</v>
+      </c>
+      <c r="P10" t="inlineStr">
+        <is>
+          <t>Jovani Moran</t>
+        </is>
+      </c>
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t>Freddy Tarnok</t>
+        </is>
+      </c>
+      <c r="R10" t="n">
         <v>0.0479353425270994</v>
       </c>
-      <c r="O10" t="inlineStr">
+      <c r="S10" t="inlineStr">
         <is>
           <t>Oakland Coliseum</t>
         </is>
       </c>
-      <c r="P10" t="inlineStr"/>
-      <c r="Q10" t="inlineStr">
+      <c r="T10" t="inlineStr"/>
+      <c r="U10" t="inlineStr">
         <is>
           <t>[]</t>
         </is>
       </c>
-      <c r="R10" s="2" t="n">
-        <v>45122.40607709075</v>
-      </c>
-      <c r="S10" t="inlineStr">
-        <is>
-          <t>2023-07-15T23:07:00Z</t>
-        </is>
-      </c>
-      <c r="T10" t="inlineStr">
-        <is>
-          <t>2023-07-15 - Minnesota Twins @ Oakland Athletics (Scheduled)</t>
-        </is>
-      </c>
+      <c r="V10" s="2" t="n">
+        <v>45122.40607709491</v>
+      </c>
+      <c r="W10" t="inlineStr"/>
+      <c r="X10" t="inlineStr"/>
+      <c r="Y10" t="inlineStr"/>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr"/>
+      <c r="A11" t="n">
+        <v>0</v>
+      </c>
       <c r="B11" t="inlineStr">
         <is>
           <t>2023-07-15</t>
@@ -1395,20 +1473,16 @@
           <t>Cincinnati Reds</t>
         </is>
       </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>-115</t>
-        </is>
+      <c r="J11" t="n">
+        <v>-115</v>
       </c>
       <c r="K11" t="inlineStr">
         <is>
           <t>WynnBET</t>
         </is>
       </c>
-      <c r="L11" t="inlineStr">
-        <is>
-          <t>+106</t>
-        </is>
+      <c r="L11" t="n">
+        <v>106</v>
       </c>
       <c r="M11" t="inlineStr">
         <is>
@@ -1416,39 +1490,50 @@
         </is>
       </c>
       <c r="N11" t="n">
+        <v>0</v>
+      </c>
+      <c r="O11" t="n">
+        <v>3</v>
+      </c>
+      <c r="P11" t="inlineStr">
+        <is>
+          <t>Freddy Peralta</t>
+        </is>
+      </c>
+      <c r="Q11" t="inlineStr">
+        <is>
+          <t>Andrew Abbott</t>
+        </is>
+      </c>
+      <c r="R11" t="n">
         <v>0.9990887093027013</v>
       </c>
-      <c r="O11" t="inlineStr">
+      <c r="S11" t="inlineStr">
         <is>
           <t>Great American Ball Park</t>
         </is>
       </c>
-      <c r="P11" t="inlineStr">
+      <c r="T11" t="inlineStr">
         <is>
           <t>MIL leads 2-1</t>
         </is>
       </c>
-      <c r="Q11" t="inlineStr">
+      <c r="U11" t="inlineStr">
         <is>
           <t>[]</t>
         </is>
       </c>
-      <c r="R11" s="2" t="n">
-        <v>45122.40607709075</v>
-      </c>
-      <c r="S11" t="inlineStr">
-        <is>
-          <t>2023-07-15T23:10:00Z</t>
-        </is>
-      </c>
-      <c r="T11" t="inlineStr">
-        <is>
-          <t>2023-07-15 - Milwaukee Brewers @ Cincinnati Reds (Scheduled)</t>
-        </is>
-      </c>
+      <c r="V11" s="2" t="n">
+        <v>45122.40607709491</v>
+      </c>
+      <c r="W11" t="inlineStr"/>
+      <c r="X11" t="inlineStr"/>
+      <c r="Y11" t="inlineStr"/>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr"/>
+      <c r="A12" t="n">
+        <v>1</v>
+      </c>
       <c r="B12" t="inlineStr">
         <is>
           <t>2023-07-14</t>
@@ -1489,20 +1574,16 @@
           <t>Tampa Bay Rays</t>
         </is>
       </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>+198</t>
-        </is>
+      <c r="J12" t="n">
+        <v>198</v>
       </c>
       <c r="K12" t="inlineStr">
         <is>
           <t>WynnBET</t>
         </is>
       </c>
-      <c r="L12" t="inlineStr">
-        <is>
-          <t>-208</t>
-        </is>
+      <c r="L12" t="n">
+        <v>-208</v>
       </c>
       <c r="M12" t="inlineStr">
         <is>
@@ -1510,35 +1591,46 @@
         </is>
       </c>
       <c r="N12" t="n">
+        <v>2</v>
+      </c>
+      <c r="O12" t="n">
+        <v>4</v>
+      </c>
+      <c r="P12" t="inlineStr">
+        <is>
+          <t>Colin Poche</t>
+        </is>
+      </c>
+      <c r="Q12" t="inlineStr">
+        <is>
+          <t>Carlos Hernandez</t>
+        </is>
+      </c>
+      <c r="R12" t="n">
         <v>0.01030191366295862</v>
       </c>
-      <c r="O12" t="inlineStr">
+      <c r="S12" t="inlineStr">
         <is>
           <t>Kauffman Stadium</t>
         </is>
       </c>
-      <c r="P12" t="inlineStr"/>
-      <c r="Q12" t="inlineStr">
+      <c r="T12" t="inlineStr"/>
+      <c r="U12" t="inlineStr">
         <is>
           <t>[]</t>
         </is>
       </c>
-      <c r="R12" s="2" t="n">
-        <v>45122.40607709075</v>
-      </c>
-      <c r="S12" t="inlineStr">
-        <is>
-          <t>2023-07-15T00:10:00Z</t>
-        </is>
-      </c>
-      <c r="T12" t="inlineStr">
-        <is>
-          <t>2023-07-14 - Tampa Bay Rays @ Kansas City Royals (Postponed)</t>
-        </is>
-      </c>
+      <c r="V12" s="2" t="n">
+        <v>45122.40607709491</v>
+      </c>
+      <c r="W12" t="inlineStr"/>
+      <c r="X12" t="inlineStr"/>
+      <c r="Y12" t="inlineStr"/>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr"/>
+      <c r="A13" t="n">
+        <v>0</v>
+      </c>
       <c r="B13" t="inlineStr">
         <is>
           <t>2023-07-15</t>
@@ -1579,20 +1671,16 @@
           <t>Atlanta Braves</t>
         </is>
       </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>-274</t>
-        </is>
+      <c r="J13" t="n">
+        <v>-274</v>
       </c>
       <c r="K13" t="inlineStr">
         <is>
           <t>LowVig.ag</t>
         </is>
       </c>
-      <c r="L13" t="inlineStr">
-        <is>
-          <t>+260</t>
-        </is>
+      <c r="L13" t="n">
+        <v>260</v>
       </c>
       <c r="M13" t="inlineStr">
         <is>
@@ -1600,35 +1688,46 @@
         </is>
       </c>
       <c r="N13" t="n">
+        <v>5</v>
+      </c>
+      <c r="O13" t="n">
+        <v>6</v>
+      </c>
+      <c r="P13" t="inlineStr">
+        <is>
+          <t>Lance Lynn</t>
+        </is>
+      </c>
+      <c r="Q13" t="inlineStr">
+        <is>
+          <t>Spencer Strider</t>
+        </is>
+      </c>
+      <c r="R13" t="n">
         <v>0.9999412748229022</v>
       </c>
-      <c r="O13" t="inlineStr">
+      <c r="S13" t="inlineStr">
         <is>
           <t>Truist Park</t>
         </is>
       </c>
-      <c r="P13" t="inlineStr"/>
-      <c r="Q13" t="inlineStr">
+      <c r="T13" t="inlineStr"/>
+      <c r="U13" t="inlineStr">
         <is>
           <t>['FOX']</t>
         </is>
       </c>
-      <c r="R13" s="2" t="n">
-        <v>45122.40607709075</v>
-      </c>
-      <c r="S13" t="inlineStr">
-        <is>
-          <t>2023-07-15T23:15:00Z</t>
-        </is>
-      </c>
-      <c r="T13" t="inlineStr">
-        <is>
-          <t>2023-07-15 - Chicago White Sox @ Atlanta Braves (Scheduled)</t>
-        </is>
-      </c>
+      <c r="V13" s="2" t="n">
+        <v>45122.40607709491</v>
+      </c>
+      <c r="W13" t="inlineStr"/>
+      <c r="X13" t="inlineStr"/>
+      <c r="Y13" t="inlineStr"/>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr"/>
+      <c r="A14" t="n">
+        <v>1</v>
+      </c>
       <c r="B14" t="inlineStr">
         <is>
           <t>2023-07-15</t>
@@ -1669,20 +1768,16 @@
           <t>Los Angeles Dodgers</t>
         </is>
       </c>
-      <c r="J14" t="inlineStr">
-        <is>
-          <t>-108</t>
-        </is>
+      <c r="J14" t="n">
+        <v>-108</v>
       </c>
       <c r="K14" t="inlineStr">
         <is>
           <t>WynnBET</t>
         </is>
       </c>
-      <c r="L14" t="inlineStr">
-        <is>
-          <t>+109</t>
-        </is>
+      <c r="L14" t="n">
+        <v>109</v>
       </c>
       <c r="M14" t="inlineStr">
         <is>
@@ -1690,35 +1785,46 @@
         </is>
       </c>
       <c r="N14" t="n">
+        <v>1</v>
+      </c>
+      <c r="O14" t="n">
+        <v>5</v>
+      </c>
+      <c r="P14" t="inlineStr">
+        <is>
+          <t>Brusdar Graterol</t>
+        </is>
+      </c>
+      <c r="Q14" t="inlineStr">
+        <is>
+          <t>Adam Ottavino</t>
+        </is>
+      </c>
+      <c r="R14" t="n">
         <v>0.03839275740075281</v>
       </c>
-      <c r="O14" t="inlineStr">
+      <c r="S14" t="inlineStr">
         <is>
           <t>Citi Field</t>
         </is>
       </c>
-      <c r="P14" t="inlineStr"/>
-      <c r="Q14" t="inlineStr">
+      <c r="T14" t="inlineStr"/>
+      <c r="U14" t="inlineStr">
         <is>
           <t>['FOX']</t>
         </is>
       </c>
-      <c r="R14" s="2" t="n">
-        <v>45122.40607709075</v>
-      </c>
-      <c r="S14" t="inlineStr">
-        <is>
-          <t>2023-07-15T23:15:00Z</t>
-        </is>
-      </c>
-      <c r="T14" t="inlineStr">
-        <is>
-          <t>2023-07-15 - Los Angeles Dodgers @ New York Mets (Scheduled)</t>
-        </is>
-      </c>
+      <c r="V14" s="2" t="n">
+        <v>45122.40607709491</v>
+      </c>
+      <c r="W14" t="inlineStr"/>
+      <c r="X14" t="inlineStr"/>
+      <c r="Y14" t="inlineStr"/>
     </row>
     <row r="15">
-      <c r="A15" t="inlineStr"/>
+      <c r="A15" t="n">
+        <v>0</v>
+      </c>
       <c r="B15" t="inlineStr">
         <is>
           <t>2023-07-15</t>
@@ -1759,20 +1865,16 @@
           <t>St. Louis Cardinals</t>
         </is>
       </c>
-      <c r="J15" t="inlineStr">
-        <is>
-          <t>-185</t>
-        </is>
+      <c r="J15" t="n">
+        <v>-185</v>
       </c>
       <c r="K15" t="inlineStr">
         <is>
           <t>LowVig.ag</t>
         </is>
       </c>
-      <c r="L15" t="inlineStr">
-        <is>
-          <t>+175</t>
-        </is>
+      <c r="L15" t="n">
+        <v>175</v>
       </c>
       <c r="M15" t="inlineStr">
         <is>
@@ -1780,35 +1882,46 @@
         </is>
       </c>
       <c r="N15" t="n">
+        <v>9</v>
+      </c>
+      <c r="O15" t="n">
+        <v>6</v>
+      </c>
+      <c r="P15" t="inlineStr">
+        <is>
+          <t>Dakota Hudson</t>
+        </is>
+      </c>
+      <c r="Q15" t="inlineStr">
+        <is>
+          <t>Amos Willingham</t>
+        </is>
+      </c>
+      <c r="R15" t="n">
         <v>0.01163660894263766</v>
       </c>
-      <c r="O15" t="inlineStr">
+      <c r="S15" t="inlineStr">
         <is>
           <t>Busch Stadium</t>
         </is>
       </c>
-      <c r="P15" t="inlineStr"/>
-      <c r="Q15" t="inlineStr">
+      <c r="T15" t="inlineStr"/>
+      <c r="U15" t="inlineStr">
         <is>
           <t>[]</t>
         </is>
       </c>
-      <c r="R15" s="2" t="n">
-        <v>45122.40607709075</v>
-      </c>
-      <c r="S15" t="inlineStr">
-        <is>
-          <t>2023-07-15T23:15:00Z</t>
-        </is>
-      </c>
-      <c r="T15" t="inlineStr">
-        <is>
-          <t>2023-07-15 - Washington Nationals @ St. Louis Cardinals (Scheduled)</t>
-        </is>
-      </c>
+      <c r="V15" s="2" t="n">
+        <v>45122.40607709491</v>
+      </c>
+      <c r="W15" t="inlineStr"/>
+      <c r="X15" t="inlineStr"/>
+      <c r="Y15" t="inlineStr"/>
     </row>
     <row r="16">
-      <c r="A16" t="inlineStr"/>
+      <c r="A16" t="n">
+        <v>1</v>
+      </c>
       <c r="B16" t="inlineStr">
         <is>
           <t>2023-07-15</t>
@@ -1849,20 +1962,16 @@
           <t>New York Yankees</t>
         </is>
       </c>
-      <c r="J16" t="inlineStr">
-        <is>
-          <t>+146</t>
-        </is>
+      <c r="J16" t="n">
+        <v>146</v>
       </c>
       <c r="K16" t="inlineStr">
         <is>
           <t>LowVig.ag</t>
         </is>
       </c>
-      <c r="L16" t="inlineStr">
-        <is>
-          <t>-154</t>
-        </is>
+      <c r="L16" t="n">
+        <v>-154</v>
       </c>
       <c r="M16" t="inlineStr">
         <is>
@@ -1870,35 +1979,46 @@
         </is>
       </c>
       <c r="N16" t="n">
+        <v>3</v>
+      </c>
+      <c r="O16" t="n">
+        <v>6</v>
+      </c>
+      <c r="P16" t="inlineStr">
+        <is>
+          <t>Clarke Schmidt</t>
+        </is>
+      </c>
+      <c r="Q16" t="inlineStr">
+        <is>
+          <t>Connor Seabold</t>
+        </is>
+      </c>
+      <c r="R16" t="n">
         <v>0.4488145151581657</v>
       </c>
-      <c r="O16" t="inlineStr">
+      <c r="S16" t="inlineStr">
         <is>
           <t>Coors Field</t>
         </is>
       </c>
-      <c r="P16" t="inlineStr"/>
-      <c r="Q16" t="inlineStr">
+      <c r="T16" t="inlineStr"/>
+      <c r="U16" t="inlineStr">
         <is>
           <t>[]</t>
         </is>
       </c>
-      <c r="R16" s="2" t="n">
-        <v>45122.40607709075</v>
-      </c>
-      <c r="S16" t="inlineStr">
-        <is>
-          <t>2023-07-16T00:10:00Z</t>
-        </is>
-      </c>
-      <c r="T16" t="inlineStr">
-        <is>
-          <t>2023-07-15 - New York Yankees @ Colorado Rockies (Scheduled)</t>
-        </is>
-      </c>
+      <c r="V16" s="2" t="n">
+        <v>45122.40607709491</v>
+      </c>
+      <c r="W16" t="inlineStr"/>
+      <c r="X16" t="inlineStr"/>
+      <c r="Y16" t="inlineStr"/>
     </row>
     <row r="17">
-      <c r="A17" t="inlineStr"/>
+      <c r="A17" t="n">
+        <v>0</v>
+      </c>
       <c r="B17" t="inlineStr">
         <is>
           <t>2023-07-15</t>
@@ -1939,20 +2059,16 @@
           <t>Houston Astros</t>
         </is>
       </c>
-      <c r="J17" t="inlineStr">
-        <is>
-          <t>+125</t>
-        </is>
+      <c r="J17" t="n">
+        <v>125</v>
       </c>
       <c r="K17" t="inlineStr">
         <is>
           <t>BetUS</t>
         </is>
       </c>
-      <c r="L17" t="inlineStr">
-        <is>
-          <t>-133</t>
-        </is>
+      <c r="L17" t="n">
+        <v>-133</v>
       </c>
       <c r="M17" t="inlineStr">
         <is>
@@ -1960,35 +2076,46 @@
         </is>
       </c>
       <c r="N17" t="n">
+        <v>13</v>
+      </c>
+      <c r="O17" t="n">
+        <v>12</v>
+      </c>
+      <c r="P17" t="inlineStr">
+        <is>
+          <t>Carlos Estevez</t>
+        </is>
+      </c>
+      <c r="Q17" t="inlineStr">
+        <is>
+          <t>Phil Maton</t>
+        </is>
+      </c>
+      <c r="R17" t="n">
         <v>0.09502862103117936</v>
       </c>
-      <c r="O17" t="inlineStr">
+      <c r="S17" t="inlineStr">
         <is>
           <t>Angel Stadium</t>
         </is>
       </c>
-      <c r="P17" t="inlineStr"/>
-      <c r="Q17" t="inlineStr">
+      <c r="T17" t="inlineStr"/>
+      <c r="U17" t="inlineStr">
         <is>
           <t>[]</t>
         </is>
       </c>
-      <c r="R17" s="2" t="n">
-        <v>45122.40607709075</v>
-      </c>
-      <c r="S17" t="inlineStr">
-        <is>
-          <t>2023-07-16T01:07:00Z</t>
-        </is>
-      </c>
-      <c r="T17" t="inlineStr">
-        <is>
-          <t>2023-07-15 - Houston Astros @ Los Angeles Angels (Scheduled)</t>
-        </is>
-      </c>
+      <c r="V17" s="2" t="n">
+        <v>45122.40607709491</v>
+      </c>
+      <c r="W17" t="inlineStr"/>
+      <c r="X17" t="inlineStr"/>
+      <c r="Y17" t="inlineStr"/>
     </row>
     <row r="18">
-      <c r="A18" t="inlineStr"/>
+      <c r="A18" t="n">
+        <v>1</v>
+      </c>
       <c r="B18" t="inlineStr">
         <is>
           <t>2023-07-15</t>
@@ -2029,20 +2156,16 @@
           <t>Seattle Mariners</t>
         </is>
       </c>
-      <c r="J18" t="inlineStr">
-        <is>
-          <t>-196</t>
-        </is>
+      <c r="J18" t="n">
+        <v>-196</v>
       </c>
       <c r="K18" t="inlineStr">
         <is>
           <t>BetOnline.ag</t>
         </is>
       </c>
-      <c r="L18" t="inlineStr">
-        <is>
-          <t>+185</t>
-        </is>
+      <c r="L18" t="n">
+        <v>185</v>
       </c>
       <c r="M18" t="inlineStr">
         <is>
@@ -2050,30 +2173,1518 @@
         </is>
       </c>
       <c r="N18" t="n">
+        <v>0</v>
+      </c>
+      <c r="O18" t="n">
+        <v>6</v>
+      </c>
+      <c r="P18" t="inlineStr">
+        <is>
+          <t>Michael Lorenzen</t>
+        </is>
+      </c>
+      <c r="Q18" t="inlineStr">
+        <is>
+          <t>George Kirby</t>
+        </is>
+      </c>
+      <c r="R18" t="n">
         <v>0.2276046638669845</v>
       </c>
-      <c r="O18" t="inlineStr">
+      <c r="S18" t="inlineStr">
         <is>
           <t>T-Mobile Park</t>
         </is>
       </c>
-      <c r="P18" t="inlineStr"/>
-      <c r="Q18" t="inlineStr">
+      <c r="T18" t="inlineStr"/>
+      <c r="U18" t="inlineStr">
         <is>
           <t>[]</t>
         </is>
       </c>
-      <c r="R18" s="2" t="n">
-        <v>45122.40607709075</v>
-      </c>
-      <c r="S18" t="inlineStr">
-        <is>
-          <t>2023-07-16T01:40:00Z</t>
-        </is>
-      </c>
-      <c r="T18" t="inlineStr">
-        <is>
-          <t>2023-07-15 - Detroit Tigers @ Seattle Mariners (Scheduled)</t>
+      <c r="V18" s="2" t="n">
+        <v>45122.40607709491</v>
+      </c>
+      <c r="W18" t="inlineStr"/>
+      <c r="X18" t="inlineStr"/>
+      <c r="Y18" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr"/>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>2023-07-17</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>12:05 am</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Pittsburgh Pirates</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Quinn Priester</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Cleveland Guardians</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr"/>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>Pittsburgh Pirates</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>San Francisco Giants</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>+250</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>FanDuel</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr"/>
+      <c r="M19" t="inlineStr"/>
+      <c r="N19" t="inlineStr"/>
+      <c r="O19" t="inlineStr"/>
+      <c r="P19" t="inlineStr"/>
+      <c r="Q19" t="inlineStr"/>
+      <c r="R19" t="n">
+        <v>0.9343306111829759</v>
+      </c>
+      <c r="S19" t="inlineStr">
+        <is>
+          <t>PNC Park</t>
+        </is>
+      </c>
+      <c r="T19" t="inlineStr"/>
+      <c r="U19" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="V19" s="2" t="n">
+        <v>45123.54770751713</v>
+      </c>
+      <c r="W19" t="inlineStr">
+        <is>
+          <t>2023-07-17T23:05:00Z</t>
+        </is>
+      </c>
+      <c r="X19" t="n">
+        <v>717371</v>
+      </c>
+      <c r="Y19" t="inlineStr">
+        <is>
+          <t>2023-07-17 - Cleveland Guardians @ Pittsburgh Pirates (Scheduled)</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr"/>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>2023-07-18</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>01:35 pm</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Atlanta Braves</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Bryce Elder</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Arizona Diamondbacks</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr"/>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>Atlanta Braves</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>Atlanta Braves</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>-164</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>WynnBET</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr"/>
+      <c r="M20" t="inlineStr"/>
+      <c r="N20" t="inlineStr"/>
+      <c r="O20" t="inlineStr"/>
+      <c r="P20" t="inlineStr"/>
+      <c r="Q20" t="inlineStr"/>
+      <c r="R20" t="n">
+        <v>0.9436012728613981</v>
+      </c>
+      <c r="S20" t="inlineStr">
+        <is>
+          <t>Truist Park</t>
+        </is>
+      </c>
+      <c r="T20" t="inlineStr"/>
+      <c r="U20" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="V20" s="2" t="n">
+        <v>45123.54770751713</v>
+      </c>
+      <c r="W20" t="inlineStr">
+        <is>
+          <t>2023-07-18T23:20:00Z</t>
+        </is>
+      </c>
+      <c r="X20" t="n">
+        <v>717358</v>
+      </c>
+      <c r="Y20" t="inlineStr">
+        <is>
+          <t>2023-07-18 - Arizona Diamondbacks @ Atlanta Braves (Scheduled)</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr"/>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>2023-07-16</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>01:35 pm</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Baltimore Orioles</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Kyle Bradish</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Miami Marlins</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>Steven Okert</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>Miami Marlins</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>Baltimore Orioles</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>-172</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>BetOnline.ag</t>
+        </is>
+      </c>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>+159</t>
+        </is>
+      </c>
+      <c r="M21" t="inlineStr">
+        <is>
+          <t>BetOnline.ag</t>
+        </is>
+      </c>
+      <c r="N21" t="inlineStr"/>
+      <c r="O21" t="inlineStr"/>
+      <c r="P21" t="inlineStr"/>
+      <c r="Q21" t="inlineStr"/>
+      <c r="R21" t="n">
+        <v>5.217156943423028e-09</v>
+      </c>
+      <c r="S21" t="inlineStr">
+        <is>
+          <t>Oriole Park at Camden Yards</t>
+        </is>
+      </c>
+      <c r="T21" t="inlineStr">
+        <is>
+          <t>BAL leads 2-0</t>
+        </is>
+      </c>
+      <c r="U21" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="V21" s="2" t="n">
+        <v>45123.54770751713</v>
+      </c>
+      <c r="W21" t="inlineStr">
+        <is>
+          <t>2023-07-16T17:35:00Z</t>
+        </is>
+      </c>
+      <c r="X21" t="n">
+        <v>717384</v>
+      </c>
+      <c r="Y21" t="inlineStr">
+        <is>
+          <t>2023-07-16 - Miami Marlins @ Baltimore Orioles (Pre-Game)</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr"/>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>2023-07-16</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>01:37 pm</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Toronto Blue Jays</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Yusei Kikuchi</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>Arizona Diamondbacks</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>Tommy Henry</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>Arizona Diamondbacks</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>Toronto Blue Jays</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>-154</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>WynnBET</t>
+        </is>
+      </c>
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>+148</t>
+        </is>
+      </c>
+      <c r="M22" t="inlineStr">
+        <is>
+          <t>LowVig.ag</t>
+        </is>
+      </c>
+      <c r="N22" t="inlineStr"/>
+      <c r="O22" t="inlineStr"/>
+      <c r="P22" t="inlineStr"/>
+      <c r="Q22" t="inlineStr"/>
+      <c r="R22" t="n">
+        <v>2.480473218613033e-05</v>
+      </c>
+      <c r="S22" t="inlineStr">
+        <is>
+          <t>Rogers Centre</t>
+        </is>
+      </c>
+      <c r="T22" t="inlineStr">
+        <is>
+          <t>TOR leads 2-0</t>
+        </is>
+      </c>
+      <c r="U22" t="inlineStr">
+        <is>
+          <t>['MLBN (out-of-market only)']</t>
+        </is>
+      </c>
+      <c r="V22" s="2" t="n">
+        <v>45123.54770751713</v>
+      </c>
+      <c r="W22" t="inlineStr">
+        <is>
+          <t>2023-07-16T17:37:00Z</t>
+        </is>
+      </c>
+      <c r="X22" t="n">
+        <v>717386</v>
+      </c>
+      <c r="Y22" t="inlineStr">
+        <is>
+          <t>2023-07-16 - Arizona Diamondbacks @ Toronto Blue Jays (Pre-Game)</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr"/>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>2023-07-16</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>01:40 pm</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Cincinnati Reds</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Ben Lively</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>Milwaukee Brewers</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>Adrian Houser</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>Cincinnati Reds</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>Cincinnati Reds</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>-139</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>LowVig.ag</t>
+        </is>
+      </c>
+      <c r="L23" t="inlineStr">
+        <is>
+          <t>+130</t>
+        </is>
+      </c>
+      <c r="M23" t="inlineStr">
+        <is>
+          <t>Barstool Sportsbook</t>
+        </is>
+      </c>
+      <c r="N23" t="inlineStr"/>
+      <c r="O23" t="inlineStr"/>
+      <c r="P23" t="inlineStr"/>
+      <c r="Q23" t="inlineStr"/>
+      <c r="R23" t="n">
+        <v>0.9955504435643163</v>
+      </c>
+      <c r="S23" t="inlineStr">
+        <is>
+          <t>Great American Ball Park</t>
+        </is>
+      </c>
+      <c r="T23" t="inlineStr">
+        <is>
+          <t>MIL leads 4-1</t>
+        </is>
+      </c>
+      <c r="U23" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="V23" s="2" t="n">
+        <v>45123.54770751713</v>
+      </c>
+      <c r="W23" t="inlineStr">
+        <is>
+          <t>2023-07-16T17:40:00Z</t>
+        </is>
+      </c>
+      <c r="X23" t="n">
+        <v>717383</v>
+      </c>
+      <c r="Y23" t="inlineStr">
+        <is>
+          <t>2023-07-16 - Milwaukee Brewers @ Cincinnati Reds (Pre-Game)</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr"/>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>2023-07-16</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>02:15 pm</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>St. Louis Cardinals</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Jack Flaherty</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>Washington Nationals</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>Josiah Gray</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>Washington Nationals</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>St. Louis Cardinals</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>-167</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>WynnBET</t>
+        </is>
+      </c>
+      <c r="L24" t="inlineStr">
+        <is>
+          <t>+156</t>
+        </is>
+      </c>
+      <c r="M24" t="inlineStr">
+        <is>
+          <t>LowVig.ag</t>
+        </is>
+      </c>
+      <c r="N24" t="inlineStr"/>
+      <c r="O24" t="inlineStr"/>
+      <c r="P24" t="inlineStr"/>
+      <c r="Q24" t="inlineStr"/>
+      <c r="R24" t="n">
+        <v>0.1068840252149751</v>
+      </c>
+      <c r="S24" t="inlineStr">
+        <is>
+          <t>Busch Stadium</t>
+        </is>
+      </c>
+      <c r="T24" t="inlineStr">
+        <is>
+          <t>Series tied 1-1</t>
+        </is>
+      </c>
+      <c r="U24" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="V24" s="2" t="n">
+        <v>45123.54770751713</v>
+      </c>
+      <c r="W24" t="inlineStr">
+        <is>
+          <t>2023-07-16T18:15:00Z</t>
+        </is>
+      </c>
+      <c r="X24" t="n">
+        <v>717380</v>
+      </c>
+      <c r="Y24" t="inlineStr">
+        <is>
+          <t>2023-07-16 - Washington Nationals @ St. Louis Cardinals (Pre-Game)</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr"/>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>2023-07-16</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>02:20 pm</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Chicago Cubs</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Justin Steele</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>Boston Red Sox</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>Kutter Crawford</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>Chicago Cubs</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>Chicago Cubs</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>-141</t>
+        </is>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>LowVig.ag</t>
+        </is>
+      </c>
+      <c r="L25" t="inlineStr">
+        <is>
+          <t>+132</t>
+        </is>
+      </c>
+      <c r="M25" t="inlineStr">
+        <is>
+          <t>WynnBET</t>
+        </is>
+      </c>
+      <c r="N25" t="inlineStr"/>
+      <c r="O25" t="inlineStr"/>
+      <c r="P25" t="inlineStr"/>
+      <c r="Q25" t="inlineStr"/>
+      <c r="R25" t="n">
+        <v>0.997081427178948</v>
+      </c>
+      <c r="S25" t="inlineStr">
+        <is>
+          <t>Wrigley Field</t>
+        </is>
+      </c>
+      <c r="T25" t="inlineStr">
+        <is>
+          <t>Series tied 1-1</t>
+        </is>
+      </c>
+      <c r="U25" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="V25" s="2" t="n">
+        <v>45123.54770751713</v>
+      </c>
+      <c r="W25" t="inlineStr">
+        <is>
+          <t>2023-07-16T18:20:00Z</t>
+        </is>
+      </c>
+      <c r="X25" t="n">
+        <v>717376</v>
+      </c>
+      <c r="Y25" t="inlineStr">
+        <is>
+          <t>2023-07-16 - Boston Red Sox @ Chicago Cubs (Pre-Game)</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr"/>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>2023-07-16</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>02:35 pm</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Texas Rangers</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Martin Perez</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>Cleveland Guardians</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>Tanner Bibee</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>Texas Rangers</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>Texas Rangers</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>-130</t>
+        </is>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>WynnBET</t>
+        </is>
+      </c>
+      <c r="L26" t="inlineStr">
+        <is>
+          <t>+121</t>
+        </is>
+      </c>
+      <c r="M26" t="inlineStr">
+        <is>
+          <t>LowVig.ag</t>
+        </is>
+      </c>
+      <c r="N26" t="inlineStr"/>
+      <c r="O26" t="inlineStr"/>
+      <c r="P26" t="inlineStr"/>
+      <c r="Q26" t="inlineStr"/>
+      <c r="R26" t="n">
+        <v>0.9991539319051719</v>
+      </c>
+      <c r="S26" t="inlineStr">
+        <is>
+          <t>Globe Life Field</t>
+        </is>
+      </c>
+      <c r="T26" t="inlineStr">
+        <is>
+          <t>TEX leads 2-0</t>
+        </is>
+      </c>
+      <c r="U26" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="V26" s="2" t="n">
+        <v>45123.54770751713</v>
+      </c>
+      <c r="W26" t="inlineStr">
+        <is>
+          <t>2023-07-16T18:35:00Z</t>
+        </is>
+      </c>
+      <c r="X26" t="n">
+        <v>717377</v>
+      </c>
+      <c r="Y26" t="inlineStr">
+        <is>
+          <t>2023-07-16 - Cleveland Guardians @ Texas Rangers (Pre-Game)</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr"/>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>2023-07-16</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>02:35 pm</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Philadelphia Phillies</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Zack Wheeler</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>San Diego Padres</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>Seth Lugo</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>Philadelphia Phillies</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>Philadelphia Phillies</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>-143</t>
+        </is>
+      </c>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>WynnBET</t>
+        </is>
+      </c>
+      <c r="L27" t="inlineStr">
+        <is>
+          <t>+135</t>
+        </is>
+      </c>
+      <c r="M27" t="inlineStr">
+        <is>
+          <t>DraftKings</t>
+        </is>
+      </c>
+      <c r="N27" t="inlineStr"/>
+      <c r="O27" t="inlineStr"/>
+      <c r="P27" t="inlineStr"/>
+      <c r="Q27" t="inlineStr"/>
+      <c r="R27" t="n">
+        <v>0.9973819811942846</v>
+      </c>
+      <c r="S27" t="inlineStr">
+        <is>
+          <t>Citizens Bank Park</t>
+        </is>
+      </c>
+      <c r="T27" t="inlineStr">
+        <is>
+          <t>PHI leads 2-1</t>
+        </is>
+      </c>
+      <c r="U27" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="V27" s="2" t="n">
+        <v>45123.54770751713</v>
+      </c>
+      <c r="W27" t="inlineStr">
+        <is>
+          <t>2023-07-16T17:35:00Z</t>
+        </is>
+      </c>
+      <c r="X27" t="n">
+        <v>717387</v>
+      </c>
+      <c r="Y27" t="inlineStr">
+        <is>
+          <t>2023-07-16 - San Diego Padres @ Philadelphia Phillies (Delayed Start: Rain)</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr"/>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>2023-07-16</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>03:10 pm</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Colorado Rockies</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Chase Anderson</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>New York Yankees</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>Gerrit Cole</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>New York Yankees</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>New York Yankees</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>+198</t>
+        </is>
+      </c>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>WynnBET</t>
+        </is>
+      </c>
+      <c r="L28" t="inlineStr">
+        <is>
+          <t>-212</t>
+        </is>
+      </c>
+      <c r="M28" t="inlineStr">
+        <is>
+          <t>LowVig.ag</t>
+        </is>
+      </c>
+      <c r="N28" t="inlineStr"/>
+      <c r="O28" t="inlineStr"/>
+      <c r="P28" t="inlineStr"/>
+      <c r="Q28" t="inlineStr"/>
+      <c r="R28" t="n">
+        <v>0.007349994338412974</v>
+      </c>
+      <c r="S28" t="inlineStr">
+        <is>
+          <t>Coors Field</t>
+        </is>
+      </c>
+      <c r="T28" t="inlineStr">
+        <is>
+          <t>Series tied 1-1</t>
+        </is>
+      </c>
+      <c r="U28" t="inlineStr">
+        <is>
+          <t>['MLB.tv Free Game']</t>
+        </is>
+      </c>
+      <c r="V28" s="2" t="n">
+        <v>45123.54770751713</v>
+      </c>
+      <c r="W28" t="inlineStr">
+        <is>
+          <t>2023-07-16T19:10:00Z</t>
+        </is>
+      </c>
+      <c r="X28" t="n">
+        <v>717378</v>
+      </c>
+      <c r="Y28" t="inlineStr">
+        <is>
+          <t>2023-07-16 - New York Yankees @ Colorado Rockies (Pre-Game)</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr"/>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>2023-07-16</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>03:10 pm</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Kansas City Royals</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Brady Singer</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>Tampa Bay Rays</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>Zach Eflin</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>Tampa Bay Rays</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>Tampa Bay Rays</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>+190</t>
+        </is>
+      </c>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>WynnBET</t>
+        </is>
+      </c>
+      <c r="L29" t="inlineStr">
+        <is>
+          <t>-200</t>
+        </is>
+      </c>
+      <c r="M29" t="inlineStr">
+        <is>
+          <t>BetRivers</t>
+        </is>
+      </c>
+      <c r="N29" t="inlineStr"/>
+      <c r="O29" t="inlineStr"/>
+      <c r="P29" t="inlineStr"/>
+      <c r="Q29" t="inlineStr"/>
+      <c r="R29" t="n">
+        <v>0.01595586693913854</v>
+      </c>
+      <c r="S29" t="inlineStr">
+        <is>
+          <t>Kauffman Stadium</t>
+        </is>
+      </c>
+      <c r="T29" t="inlineStr">
+        <is>
+          <t>TB leads 2-0</t>
+        </is>
+      </c>
+      <c r="U29" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="V29" s="2" t="n">
+        <v>45123.54770751713</v>
+      </c>
+      <c r="W29" t="inlineStr">
+        <is>
+          <t>2023-07-16T18:10:00Z</t>
+        </is>
+      </c>
+      <c r="X29" t="n">
+        <v>717382</v>
+      </c>
+      <c r="Y29" t="inlineStr">
+        <is>
+          <t>2023-07-16 - Tampa Bay Rays @ Kansas City Royals (Pre-Game)</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr"/>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>2023-07-16</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>04:07 pm</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Oakland Athletics</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>JP Sears</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>Minnesota Twins</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>Joe Ryan</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>Minnesota Twins</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>Minnesota Twins</t>
+        </is>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>+170</t>
+        </is>
+      </c>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>SuperBook</t>
+        </is>
+      </c>
+      <c r="L30" t="inlineStr">
+        <is>
+          <t>-175</t>
+        </is>
+      </c>
+      <c r="M30" t="inlineStr">
+        <is>
+          <t>BetOnline.ag</t>
+        </is>
+      </c>
+      <c r="N30" t="inlineStr"/>
+      <c r="O30" t="inlineStr"/>
+      <c r="P30" t="inlineStr"/>
+      <c r="Q30" t="inlineStr"/>
+      <c r="R30" t="n">
+        <v>0.0004614629880784581</v>
+      </c>
+      <c r="S30" t="inlineStr">
+        <is>
+          <t>Oakland Coliseum</t>
+        </is>
+      </c>
+      <c r="T30" t="inlineStr">
+        <is>
+          <t>MIN leads 2-0</t>
+        </is>
+      </c>
+      <c r="U30" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="V30" s="2" t="n">
+        <v>45123.54770751713</v>
+      </c>
+      <c r="W30" t="inlineStr">
+        <is>
+          <t>2023-07-16T20:07:00Z</t>
+        </is>
+      </c>
+      <c r="X30" t="n">
+        <v>717379</v>
+      </c>
+      <c r="Y30" t="inlineStr">
+        <is>
+          <t>2023-07-16 - Minnesota Twins @ Oakland Athletics (Pre-Game)</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr"/>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>2023-07-16</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>04:10 pm</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Seattle Mariners</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>Bryce Miller</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>Detroit Tigers</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>Reese Olson</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>Seattle Mariners</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>Seattle Mariners</t>
+        </is>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>-159</t>
+        </is>
+      </c>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>WynnBET</t>
+        </is>
+      </c>
+      <c r="L31" t="inlineStr">
+        <is>
+          <t>+155</t>
+        </is>
+      </c>
+      <c r="M31" t="inlineStr">
+        <is>
+          <t>DraftKings</t>
+        </is>
+      </c>
+      <c r="N31" t="inlineStr"/>
+      <c r="O31" t="inlineStr"/>
+      <c r="P31" t="inlineStr"/>
+      <c r="Q31" t="inlineStr"/>
+      <c r="R31" t="n">
+        <v>0.9975393207517835</v>
+      </c>
+      <c r="S31" t="inlineStr">
+        <is>
+          <t>T-Mobile Park</t>
+        </is>
+      </c>
+      <c r="T31" t="inlineStr">
+        <is>
+          <t>DET leads 2-0</t>
+        </is>
+      </c>
+      <c r="U31" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="V31" s="2" t="n">
+        <v>45123.54770751713</v>
+      </c>
+      <c r="W31" t="inlineStr">
+        <is>
+          <t>2023-07-16T20:10:00Z</t>
+        </is>
+      </c>
+      <c r="X31" t="n">
+        <v>717373</v>
+      </c>
+      <c r="Y31" t="inlineStr">
+        <is>
+          <t>2023-07-16 - Detroit Tigers @ Seattle Mariners (Pre-Game)</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr"/>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>2023-07-16</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>05:10 pm</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>New York Mets</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Max Scherzer</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>Los Angeles Dodgers</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>Bobby Miller</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>Los Angeles Dodgers</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>New York Mets</t>
+        </is>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>-106</t>
+        </is>
+      </c>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>BetOnline.ag</t>
+        </is>
+      </c>
+      <c r="L32" t="inlineStr">
+        <is>
+          <t>-103</t>
+        </is>
+      </c>
+      <c r="M32" t="inlineStr">
+        <is>
+          <t>BetOnline.ag</t>
+        </is>
+      </c>
+      <c r="N32" t="inlineStr"/>
+      <c r="O32" t="inlineStr"/>
+      <c r="P32" t="inlineStr"/>
+      <c r="Q32" t="inlineStr"/>
+      <c r="R32" t="n">
+        <v>0.2954685844805013</v>
+      </c>
+      <c r="S32" t="inlineStr">
+        <is>
+          <t>Citi Field</t>
+        </is>
+      </c>
+      <c r="T32" t="inlineStr">
+        <is>
+          <t>LAD leads 2-0</t>
+        </is>
+      </c>
+      <c r="U32" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="V32" s="2" t="n">
+        <v>45123.54770751713</v>
+      </c>
+      <c r="W32" t="inlineStr">
+        <is>
+          <t>2023-07-16T21:10:00Z</t>
+        </is>
+      </c>
+      <c r="X32" t="n">
+        <v>717385</v>
+      </c>
+      <c r="Y32" t="inlineStr">
+        <is>
+          <t>2023-07-16 - Los Angeles Dodgers @ New York Mets (Scheduled)</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr"/>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>2023-07-16</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>07:10 pm</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Los Angeles Angels</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Tyler Anderson</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>Houston Astros</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>Cristian Javier</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>Houston Astros</t>
+        </is>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>Houston Astros</t>
+        </is>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>+115</t>
+        </is>
+      </c>
+      <c r="K33" t="inlineStr">
+        <is>
+          <t>William Hill (US)</t>
+        </is>
+      </c>
+      <c r="L33" t="inlineStr">
+        <is>
+          <t>-123</t>
+        </is>
+      </c>
+      <c r="M33" t="inlineStr">
+        <is>
+          <t>BetOnline.ag</t>
+        </is>
+      </c>
+      <c r="N33" t="inlineStr"/>
+      <c r="O33" t="inlineStr"/>
+      <c r="P33" t="inlineStr"/>
+      <c r="Q33" t="inlineStr"/>
+      <c r="R33" t="n">
+        <v>0.1029624895871727</v>
+      </c>
+      <c r="S33" t="inlineStr">
+        <is>
+          <t>Angel Stadium</t>
+        </is>
+      </c>
+      <c r="T33" t="inlineStr"/>
+      <c r="U33" t="inlineStr">
+        <is>
+          <t>['ESPN']</t>
+        </is>
+      </c>
+      <c r="V33" s="2" t="n">
+        <v>45123.54770751713</v>
+      </c>
+      <c r="W33" t="inlineStr">
+        <is>
+          <t>2023-07-16T23:10:00Z</t>
+        </is>
+      </c>
+      <c r="X33" t="n">
+        <v>717381</v>
+      </c>
+      <c r="Y33" t="inlineStr">
+        <is>
+          <t>2023-07-16 - Houston Astros @ Los Angeles Angels (Scheduled)</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
predictions for 07/20/2023 (75% yesterday)
</commit_message>
<xml_diff>
--- a/data/predictions.xlsx
+++ b/data/predictions.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA57"/>
+  <dimension ref="A1:AA62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5350,7 +5350,9 @@
       </c>
     </row>
     <row r="43">
-      <c r="A43" t="inlineStr"/>
+      <c r="A43" t="n">
+        <v>0</v>
+      </c>
       <c r="B43" t="inlineStr">
         <is>
           <t>2023-07-19</t>
@@ -5412,10 +5414,22 @@
           <t>PointsBet (US)</t>
         </is>
       </c>
-      <c r="O43" t="inlineStr"/>
-      <c r="P43" t="inlineStr"/>
-      <c r="Q43" t="inlineStr"/>
-      <c r="R43" t="inlineStr"/>
+      <c r="O43" t="n">
+        <v>7</v>
+      </c>
+      <c r="P43" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q43" t="inlineStr">
+        <is>
+          <t>Ryan Borucki</t>
+        </is>
+      </c>
+      <c r="R43" t="inlineStr">
+        <is>
+          <t>Sam Hentges</t>
+        </is>
+      </c>
       <c r="S43" t="n">
         <v>0.1388673560909337</v>
       </c>
@@ -5446,12 +5460,14 @@
       </c>
       <c r="AA43" t="inlineStr">
         <is>
-          <t>2023-07-19 - Cleveland Guardians @ Pittsburgh Pirates (Scheduled)</t>
+          <t>2023-07-19 - Cleveland Guardians (5) @ Pittsburgh Pirates (7) (Final)</t>
         </is>
       </c>
     </row>
     <row r="44">
-      <c r="A44" t="inlineStr"/>
+      <c r="A44" t="n">
+        <v>1</v>
+      </c>
       <c r="B44" t="inlineStr">
         <is>
           <t>2023-07-19</t>
@@ -5513,10 +5529,22 @@
           <t>LowVig.ag</t>
         </is>
       </c>
-      <c r="O44" t="inlineStr"/>
-      <c r="P44" t="inlineStr"/>
-      <c r="Q44" t="inlineStr"/>
-      <c r="R44" t="inlineStr"/>
+      <c r="O44" t="n">
+        <v>8</v>
+      </c>
+      <c r="P44" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q44" t="inlineStr">
+        <is>
+          <t>Danny Coulombe</t>
+        </is>
+      </c>
+      <c r="R44" t="inlineStr">
+        <is>
+          <t>Julio Urias</t>
+        </is>
+      </c>
       <c r="S44" t="n">
         <v>0.7168255308352357</v>
       </c>
@@ -5547,12 +5575,14 @@
       </c>
       <c r="AA44" t="inlineStr">
         <is>
-          <t>2023-07-19 - Los Angeles Dodgers @ Baltimore Orioles (Scheduled)</t>
+          <t>2023-07-19 - Los Angeles Dodgers (5) @ Baltimore Orioles (8) (Final)</t>
         </is>
       </c>
     </row>
     <row r="45">
-      <c r="A45" t="inlineStr"/>
+      <c r="A45" t="n">
+        <v>1</v>
+      </c>
       <c r="B45" t="inlineStr">
         <is>
           <t>2023-07-19</t>
@@ -5614,10 +5644,22 @@
           <t>BetUS</t>
         </is>
       </c>
-      <c r="O45" t="inlineStr"/>
-      <c r="P45" t="inlineStr"/>
-      <c r="Q45" t="inlineStr"/>
-      <c r="R45" t="inlineStr"/>
+      <c r="O45" t="n">
+        <v>5</v>
+      </c>
+      <c r="P45" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q45" t="inlineStr">
+        <is>
+          <t>Brock Burke</t>
+        </is>
+      </c>
+      <c r="R45" t="inlineStr">
+        <is>
+          <t>Zack Littell</t>
+        </is>
+      </c>
       <c r="S45" t="n">
         <v>0.9997694620591119</v>
       </c>
@@ -5652,12 +5694,14 @@
       </c>
       <c r="AA45" t="inlineStr">
         <is>
-          <t>2023-07-19 - Tampa Bay Rays @ Texas Rangers (Scheduled)</t>
+          <t>2023-07-19 - Tampa Bay Rays (1) @ Texas Rangers (5) (Final)</t>
         </is>
       </c>
     </row>
     <row r="46">
-      <c r="A46" t="inlineStr"/>
+      <c r="A46" t="n">
+        <v>0</v>
+      </c>
       <c r="B46" t="inlineStr">
         <is>
           <t>2023-07-19</t>
@@ -5719,10 +5763,22 @@
           <t>FanDuel</t>
         </is>
       </c>
-      <c r="O46" t="inlineStr"/>
-      <c r="P46" t="inlineStr"/>
-      <c r="Q46" t="inlineStr"/>
-      <c r="R46" t="inlineStr"/>
+      <c r="O46" t="n">
+        <v>6</v>
+      </c>
+      <c r="P46" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q46" t="inlineStr">
+        <is>
+          <t>Zack Thompson</t>
+        </is>
+      </c>
+      <c r="R46" t="inlineStr">
+        <is>
+          <t>Sandy Alcantara</t>
+        </is>
+      </c>
       <c r="S46" t="n">
         <v>0.004766540830195167</v>
       </c>
@@ -5757,12 +5813,14 @@
       </c>
       <c r="AA46" t="inlineStr">
         <is>
-          <t>2023-07-19 - Miami Marlins @ St. Louis Cardinals (Scheduled)</t>
+          <t>2023-07-19 - Miami Marlins (4) @ St. Louis Cardinals (6) (Final)</t>
         </is>
       </c>
     </row>
     <row r="47">
-      <c r="A47" t="inlineStr"/>
+      <c r="A47" t="n">
+        <v>1</v>
+      </c>
       <c r="B47" t="inlineStr">
         <is>
           <t>2023-07-19</t>
@@ -5824,10 +5882,22 @@
           <t>BetOnline.ag</t>
         </is>
       </c>
-      <c r="O47" t="inlineStr"/>
-      <c r="P47" t="inlineStr"/>
-      <c r="Q47" t="inlineStr"/>
-      <c r="R47" t="inlineStr"/>
+      <c r="O47" t="n">
+        <v>1</v>
+      </c>
+      <c r="P47" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q47" t="inlineStr">
+        <is>
+          <t>Brandon Bielak</t>
+        </is>
+      </c>
+      <c r="R47" t="inlineStr">
+        <is>
+          <t>Austin Gomber</t>
+        </is>
+      </c>
       <c r="S47" t="n">
         <v>0.4733351460343699</v>
       </c>
@@ -5858,12 +5928,14 @@
       </c>
       <c r="AA47" t="inlineStr">
         <is>
-          <t>2023-07-19 - Houston Astros @ Colorado Rockies (Scheduled)</t>
+          <t>2023-07-19 - Houston Astros (4) @ Colorado Rockies (1) (Final)</t>
         </is>
       </c>
     </row>
     <row r="48">
-      <c r="A48" t="inlineStr"/>
+      <c r="A48" t="n">
+        <v>1</v>
+      </c>
       <c r="B48" t="inlineStr">
         <is>
           <t>2023-07-19</t>
@@ -5925,10 +5997,22 @@
           <t>Barstool Sportsbook</t>
         </is>
       </c>
-      <c r="O48" t="inlineStr"/>
-      <c r="P48" t="inlineStr"/>
-      <c r="Q48" t="inlineStr"/>
-      <c r="R48" t="inlineStr"/>
+      <c r="O48" t="n">
+        <v>6</v>
+      </c>
+      <c r="P48" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q48" t="inlineStr">
+        <is>
+          <t>Angel Felipe</t>
+        </is>
+      </c>
+      <c r="R48" t="inlineStr">
+        <is>
+          <t>Brayan Bello</t>
+        </is>
+      </c>
       <c r="S48" t="n">
         <v>0.9999978351043585</v>
       </c>
@@ -5959,12 +6043,14 @@
       </c>
       <c r="AA48" t="inlineStr">
         <is>
-          <t>2023-07-19 - Boston Red Sox @ Oakland Athletics (Scheduled)</t>
+          <t>2023-07-19 - Boston Red Sox (5) @ Oakland Athletics (6) (Final)</t>
         </is>
       </c>
     </row>
     <row r="49">
-      <c r="A49" t="inlineStr"/>
+      <c r="A49" t="n">
+        <v>1</v>
+      </c>
       <c r="B49" t="inlineStr">
         <is>
           <t>2023-07-19</t>
@@ -6026,10 +6112,22 @@
           <t>WynnBET</t>
         </is>
       </c>
-      <c r="O49" t="inlineStr"/>
-      <c r="P49" t="inlineStr"/>
-      <c r="Q49" t="inlineStr"/>
-      <c r="R49" t="inlineStr"/>
+      <c r="O49" t="n">
+        <v>3</v>
+      </c>
+      <c r="P49" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q49" t="inlineStr">
+        <is>
+          <t>Hoby Milner</t>
+        </is>
+      </c>
+      <c r="R49" t="inlineStr">
+        <is>
+          <t>Jeff Hoffman</t>
+        </is>
+      </c>
       <c r="S49" t="n">
         <v>0.0009301229950238579</v>
       </c>
@@ -6060,12 +6158,14 @@
       </c>
       <c r="AA49" t="inlineStr">
         <is>
-          <t>2023-07-19 - Milwaukee Brewers @ Philadelphia Phillies (Scheduled)</t>
+          <t>2023-07-19 - Milwaukee Brewers (5) @ Philadelphia Phillies (3) (Final)</t>
         </is>
       </c>
     </row>
     <row r="50">
-      <c r="A50" t="inlineStr"/>
+      <c r="A50" t="n">
+        <v>1</v>
+      </c>
       <c r="B50" t="inlineStr">
         <is>
           <t>2023-07-19</t>
@@ -6127,10 +6227,22 @@
           <t>WynnBET</t>
         </is>
       </c>
-      <c r="O50" t="inlineStr"/>
-      <c r="P50" t="inlineStr"/>
-      <c r="Q50" t="inlineStr"/>
-      <c r="R50" t="inlineStr"/>
+      <c r="O50" t="n">
+        <v>7</v>
+      </c>
+      <c r="P50" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q50" t="inlineStr">
+        <is>
+          <t>Chase Silseth</t>
+        </is>
+      </c>
+      <c r="R50" t="inlineStr">
+        <is>
+          <t>Carlos Rodon</t>
+        </is>
+      </c>
       <c r="S50" t="n">
         <v>0.8668874266933613</v>
       </c>
@@ -6165,12 +6277,14 @@
       </c>
       <c r="AA50" t="inlineStr">
         <is>
-          <t>2023-07-19 - New York Yankees @ Los Angeles Angels (Scheduled)</t>
+          <t>2023-07-19 - New York Yankees (3) @ Los Angeles Angels (7) (Final)</t>
         </is>
       </c>
     </row>
     <row r="51">
-      <c r="A51" t="inlineStr"/>
+      <c r="A51" t="n">
+        <v>0</v>
+      </c>
       <c r="B51" t="inlineStr">
         <is>
           <t>2023-07-19</t>
@@ -6232,10 +6346,22 @@
           <t>BetUS</t>
         </is>
       </c>
-      <c r="O51" t="inlineStr"/>
-      <c r="P51" t="inlineStr"/>
-      <c r="Q51" t="inlineStr"/>
-      <c r="R51" t="inlineStr"/>
+      <c r="O51" t="n">
+        <v>0</v>
+      </c>
+      <c r="P51" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q51" t="inlineStr">
+        <is>
+          <t>Yu Darvish</t>
+        </is>
+      </c>
+      <c r="R51" t="inlineStr">
+        <is>
+          <t>Jose Berrios</t>
+        </is>
+      </c>
       <c r="S51" t="n">
         <v>0.9363515524218616</v>
       </c>
@@ -6266,12 +6392,14 @@
       </c>
       <c r="AA51" t="inlineStr">
         <is>
-          <t>2023-07-19 - San Diego Padres @ Toronto Blue Jays (Scheduled)</t>
+          <t>2023-07-19 - San Diego Padres (2) @ Toronto Blue Jays (0) (Final)</t>
         </is>
       </c>
     </row>
     <row r="52">
-      <c r="A52" t="inlineStr"/>
+      <c r="A52" t="n">
+        <v>1</v>
+      </c>
       <c r="B52" t="inlineStr">
         <is>
           <t>2023-07-19</t>
@@ -6333,10 +6461,22 @@
           <t>BetUS</t>
         </is>
       </c>
-      <c r="O52" t="inlineStr"/>
-      <c r="P52" t="inlineStr"/>
-      <c r="Q52" t="inlineStr"/>
-      <c r="R52" t="inlineStr"/>
+      <c r="O52" t="n">
+        <v>5</v>
+      </c>
+      <c r="P52" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q52" t="inlineStr">
+        <is>
+          <t>Justin Verlander</t>
+        </is>
+      </c>
+      <c r="R52" t="inlineStr">
+        <is>
+          <t>Touki Toussaint</t>
+        </is>
+      </c>
       <c r="S52" t="n">
         <v>0.9993667752532492</v>
       </c>
@@ -6367,12 +6507,14 @@
       </c>
       <c r="AA52" t="inlineStr">
         <is>
-          <t>2023-07-19 - Chicago White Sox @ New York Mets (Scheduled)</t>
+          <t>2023-07-19 - Chicago White Sox (1) @ New York Mets (5) (Final)</t>
         </is>
       </c>
     </row>
     <row r="53">
-      <c r="A53" t="inlineStr"/>
+      <c r="A53" t="n">
+        <v>1</v>
+      </c>
       <c r="B53" t="inlineStr">
         <is>
           <t>2023-07-19</t>
@@ -6434,10 +6576,22 @@
           <t>LowVig.ag</t>
         </is>
       </c>
-      <c r="O53" t="inlineStr"/>
-      <c r="P53" t="inlineStr"/>
-      <c r="Q53" t="inlineStr"/>
-      <c r="R53" t="inlineStr"/>
+      <c r="O53" t="n">
+        <v>3</v>
+      </c>
+      <c r="P53" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q53" t="inlineStr">
+        <is>
+          <t>Graham Ashcraft</t>
+        </is>
+      </c>
+      <c r="R53" t="inlineStr">
+        <is>
+          <t>Ross Stripling</t>
+        </is>
+      </c>
       <c r="S53" t="n">
         <v>0.536277916375046</v>
       </c>
@@ -6468,12 +6622,14 @@
       </c>
       <c r="AA53" t="inlineStr">
         <is>
-          <t>2023-07-19 - San Francisco Giants @ Cincinnati Reds (Scheduled)</t>
+          <t>2023-07-19 - San Francisco Giants (2) @ Cincinnati Reds (3) (Final)</t>
         </is>
       </c>
     </row>
     <row r="54">
-      <c r="A54" t="inlineStr"/>
+      <c r="A54" t="n">
+        <v>1</v>
+      </c>
       <c r="B54" t="inlineStr">
         <is>
           <t>2023-07-19</t>
@@ -6535,10 +6691,22 @@
           <t>WynnBET</t>
         </is>
       </c>
-      <c r="O54" t="inlineStr"/>
-      <c r="P54" t="inlineStr"/>
-      <c r="Q54" t="inlineStr"/>
-      <c r="R54" t="inlineStr"/>
+      <c r="O54" t="n">
+        <v>3</v>
+      </c>
+      <c r="P54" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q54" t="inlineStr">
+        <is>
+          <t>Ryne Nelson</t>
+        </is>
+      </c>
+      <c r="R54" t="inlineStr">
+        <is>
+          <t>Charlie Morton</t>
+        </is>
+      </c>
       <c r="S54" t="n">
         <v>0.1525434741056577</v>
       </c>
@@ -6573,7 +6741,7 @@
       </c>
       <c r="AA54" t="inlineStr">
         <is>
-          <t>2023-07-19 - Arizona Diamondbacks @ Atlanta Braves (Scheduled)</t>
+          <t>2023-07-19 - Arizona Diamondbacks (5) @ Atlanta Braves (3) (Final)</t>
         </is>
       </c>
     </row>
@@ -6581,38 +6749,42 @@
       <c r="A55" t="inlineStr"/>
       <c r="B55" t="inlineStr">
         <is>
-          <t>2023-07-19</t>
+          <t>2023-07-20</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>08:05 pm</t>
+          <t>12:20 am</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>Chicago Cubs</t>
+          <t>Atlanta Braves</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>Kyle Hendricks</t>
+          <t>Spencer Strider</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>Washington Nationals</t>
-        </is>
-      </c>
-      <c r="G55" t="inlineStr"/>
+          <t>Arizona Diamondbacks</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>Zac Gallen</t>
+        </is>
+      </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>Washington Nationals</t>
+          <t>Arizona Diamondbacks</t>
         </is>
       </c>
       <c r="I55" t="inlineStr">
         <is>
-          <t>Chicago Cubs</t>
+          <t>Atlanta Braves</t>
         </is>
       </c>
       <c r="J55" t="inlineStr">
@@ -6620,20 +6792,24 @@
           <t>mlb3year</t>
         </is>
       </c>
-      <c r="K55" t="n">
-        <v>-156</v>
+      <c r="K55" t="inlineStr">
+        <is>
+          <t>-185</t>
+        </is>
       </c>
       <c r="L55" t="inlineStr">
         <is>
-          <t>BetOnline.ag</t>
-        </is>
-      </c>
-      <c r="M55" t="n">
-        <v>145</v>
+          <t>WynnBET</t>
+        </is>
+      </c>
+      <c r="M55" t="inlineStr">
+        <is>
+          <t>+173</t>
+        </is>
       </c>
       <c r="N55" t="inlineStr">
         <is>
-          <t>WynnBET</t>
+          <t>LowVig.ag</t>
         </is>
       </c>
       <c r="O55" t="inlineStr"/>
@@ -6641,36 +6817,40 @@
       <c r="Q55" t="inlineStr"/>
       <c r="R55" t="inlineStr"/>
       <c r="S55" t="n">
-        <v>0.07488718946408701</v>
+        <v>0.4695206874968715</v>
       </c>
       <c r="T55" t="inlineStr">
         <is>
-          <t>Wrigley Field</t>
-        </is>
-      </c>
-      <c r="U55" t="inlineStr"/>
+          <t>Truist Park</t>
+        </is>
+      </c>
+      <c r="U55" t="inlineStr">
+        <is>
+          <t>AZ leads 1-0</t>
+        </is>
+      </c>
       <c r="V55" t="inlineStr">
         <is>
           <t>['MLB.tv Free Game']</t>
         </is>
       </c>
       <c r="W55" s="2" t="n">
-        <v>45126.38147372685</v>
+        <v>45127.27906369951</v>
       </c>
       <c r="X55" s="2" t="n">
-        <v>45126.38227392361</v>
+        <v>45127.27912535644</v>
       </c>
       <c r="Y55" t="inlineStr">
         <is>
-          <t>2023-07-20T00:05:00Z</t>
+          <t>2023-07-20T16:20:00Z</t>
         </is>
       </c>
       <c r="Z55" t="n">
-        <v>717336</v>
+        <v>717337</v>
       </c>
       <c r="AA55" t="inlineStr">
         <is>
-          <t>2023-07-19 - Washington Nationals @ Chicago Cubs (Scheduled)</t>
+          <t>2023-07-20 - Arizona Diamondbacks @ Atlanta Braves (Scheduled)</t>
         </is>
       </c>
     </row>
@@ -6678,42 +6858,42 @@
       <c r="A56" t="inlineStr"/>
       <c r="B56" t="inlineStr">
         <is>
-          <t>2023-07-19</t>
+          <t>2023-07-20</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>08:10 pm</t>
+          <t>12:35 am</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>Kansas City Royals</t>
+          <t>Cincinnati Reds</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>Ryan Yarbrough</t>
+          <t>Andrew Abbott</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>Detroit Tigers</t>
+          <t>San Francisco Giants</t>
         </is>
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>Eduardo Rodriguez</t>
+          <t>Alex Cobb</t>
         </is>
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>Kansas City Royals</t>
+          <t>San Francisco Giants</t>
         </is>
       </c>
       <c r="I56" t="inlineStr">
         <is>
-          <t>Detroit Tigers</t>
+          <t>San Francisco Giants</t>
         </is>
       </c>
       <c r="J56" t="inlineStr">
@@ -6721,20 +6901,24 @@
           <t>mlb3year</t>
         </is>
       </c>
-      <c r="K56" t="n">
-        <v>137</v>
+      <c r="K56" t="inlineStr">
+        <is>
+          <t>+100</t>
+        </is>
       </c>
       <c r="L56" t="inlineStr">
         <is>
           <t>WynnBET</t>
         </is>
       </c>
-      <c r="M56" t="n">
-        <v>-144</v>
+      <c r="M56" t="inlineStr">
+        <is>
+          <t>-108</t>
+        </is>
       </c>
       <c r="N56" t="inlineStr">
         <is>
-          <t>BetUS</t>
+          <t>LowVig.ag</t>
         </is>
       </c>
       <c r="O56" t="inlineStr"/>
@@ -6742,11 +6926,11 @@
       <c r="Q56" t="inlineStr"/>
       <c r="R56" t="inlineStr"/>
       <c r="S56" t="n">
-        <v>0.8731348014230707</v>
+        <v>0.0732468978741056</v>
       </c>
       <c r="T56" t="inlineStr">
         <is>
-          <t>Kauffman Stadium</t>
+          <t>Great American Ball Park</t>
         </is>
       </c>
       <c r="U56" t="inlineStr"/>
@@ -6756,22 +6940,22 @@
         </is>
       </c>
       <c r="W56" s="2" t="n">
-        <v>45126.38147372685</v>
+        <v>45127.27906369951</v>
       </c>
       <c r="X56" s="2" t="n">
-        <v>45126.38233221065</v>
+        <v>45127.27918272444</v>
       </c>
       <c r="Y56" t="inlineStr">
         <is>
-          <t>2023-07-20T00:10:00Z</t>
+          <t>2023-07-20T16:35:00Z</t>
         </is>
       </c>
       <c r="Z56" t="n">
-        <v>717333</v>
+        <v>717334</v>
       </c>
       <c r="AA56" t="inlineStr">
         <is>
-          <t>2023-07-19 - Detroit Tigers @ Kansas City Royals (Scheduled)</t>
+          <t>2023-07-20 - San Francisco Giants @ Cincinnati Reds (Scheduled)</t>
         </is>
       </c>
     </row>
@@ -6779,42 +6963,42 @@
       <c r="A57" t="inlineStr"/>
       <c r="B57" t="inlineStr">
         <is>
-          <t>2023-07-19</t>
+          <t>2023-07-20</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>09:40 pm</t>
+          <t>12:35 am</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>Seattle Mariners</t>
+          <t>Philadelphia Phillies</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>Luis Castillo</t>
+          <t>Taijuan Walker</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>Minnesota Twins</t>
+          <t>Milwaukee Brewers</t>
         </is>
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>Kenta Maeda</t>
+          <t>Corbin Burnes</t>
         </is>
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>Seattle Mariners</t>
+          <t>Milwaukee Brewers</t>
         </is>
       </c>
       <c r="I57" t="inlineStr">
         <is>
-          <t>Seattle Mariners</t>
+          <t>Philadelphia Phillies</t>
         </is>
       </c>
       <c r="J57" t="inlineStr">
@@ -6822,20 +7006,24 @@
           <t>mlb3year</t>
         </is>
       </c>
-      <c r="K57" t="n">
-        <v>-154</v>
+      <c r="K57" t="inlineStr">
+        <is>
+          <t>-115</t>
+        </is>
       </c>
       <c r="L57" t="inlineStr">
         <is>
-          <t>WynnBET</t>
-        </is>
-      </c>
-      <c r="M57" t="n">
-        <v>143</v>
+          <t>DraftKings</t>
+        </is>
+      </c>
+      <c r="M57" t="inlineStr">
+        <is>
+          <t>+108</t>
+        </is>
       </c>
       <c r="N57" t="inlineStr">
         <is>
-          <t>BetRivers</t>
+          <t>BetUS</t>
         </is>
       </c>
       <c r="O57" t="inlineStr"/>
@@ -6843,36 +7031,561 @@
       <c r="Q57" t="inlineStr"/>
       <c r="R57" t="inlineStr"/>
       <c r="S57" t="n">
-        <v>0.9988873370697626</v>
+        <v>0.3252375958705956</v>
       </c>
       <c r="T57" t="inlineStr">
         <is>
-          <t>T-Mobile Park</t>
+          <t>Citizens Bank Park</t>
         </is>
       </c>
       <c r="U57" t="inlineStr"/>
       <c r="V57" t="inlineStr">
         <is>
+          <t>['MLB.tv Free Game']</t>
+        </is>
+      </c>
+      <c r="W57" s="2" t="n">
+        <v>45127.27906369951</v>
+      </c>
+      <c r="X57" s="2" t="n">
+        <v>45127.27924562299</v>
+      </c>
+      <c r="Y57" t="inlineStr">
+        <is>
+          <t>2023-07-20T16:35:00Z</t>
+        </is>
+      </c>
+      <c r="Z57" t="n">
+        <v>717329</v>
+      </c>
+      <c r="AA57" t="inlineStr">
+        <is>
+          <t>2023-07-20 - Milwaukee Brewers @ Philadelphia Phillies (Scheduled)</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr"/>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>2023-07-20</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>01:07 pm</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>Toronto Blue Jays</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>Chris Bassitt</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>San Diego Padres</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>Blake Snell</t>
+        </is>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>Toronto Blue Jays</t>
+        </is>
+      </c>
+      <c r="I58" t="inlineStr">
+        <is>
+          <t>San Diego Padres</t>
+        </is>
+      </c>
+      <c r="J58" t="inlineStr">
+        <is>
+          <t>mlb3year</t>
+        </is>
+      </c>
+      <c r="K58" t="inlineStr">
+        <is>
+          <t>+108</t>
+        </is>
+      </c>
+      <c r="L58" t="inlineStr">
+        <is>
+          <t>WynnBET</t>
+        </is>
+      </c>
+      <c r="M58" t="inlineStr">
+        <is>
+          <t>-108</t>
+        </is>
+      </c>
+      <c r="N58" t="inlineStr">
+        <is>
+          <t>BetUS</t>
+        </is>
+      </c>
+      <c r="O58" t="inlineStr"/>
+      <c r="P58" t="inlineStr"/>
+      <c r="Q58" t="inlineStr"/>
+      <c r="R58" t="inlineStr"/>
+      <c r="S58" t="n">
+        <v>0.8887572426968487</v>
+      </c>
+      <c r="T58" t="inlineStr">
+        <is>
+          <t>Rogers Centre</t>
+        </is>
+      </c>
+      <c r="U58" t="inlineStr"/>
+      <c r="V58" t="inlineStr">
+        <is>
+          <t>['MLBN (out-of-market only)']</t>
+        </is>
+      </c>
+      <c r="W58" s="2" t="n">
+        <v>45127.27906369951</v>
+      </c>
+      <c r="X58" s="2" t="n">
+        <v>45127.27929616844</v>
+      </c>
+      <c r="Y58" t="inlineStr">
+        <is>
+          <t>2023-07-20T17:07:00Z</t>
+        </is>
+      </c>
+      <c r="Z58" t="n">
+        <v>717331</v>
+      </c>
+      <c r="AA58" t="inlineStr">
+        <is>
+          <t>2023-07-20 - San Diego Padres @ Toronto Blue Jays (Scheduled)</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr"/>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>2023-07-20</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>03:40 pm</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>Seattle Mariners</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>George Kirby</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>Minnesota Twins</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>Pablo Lopez</t>
+        </is>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>Seattle Mariners</t>
+        </is>
+      </c>
+      <c r="I59" t="inlineStr">
+        <is>
+          <t>Seattle Mariners</t>
+        </is>
+      </c>
+      <c r="J59" t="inlineStr">
+        <is>
+          <t>mlb3year</t>
+        </is>
+      </c>
+      <c r="K59" t="inlineStr">
+        <is>
+          <t>-125</t>
+        </is>
+      </c>
+      <c r="L59" t="inlineStr">
+        <is>
+          <t>LowVig.ag</t>
+        </is>
+      </c>
+      <c r="M59" t="inlineStr">
+        <is>
+          <t>+120</t>
+        </is>
+      </c>
+      <c r="N59" t="inlineStr">
+        <is>
+          <t>BetUS</t>
+        </is>
+      </c>
+      <c r="O59" t="inlineStr"/>
+      <c r="P59" t="inlineStr"/>
+      <c r="Q59" t="inlineStr"/>
+      <c r="R59" t="inlineStr"/>
+      <c r="S59" t="n">
+        <v>0.9938109105629366</v>
+      </c>
+      <c r="T59" t="inlineStr">
+        <is>
+          <t>T-Mobile Park</t>
+        </is>
+      </c>
+      <c r="U59" t="inlineStr"/>
+      <c r="V59" t="inlineStr">
+        <is>
           <t>[]</t>
         </is>
       </c>
-      <c r="W57" s="2" t="n">
-        <v>45126.38147372685</v>
-      </c>
-      <c r="X57" s="2" t="n">
-        <v>45126.38239841435</v>
-      </c>
-      <c r="Y57" t="inlineStr">
-        <is>
-          <t>2023-07-20T01:40:00Z</t>
-        </is>
-      </c>
-      <c r="Z57" t="n">
-        <v>717335</v>
-      </c>
-      <c r="AA57" t="inlineStr">
-        <is>
-          <t>2023-07-19 - Minnesota Twins @ Seattle Mariners (Scheduled)</t>
+      <c r="W59" s="2" t="n">
+        <v>45127.27906369951</v>
+      </c>
+      <c r="X59" s="2" t="n">
+        <v>45127.27940342962</v>
+      </c>
+      <c r="Y59" t="inlineStr">
+        <is>
+          <t>2023-07-20T19:40:00Z</t>
+        </is>
+      </c>
+      <c r="Z59" t="n">
+        <v>717327</v>
+      </c>
+      <c r="AA59" t="inlineStr">
+        <is>
+          <t>2023-07-20 - Minnesota Twins @ Seattle Mariners (Scheduled)</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr"/>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>2023-07-20</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>06:40 pm</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>Tampa Bay Rays</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>Tyler Glasnow</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>Baltimore Orioles</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>Kyle Gibson</t>
+        </is>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>Baltimore Orioles</t>
+        </is>
+      </c>
+      <c r="I60" t="inlineStr">
+        <is>
+          <t>Tampa Bay Rays</t>
+        </is>
+      </c>
+      <c r="J60" t="inlineStr">
+        <is>
+          <t>mlb3year</t>
+        </is>
+      </c>
+      <c r="K60" t="inlineStr">
+        <is>
+          <t>-172</t>
+        </is>
+      </c>
+      <c r="L60" t="inlineStr">
+        <is>
+          <t>BetOnline.ag</t>
+        </is>
+      </c>
+      <c r="M60" t="inlineStr">
+        <is>
+          <t>+163</t>
+        </is>
+      </c>
+      <c r="N60" t="inlineStr">
+        <is>
+          <t>WynnBET</t>
+        </is>
+      </c>
+      <c r="O60" t="inlineStr"/>
+      <c r="P60" t="inlineStr"/>
+      <c r="Q60" t="inlineStr"/>
+      <c r="R60" t="inlineStr"/>
+      <c r="S60" t="n">
+        <v>0.001574099333216134</v>
+      </c>
+      <c r="T60" t="inlineStr">
+        <is>
+          <t>Tropicana Field</t>
+        </is>
+      </c>
+      <c r="U60" t="inlineStr"/>
+      <c r="V60" t="inlineStr">
+        <is>
+          <t>['MLBN (out-of-market only)']</t>
+        </is>
+      </c>
+      <c r="W60" s="2" t="n">
+        <v>45127.27906369951</v>
+      </c>
+      <c r="X60" s="2" t="n">
+        <v>45127.27946030719</v>
+      </c>
+      <c r="Y60" t="inlineStr">
+        <is>
+          <t>2023-07-20T22:40:00Z</t>
+        </is>
+      </c>
+      <c r="Z60" t="n">
+        <v>717328</v>
+      </c>
+      <c r="AA60" t="inlineStr">
+        <is>
+          <t>2023-07-20 - Baltimore Orioles @ Tampa Bay Rays (Scheduled)</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr"/>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>2023-07-20</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>08:05 pm</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>Chicago Cubs</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>Marcus Stroman</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>St. Louis Cardinals</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>Steven Matz</t>
+        </is>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>Chicago Cubs</t>
+        </is>
+      </c>
+      <c r="I61" t="inlineStr">
+        <is>
+          <t>Chicago Cubs</t>
+        </is>
+      </c>
+      <c r="J61" t="inlineStr">
+        <is>
+          <t>mlb3year</t>
+        </is>
+      </c>
+      <c r="K61" t="inlineStr">
+        <is>
+          <t>-122</t>
+        </is>
+      </c>
+      <c r="L61" t="inlineStr">
+        <is>
+          <t>BetOnline.ag</t>
+        </is>
+      </c>
+      <c r="M61" t="inlineStr">
+        <is>
+          <t>+120</t>
+        </is>
+      </c>
+      <c r="N61" t="inlineStr">
+        <is>
+          <t>BetUS</t>
+        </is>
+      </c>
+      <c r="O61" t="inlineStr"/>
+      <c r="P61" t="inlineStr"/>
+      <c r="Q61" t="inlineStr"/>
+      <c r="R61" t="inlineStr"/>
+      <c r="S61" t="n">
+        <v>0.9994137162646376</v>
+      </c>
+      <c r="T61" t="inlineStr">
+        <is>
+          <t>Wrigley Field</t>
+        </is>
+      </c>
+      <c r="U61" t="inlineStr"/>
+      <c r="V61" t="inlineStr">
+        <is>
+          <t>['MLBN (out-of-market only)']</t>
+        </is>
+      </c>
+      <c r="W61" s="2" t="n">
+        <v>45127.27906369951</v>
+      </c>
+      <c r="X61" s="2" t="n">
+        <v>45127.27951728118</v>
+      </c>
+      <c r="Y61" t="inlineStr">
+        <is>
+          <t>2023-07-21T00:05:00Z</t>
+        </is>
+      </c>
+      <c r="Z61" t="n">
+        <v>717322</v>
+      </c>
+      <c r="AA61" t="inlineStr">
+        <is>
+          <t>2023-07-20 - St. Louis Cardinals @ Chicago Cubs (Scheduled)</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr"/>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>2023-07-20</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>09:40 pm</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>Oakland Athletics</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>Hogan Harris</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>Houston Astros</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>J.P. France</t>
+        </is>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>Oakland Athletics</t>
+        </is>
+      </c>
+      <c r="I62" t="inlineStr">
+        <is>
+          <t>Houston Astros</t>
+        </is>
+      </c>
+      <c r="J62" t="inlineStr">
+        <is>
+          <t>mlb3year</t>
+        </is>
+      </c>
+      <c r="K62" t="inlineStr">
+        <is>
+          <t>+170</t>
+        </is>
+      </c>
+      <c r="L62" t="inlineStr">
+        <is>
+          <t>BetUS</t>
+        </is>
+      </c>
+      <c r="M62" t="inlineStr">
+        <is>
+          <t>-179</t>
+        </is>
+      </c>
+      <c r="N62" t="inlineStr">
+        <is>
+          <t>WynnBET</t>
+        </is>
+      </c>
+      <c r="O62" t="inlineStr"/>
+      <c r="P62" t="inlineStr"/>
+      <c r="Q62" t="inlineStr"/>
+      <c r="R62" t="inlineStr"/>
+      <c r="S62" t="n">
+        <v>0.9995162971117549</v>
+      </c>
+      <c r="T62" t="inlineStr">
+        <is>
+          <t>Oakland Coliseum</t>
+        </is>
+      </c>
+      <c r="U62" t="inlineStr"/>
+      <c r="V62" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="W62" s="2" t="n">
+        <v>45127.27906369951</v>
+      </c>
+      <c r="X62" s="2" t="n">
+        <v>45127.27958179291</v>
+      </c>
+      <c r="Y62" t="inlineStr">
+        <is>
+          <t>2023-07-21T01:40:00Z</t>
+        </is>
+      </c>
+      <c r="Z62" t="n">
+        <v>717323</v>
+      </c>
+      <c r="AA62" t="inlineStr">
+        <is>
+          <t>2023-07-20 - Houston Astros @ Oakland Athletics (Scheduled)</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
predictions for 7/22/2023 (64% acc yesterday)
</commit_message>
<xml_diff>
--- a/data/predictions.xlsx
+++ b/data/predictions.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA62"/>
+  <dimension ref="A1:AA83"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6746,7 +6746,9 @@
       </c>
     </row>
     <row r="55">
-      <c r="A55" t="inlineStr"/>
+      <c r="A55" t="n">
+        <v>0</v>
+      </c>
       <c r="B55" t="inlineStr">
         <is>
           <t>2023-07-20</t>
@@ -6792,30 +6794,38 @@
           <t>mlb3year</t>
         </is>
       </c>
-      <c r="K55" t="inlineStr">
-        <is>
-          <t>-185</t>
-        </is>
+      <c r="K55" t="n">
+        <v>-185</v>
       </c>
       <c r="L55" t="inlineStr">
         <is>
           <t>WynnBET</t>
         </is>
       </c>
-      <c r="M55" t="inlineStr">
-        <is>
-          <t>+173</t>
-        </is>
+      <c r="M55" t="n">
+        <v>173</v>
       </c>
       <c r="N55" t="inlineStr">
         <is>
           <t>LowVig.ag</t>
         </is>
       </c>
-      <c r="O55" t="inlineStr"/>
-      <c r="P55" t="inlineStr"/>
-      <c r="Q55" t="inlineStr"/>
-      <c r="R55" t="inlineStr"/>
+      <c r="O55" t="n">
+        <v>7</v>
+      </c>
+      <c r="P55" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q55" t="inlineStr">
+        <is>
+          <t>Kirby Yates</t>
+        </is>
+      </c>
+      <c r="R55" t="inlineStr">
+        <is>
+          <t>Miguel Castro</t>
+        </is>
+      </c>
       <c r="S55" t="n">
         <v>0.4695206874968715</v>
       </c>
@@ -6835,10 +6845,10 @@
         </is>
       </c>
       <c r="W55" s="2" t="n">
-        <v>45127.27906369951</v>
+        <v>45127.2790637037</v>
       </c>
       <c r="X55" s="2" t="n">
-        <v>45127.27912535644</v>
+        <v>45127.27912535879</v>
       </c>
       <c r="Y55" t="inlineStr">
         <is>
@@ -6850,12 +6860,14 @@
       </c>
       <c r="AA55" t="inlineStr">
         <is>
-          <t>2023-07-20 - Arizona Diamondbacks @ Atlanta Braves (Scheduled)</t>
+          <t>2023-07-20 - Arizona Diamondbacks (5) @ Atlanta Braves (7) (Final)</t>
         </is>
       </c>
     </row>
     <row r="56">
-      <c r="A56" t="inlineStr"/>
+      <c r="A56" t="n">
+        <v>0</v>
+      </c>
       <c r="B56" t="inlineStr">
         <is>
           <t>2023-07-20</t>
@@ -6901,30 +6913,38 @@
           <t>mlb3year</t>
         </is>
       </c>
-      <c r="K56" t="inlineStr">
-        <is>
-          <t>+100</t>
-        </is>
+      <c r="K56" t="n">
+        <v>100</v>
       </c>
       <c r="L56" t="inlineStr">
         <is>
           <t>WynnBET</t>
         </is>
       </c>
-      <c r="M56" t="inlineStr">
-        <is>
-          <t>-108</t>
-        </is>
+      <c r="M56" t="n">
+        <v>-108</v>
       </c>
       <c r="N56" t="inlineStr">
         <is>
           <t>LowVig.ag</t>
         </is>
       </c>
-      <c r="O56" t="inlineStr"/>
-      <c r="P56" t="inlineStr"/>
-      <c r="Q56" t="inlineStr"/>
-      <c r="R56" t="inlineStr"/>
+      <c r="O56" t="n">
+        <v>5</v>
+      </c>
+      <c r="P56" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q56" t="inlineStr">
+        <is>
+          <t>Andrew Abbott</t>
+        </is>
+      </c>
+      <c r="R56" t="inlineStr">
+        <is>
+          <t>Alex Cobb</t>
+        </is>
+      </c>
       <c r="S56" t="n">
         <v>0.0732468978741056</v>
       </c>
@@ -6940,10 +6960,10 @@
         </is>
       </c>
       <c r="W56" s="2" t="n">
-        <v>45127.27906369951</v>
+        <v>45127.2790637037</v>
       </c>
       <c r="X56" s="2" t="n">
-        <v>45127.27918272444</v>
+        <v>45127.27918271991</v>
       </c>
       <c r="Y56" t="inlineStr">
         <is>
@@ -6955,12 +6975,14 @@
       </c>
       <c r="AA56" t="inlineStr">
         <is>
-          <t>2023-07-20 - San Francisco Giants @ Cincinnati Reds (Scheduled)</t>
+          <t>2023-07-20 - San Francisco Giants (1) @ Cincinnati Reds (5) (Final)</t>
         </is>
       </c>
     </row>
     <row r="57">
-      <c r="A57" t="inlineStr"/>
+      <c r="A57" t="n">
+        <v>1</v>
+      </c>
       <c r="B57" t="inlineStr">
         <is>
           <t>2023-07-20</t>
@@ -7006,30 +7028,38 @@
           <t>mlb3year</t>
         </is>
       </c>
-      <c r="K57" t="inlineStr">
-        <is>
-          <t>-115</t>
-        </is>
+      <c r="K57" t="n">
+        <v>-115</v>
       </c>
       <c r="L57" t="inlineStr">
         <is>
           <t>DraftKings</t>
         </is>
       </c>
-      <c r="M57" t="inlineStr">
-        <is>
-          <t>+108</t>
-        </is>
+      <c r="M57" t="n">
+        <v>108</v>
       </c>
       <c r="N57" t="inlineStr">
         <is>
           <t>BetUS</t>
         </is>
       </c>
-      <c r="O57" t="inlineStr"/>
-      <c r="P57" t="inlineStr"/>
-      <c r="Q57" t="inlineStr"/>
-      <c r="R57" t="inlineStr"/>
+      <c r="O57" t="n">
+        <v>0</v>
+      </c>
+      <c r="P57" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q57" t="inlineStr">
+        <is>
+          <t>Corbin Burnes</t>
+        </is>
+      </c>
+      <c r="R57" t="inlineStr">
+        <is>
+          <t>Taijuan Walker</t>
+        </is>
+      </c>
       <c r="S57" t="n">
         <v>0.3252375958705956</v>
       </c>
@@ -7045,10 +7075,10 @@
         </is>
       </c>
       <c r="W57" s="2" t="n">
-        <v>45127.27906369951</v>
+        <v>45127.2790637037</v>
       </c>
       <c r="X57" s="2" t="n">
-        <v>45127.27924562299</v>
+        <v>45127.279245625</v>
       </c>
       <c r="Y57" t="inlineStr">
         <is>
@@ -7060,12 +7090,14 @@
       </c>
       <c r="AA57" t="inlineStr">
         <is>
-          <t>2023-07-20 - Milwaukee Brewers @ Philadelphia Phillies (Scheduled)</t>
+          <t>2023-07-20 - Milwaukee Brewers (4) @ Philadelphia Phillies (0) (Final)</t>
         </is>
       </c>
     </row>
     <row r="58">
-      <c r="A58" t="inlineStr"/>
+      <c r="A58" t="n">
+        <v>1</v>
+      </c>
       <c r="B58" t="inlineStr">
         <is>
           <t>2023-07-20</t>
@@ -7111,30 +7143,38 @@
           <t>mlb3year</t>
         </is>
       </c>
-      <c r="K58" t="inlineStr">
-        <is>
-          <t>+108</t>
-        </is>
+      <c r="K58" t="n">
+        <v>108</v>
       </c>
       <c r="L58" t="inlineStr">
         <is>
           <t>WynnBET</t>
         </is>
       </c>
-      <c r="M58" t="inlineStr">
-        <is>
-          <t>-108</t>
-        </is>
+      <c r="M58" t="n">
+        <v>-108</v>
       </c>
       <c r="N58" t="inlineStr">
         <is>
           <t>BetUS</t>
         </is>
       </c>
-      <c r="O58" t="inlineStr"/>
-      <c r="P58" t="inlineStr"/>
-      <c r="Q58" t="inlineStr"/>
-      <c r="R58" t="inlineStr"/>
+      <c r="O58" t="n">
+        <v>4</v>
+      </c>
+      <c r="P58" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q58" t="inlineStr">
+        <is>
+          <t>Chris Bassitt</t>
+        </is>
+      </c>
+      <c r="R58" t="inlineStr">
+        <is>
+          <t>Blake Snell</t>
+        </is>
+      </c>
       <c r="S58" t="n">
         <v>0.8887572426968487</v>
       </c>
@@ -7150,10 +7190,10 @@
         </is>
       </c>
       <c r="W58" s="2" t="n">
-        <v>45127.27906369951</v>
+        <v>45127.2790637037</v>
       </c>
       <c r="X58" s="2" t="n">
-        <v>45127.27929616844</v>
+        <v>45127.27929616898</v>
       </c>
       <c r="Y58" t="inlineStr">
         <is>
@@ -7165,12 +7205,14 @@
       </c>
       <c r="AA58" t="inlineStr">
         <is>
-          <t>2023-07-20 - San Diego Padres @ Toronto Blue Jays (Scheduled)</t>
+          <t>2023-07-20 - San Diego Padres (0) @ Toronto Blue Jays (4) (Final)</t>
         </is>
       </c>
     </row>
     <row r="59">
-      <c r="A59" t="inlineStr"/>
+      <c r="A59" t="n">
+        <v>1</v>
+      </c>
       <c r="B59" t="inlineStr">
         <is>
           <t>2023-07-20</t>
@@ -7216,30 +7258,38 @@
           <t>mlb3year</t>
         </is>
       </c>
-      <c r="K59" t="inlineStr">
-        <is>
-          <t>-125</t>
-        </is>
+      <c r="K59" t="n">
+        <v>-125</v>
       </c>
       <c r="L59" t="inlineStr">
         <is>
           <t>LowVig.ag</t>
         </is>
       </c>
-      <c r="M59" t="inlineStr">
-        <is>
-          <t>+120</t>
-        </is>
+      <c r="M59" t="n">
+        <v>120</v>
       </c>
       <c r="N59" t="inlineStr">
         <is>
           <t>BetUS</t>
         </is>
       </c>
-      <c r="O59" t="inlineStr"/>
-      <c r="P59" t="inlineStr"/>
-      <c r="Q59" t="inlineStr"/>
-      <c r="R59" t="inlineStr"/>
+      <c r="O59" t="n">
+        <v>5</v>
+      </c>
+      <c r="P59" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q59" t="inlineStr">
+        <is>
+          <t>George Kirby</t>
+        </is>
+      </c>
+      <c r="R59" t="inlineStr">
+        <is>
+          <t>Pablo Lopez</t>
+        </is>
+      </c>
       <c r="S59" t="n">
         <v>0.9938109105629366</v>
       </c>
@@ -7255,10 +7305,10 @@
         </is>
       </c>
       <c r="W59" s="2" t="n">
-        <v>45127.27906369951</v>
+        <v>45127.2790637037</v>
       </c>
       <c r="X59" s="2" t="n">
-        <v>45127.27940342962</v>
+        <v>45127.27940342593</v>
       </c>
       <c r="Y59" t="inlineStr">
         <is>
@@ -7270,12 +7320,14 @@
       </c>
       <c r="AA59" t="inlineStr">
         <is>
-          <t>2023-07-20 - Minnesota Twins @ Seattle Mariners (Scheduled)</t>
+          <t>2023-07-20 - Minnesota Twins (0) @ Seattle Mariners (5) (Final)</t>
         </is>
       </c>
     </row>
     <row r="60">
-      <c r="A60" t="inlineStr"/>
+      <c r="A60" t="n">
+        <v>1</v>
+      </c>
       <c r="B60" t="inlineStr">
         <is>
           <t>2023-07-20</t>
@@ -7321,30 +7373,38 @@
           <t>mlb3year</t>
         </is>
       </c>
-      <c r="K60" t="inlineStr">
-        <is>
-          <t>-172</t>
-        </is>
+      <c r="K60" t="n">
+        <v>-172</v>
       </c>
       <c r="L60" t="inlineStr">
         <is>
           <t>BetOnline.ag</t>
         </is>
       </c>
-      <c r="M60" t="inlineStr">
-        <is>
-          <t>+163</t>
-        </is>
+      <c r="M60" t="n">
+        <v>163</v>
       </c>
       <c r="N60" t="inlineStr">
         <is>
           <t>WynnBET</t>
         </is>
       </c>
-      <c r="O60" t="inlineStr"/>
-      <c r="P60" t="inlineStr"/>
-      <c r="Q60" t="inlineStr"/>
-      <c r="R60" t="inlineStr"/>
+      <c r="O60" t="n">
+        <v>3</v>
+      </c>
+      <c r="P60" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q60" t="inlineStr">
+        <is>
+          <t>Felix Bautista</t>
+        </is>
+      </c>
+      <c r="R60" t="inlineStr">
+        <is>
+          <t>Robert Stephenson</t>
+        </is>
+      </c>
       <c r="S60" t="n">
         <v>0.001574099333216134</v>
       </c>
@@ -7360,10 +7420,10 @@
         </is>
       </c>
       <c r="W60" s="2" t="n">
-        <v>45127.27906369951</v>
+        <v>45127.2790637037</v>
       </c>
       <c r="X60" s="2" t="n">
-        <v>45127.27946030719</v>
+        <v>45127.2794603125</v>
       </c>
       <c r="Y60" t="inlineStr">
         <is>
@@ -7375,20 +7435,22 @@
       </c>
       <c r="AA60" t="inlineStr">
         <is>
-          <t>2023-07-20 - Baltimore Orioles @ Tampa Bay Rays (Scheduled)</t>
+          <t>2023-07-20 - Baltimore Orioles (4) @ Tampa Bay Rays (3) (Final)</t>
         </is>
       </c>
     </row>
     <row r="61">
-      <c r="A61" t="inlineStr"/>
+      <c r="A61" t="n">
+        <v>1</v>
+      </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>2023-07-20</t>
+          <t>2023-07-21</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>08:05 pm</t>
+          <t>02:20 pm</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
@@ -7398,7 +7460,7 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>Marcus Stroman</t>
+          <t>Justin Steele</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -7408,7 +7470,7 @@
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>Steven Matz</t>
+          <t>Jack Flaherty</t>
         </is>
       </c>
       <c r="H61" t="inlineStr">
@@ -7426,32 +7488,40 @@
           <t>mlb3year</t>
         </is>
       </c>
-      <c r="K61" t="inlineStr">
-        <is>
-          <t>-122</t>
-        </is>
+      <c r="K61" t="n">
+        <v>-122</v>
       </c>
       <c r="L61" t="inlineStr">
         <is>
-          <t>BetOnline.ag</t>
-        </is>
-      </c>
-      <c r="M61" t="inlineStr">
-        <is>
-          <t>+120</t>
-        </is>
+          <t>WynnBET</t>
+        </is>
+      </c>
+      <c r="M61" t="n">
+        <v>114</v>
       </c>
       <c r="N61" t="inlineStr">
         <is>
           <t>BetUS</t>
         </is>
       </c>
-      <c r="O61" t="inlineStr"/>
-      <c r="P61" t="inlineStr"/>
-      <c r="Q61" t="inlineStr"/>
-      <c r="R61" t="inlineStr"/>
+      <c r="O61" t="n">
+        <v>4</v>
+      </c>
+      <c r="P61" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q61" t="inlineStr">
+        <is>
+          <t>Justin Steele</t>
+        </is>
+      </c>
+      <c r="R61" t="inlineStr">
+        <is>
+          <t>Jack Flaherty</t>
+        </is>
+      </c>
       <c r="S61" t="n">
-        <v>0.9994137162646376</v>
+        <v>0.9976013897168008</v>
       </c>
       <c r="T61" t="inlineStr">
         <is>
@@ -7461,69 +7531,71 @@
       <c r="U61" t="inlineStr"/>
       <c r="V61" t="inlineStr">
         <is>
-          <t>['MLBN (out-of-market only)']</t>
+          <t>['Apple TV+']</t>
         </is>
       </c>
       <c r="W61" s="2" t="n">
-        <v>45127.27906369951</v>
+        <v>45128.41919939815</v>
       </c>
       <c r="X61" s="2" t="n">
-        <v>45127.27951728118</v>
+        <v>45128.41927060185</v>
       </c>
       <c r="Y61" t="inlineStr">
         <is>
-          <t>2023-07-21T00:05:00Z</t>
+          <t>2023-07-21T18:20:00Z</t>
         </is>
       </c>
       <c r="Z61" t="n">
-        <v>717322</v>
+        <v>717325</v>
       </c>
       <c r="AA61" t="inlineStr">
         <is>
-          <t>2023-07-20 - St. Louis Cardinals @ Chicago Cubs (Scheduled)</t>
+          <t>2023-07-21 - St. Louis Cardinals (3) @ Chicago Cubs (4) (Final)</t>
         </is>
       </c>
     </row>
     <row r="62">
-      <c r="A62" t="inlineStr"/>
+      <c r="A62" t="n">
+        <v>0</v>
+      </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>2023-07-20</t>
+          <t>2023-07-21</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>09:40 pm</t>
+          <t>06:40 pm</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>Oakland Athletics</t>
+          <t>Tampa Bay Rays</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>Hogan Harris</t>
+          <t>Zach Eflin</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>Houston Astros</t>
+          <t>Baltimore Orioles</t>
         </is>
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>J.P. France</t>
+          <t>Kyle Bradish</t>
         </is>
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>Oakland Athletics</t>
+          <t>Baltimore Orioles</t>
         </is>
       </c>
       <c r="I62" t="inlineStr">
         <is>
-          <t>Houston Astros</t>
+          <t>Tampa Bay Rays</t>
         </is>
       </c>
       <c r="J62" t="inlineStr">
@@ -7531,36 +7603,44 @@
           <t>mlb3year</t>
         </is>
       </c>
-      <c r="K62" t="inlineStr">
-        <is>
-          <t>+170</t>
-        </is>
+      <c r="K62" t="n">
+        <v>-140</v>
       </c>
       <c r="L62" t="inlineStr">
         <is>
           <t>BetUS</t>
         </is>
       </c>
-      <c r="M62" t="inlineStr">
-        <is>
-          <t>-179</t>
-        </is>
+      <c r="M62" t="n">
+        <v>132</v>
       </c>
       <c r="N62" t="inlineStr">
         <is>
-          <t>WynnBET</t>
-        </is>
-      </c>
-      <c r="O62" t="inlineStr"/>
-      <c r="P62" t="inlineStr"/>
-      <c r="Q62" t="inlineStr"/>
-      <c r="R62" t="inlineStr"/>
+          <t>FanDuel</t>
+        </is>
+      </c>
+      <c r="O62" t="n">
+        <v>3</v>
+      </c>
+      <c r="P62" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q62" t="inlineStr">
+        <is>
+          <t>Zach Eflin</t>
+        </is>
+      </c>
+      <c r="R62" t="inlineStr">
+        <is>
+          <t>Kyle Bradish</t>
+        </is>
+      </c>
       <c r="S62" t="n">
-        <v>0.9995162971117549</v>
+        <v>0.1492536186240842</v>
       </c>
       <c r="T62" t="inlineStr">
         <is>
-          <t>Oakland Coliseum</t>
+          <t>Tropicana Field</t>
         </is>
       </c>
       <c r="U62" t="inlineStr"/>
@@ -7570,22 +7650,2287 @@
         </is>
       </c>
       <c r="W62" s="2" t="n">
-        <v>45127.27906369951</v>
+        <v>45128.41919939815</v>
       </c>
       <c r="X62" s="2" t="n">
-        <v>45127.27958179291</v>
+        <v>45128.41932818287</v>
       </c>
       <c r="Y62" t="inlineStr">
         <is>
-          <t>2023-07-21T01:40:00Z</t>
+          <t>2023-07-21T22:40:00Z</t>
         </is>
       </c>
       <c r="Z62" t="n">
-        <v>717323</v>
+        <v>717320</v>
       </c>
       <c r="AA62" t="inlineStr">
         <is>
-          <t>2023-07-20 - Houston Astros @ Oakland Athletics (Scheduled)</t>
+          <t>2023-07-21 - Baltimore Orioles (0) @ Tampa Bay Rays (3) (Final)</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>1</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>2023-07-21</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>06:40 pm</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>Miami Marlins</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>Braxton Garrett</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>Colorado Rockies</t>
+        </is>
+      </c>
+      <c r="G63" t="inlineStr"/>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>Colorado Rockies</t>
+        </is>
+      </c>
+      <c r="I63" t="inlineStr">
+        <is>
+          <t>Miami Marlins</t>
+        </is>
+      </c>
+      <c r="J63" t="inlineStr">
+        <is>
+          <t>mlb3year</t>
+        </is>
+      </c>
+      <c r="K63" t="n">
+        <v>-220</v>
+      </c>
+      <c r="L63" t="inlineStr">
+        <is>
+          <t>Barstool Sportsbook</t>
+        </is>
+      </c>
+      <c r="M63" t="n">
+        <v>206</v>
+      </c>
+      <c r="N63" t="inlineStr">
+        <is>
+          <t>BetOnline.ag</t>
+        </is>
+      </c>
+      <c r="O63" t="n">
+        <v>1</v>
+      </c>
+      <c r="P63" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q63" t="inlineStr">
+        <is>
+          <t>Peter Lambert</t>
+        </is>
+      </c>
+      <c r="R63" t="inlineStr">
+        <is>
+          <t>Braxton Garrett</t>
+        </is>
+      </c>
+      <c r="S63" t="n">
+        <v>0.003782067949911876</v>
+      </c>
+      <c r="T63" t="inlineStr">
+        <is>
+          <t>loanDepot park</t>
+        </is>
+      </c>
+      <c r="U63" t="inlineStr"/>
+      <c r="V63" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="W63" s="2" t="n">
+        <v>45128.41919939815</v>
+      </c>
+      <c r="X63" s="2" t="n">
+        <v>45128.41938325232</v>
+      </c>
+      <c r="Y63" t="inlineStr">
+        <is>
+          <t>2023-07-21T22:40:00Z</t>
+        </is>
+      </c>
+      <c r="Z63" t="n">
+        <v>717319</v>
+      </c>
+      <c r="AA63" t="inlineStr">
+        <is>
+          <t>2023-07-21 - Colorado Rockies (6) @ Miami Marlins (1) (Final)</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>1</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>2023-07-21</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>06:40 pm</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>Detroit Tigers</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>Reese Olson</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>San Diego Padres</t>
+        </is>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>Seth Lugo</t>
+        </is>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>San Diego Padres</t>
+        </is>
+      </c>
+      <c r="I64" t="inlineStr">
+        <is>
+          <t>San Diego Padres</t>
+        </is>
+      </c>
+      <c r="J64" t="inlineStr">
+        <is>
+          <t>mlb3year</t>
+        </is>
+      </c>
+      <c r="K64" t="n">
+        <v>128</v>
+      </c>
+      <c r="L64" t="inlineStr">
+        <is>
+          <t>WynnBET</t>
+        </is>
+      </c>
+      <c r="M64" t="n">
+        <v>-135</v>
+      </c>
+      <c r="N64" t="inlineStr">
+        <is>
+          <t>BetOnline.ag</t>
+        </is>
+      </c>
+      <c r="O64" t="n">
+        <v>4</v>
+      </c>
+      <c r="P64" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q64" t="inlineStr">
+        <is>
+          <t>Seth Lugo</t>
+        </is>
+      </c>
+      <c r="R64" t="inlineStr">
+        <is>
+          <t>Reese Olson</t>
+        </is>
+      </c>
+      <c r="S64" t="n">
+        <v>0.005051182798390572</v>
+      </c>
+      <c r="T64" t="inlineStr">
+        <is>
+          <t>Comerica Park</t>
+        </is>
+      </c>
+      <c r="U64" t="inlineStr"/>
+      <c r="V64" t="inlineStr">
+        <is>
+          <t>['Apple TV+']</t>
+        </is>
+      </c>
+      <c r="W64" s="2" t="n">
+        <v>45128.41919939815</v>
+      </c>
+      <c r="X64" s="2" t="n">
+        <v>45128.41944046296</v>
+      </c>
+      <c r="Y64" t="inlineStr">
+        <is>
+          <t>2023-07-21T22:40:00Z</t>
+        </is>
+      </c>
+      <c r="Z64" t="n">
+        <v>717317</v>
+      </c>
+      <c r="AA64" t="inlineStr">
+        <is>
+          <t>2023-07-21 - San Diego Padres (5) @ Detroit Tigers (4) (Final)</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>1</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>2023-07-21</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>07:05 pm</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>New York Yankees</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>Clarke Schmidt</t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>Kansas City Royals</t>
+        </is>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>Alec Marsh</t>
+        </is>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>New York Yankees</t>
+        </is>
+      </c>
+      <c r="I65" t="inlineStr">
+        <is>
+          <t>New York Yankees</t>
+        </is>
+      </c>
+      <c r="J65" t="inlineStr">
+        <is>
+          <t>mlb3year</t>
+        </is>
+      </c>
+      <c r="K65" t="n">
+        <v>-189</v>
+      </c>
+      <c r="L65" t="inlineStr">
+        <is>
+          <t>BetOnline.ag</t>
+        </is>
+      </c>
+      <c r="M65" t="n">
+        <v>182</v>
+      </c>
+      <c r="N65" t="inlineStr">
+        <is>
+          <t>WynnBET</t>
+        </is>
+      </c>
+      <c r="O65" t="n">
+        <v>5</v>
+      </c>
+      <c r="P65" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q65" t="inlineStr">
+        <is>
+          <t>Clarke Schmidt</t>
+        </is>
+      </c>
+      <c r="R65" t="inlineStr">
+        <is>
+          <t>Alec Marsh</t>
+        </is>
+      </c>
+      <c r="S65" t="n">
+        <v>0.5594420019458309</v>
+      </c>
+      <c r="T65" t="inlineStr">
+        <is>
+          <t>Yankee Stadium</t>
+        </is>
+      </c>
+      <c r="U65" t="inlineStr"/>
+      <c r="V65" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="W65" s="2" t="n">
+        <v>45128.41919939815</v>
+      </c>
+      <c r="X65" s="2" t="n">
+        <v>45128.41949083333</v>
+      </c>
+      <c r="Y65" t="inlineStr">
+        <is>
+          <t>2023-07-21T23:05:00Z</t>
+        </is>
+      </c>
+      <c r="Z65" t="n">
+        <v>717318</v>
+      </c>
+      <c r="AA65" t="inlineStr">
+        <is>
+          <t>2023-07-21 - Kansas City Royals (4) @ New York Yankees (5) (Final)</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>0</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>2023-07-21</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>07:05 pm</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>Washington Nationals</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>Jake Irvin</t>
+        </is>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>San Francisco Giants</t>
+        </is>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>Alex Wood</t>
+        </is>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>San Francisco Giants</t>
+        </is>
+      </c>
+      <c r="I66" t="inlineStr">
+        <is>
+          <t>San Francisco Giants</t>
+        </is>
+      </c>
+      <c r="J66" t="inlineStr">
+        <is>
+          <t>mlb3year</t>
+        </is>
+      </c>
+      <c r="K66" t="n">
+        <v>135</v>
+      </c>
+      <c r="L66" t="inlineStr">
+        <is>
+          <t>LowVig.ag</t>
+        </is>
+      </c>
+      <c r="M66" t="n">
+        <v>-147</v>
+      </c>
+      <c r="N66" t="inlineStr">
+        <is>
+          <t>BetUS</t>
+        </is>
+      </c>
+      <c r="O66" t="n">
+        <v>5</v>
+      </c>
+      <c r="P66" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q66" t="inlineStr">
+        <is>
+          <t>Jake Irvin</t>
+        </is>
+      </c>
+      <c r="R66" t="inlineStr">
+        <is>
+          <t>Alex Wood</t>
+        </is>
+      </c>
+      <c r="S66" t="n">
+        <v>0.4414610961198251</v>
+      </c>
+      <c r="T66" t="inlineStr">
+        <is>
+          <t>Nationals Park</t>
+        </is>
+      </c>
+      <c r="U66" t="inlineStr"/>
+      <c r="V66" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="W66" s="2" t="n">
+        <v>45128.41919939815</v>
+      </c>
+      <c r="X66" s="2" t="n">
+        <v>45128.41955920139</v>
+      </c>
+      <c r="Y66" t="inlineStr">
+        <is>
+          <t>2023-07-21T23:05:00Z</t>
+        </is>
+      </c>
+      <c r="Z66" t="n">
+        <v>717326</v>
+      </c>
+      <c r="AA66" t="inlineStr">
+        <is>
+          <t>2023-07-21 - San Francisco Giants (3) @ Washington Nationals (5) (Final)</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>0</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>2023-07-21</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>07:10 pm</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>Cincinnati Reds</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>Ben Lively</t>
+        </is>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>Arizona Diamondbacks</t>
+        </is>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>Tommy Henry</t>
+        </is>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>Arizona Diamondbacks</t>
+        </is>
+      </c>
+      <c r="I67" t="inlineStr">
+        <is>
+          <t>Cincinnati Reds</t>
+        </is>
+      </c>
+      <c r="J67" t="inlineStr">
+        <is>
+          <t>mlb3year</t>
+        </is>
+      </c>
+      <c r="K67" t="n">
+        <v>-115</v>
+      </c>
+      <c r="L67" t="inlineStr">
+        <is>
+          <t>DraftKings</t>
+        </is>
+      </c>
+      <c r="M67" t="n">
+        <v>109</v>
+      </c>
+      <c r="N67" t="inlineStr">
+        <is>
+          <t>LowVig.ag</t>
+        </is>
+      </c>
+      <c r="O67" t="n">
+        <v>9</v>
+      </c>
+      <c r="P67" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q67" t="inlineStr">
+        <is>
+          <t>Alex Young</t>
+        </is>
+      </c>
+      <c r="R67" t="inlineStr">
+        <is>
+          <t>Tommy Henry</t>
+        </is>
+      </c>
+      <c r="S67" t="n">
+        <v>0.0007879759361132147</v>
+      </c>
+      <c r="T67" t="inlineStr">
+        <is>
+          <t>Great American Ball Park</t>
+        </is>
+      </c>
+      <c r="U67" t="inlineStr"/>
+      <c r="V67" t="inlineStr">
+        <is>
+          <t>['MLBN (out-of-market only)', 'MLB.tv Free Game']</t>
+        </is>
+      </c>
+      <c r="W67" s="2" t="n">
+        <v>45128.41919939815</v>
+      </c>
+      <c r="X67" s="2" t="n">
+        <v>45128.41961300926</v>
+      </c>
+      <c r="Y67" t="inlineStr">
+        <is>
+          <t>2023-07-21T23:10:00Z</t>
+        </is>
+      </c>
+      <c r="Z67" t="n">
+        <v>717321</v>
+      </c>
+      <c r="AA67" t="inlineStr">
+        <is>
+          <t>2023-07-21 - Arizona Diamondbacks (6) @ Cincinnati Reds (9) (Final)</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr"/>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>2023-07-21</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>07:10 pm</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>Boston Red Sox</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>Kutter Crawford</t>
+        </is>
+      </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>New York Mets</t>
+        </is>
+      </c>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>Kodai Senga</t>
+        </is>
+      </c>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>New York Mets</t>
+        </is>
+      </c>
+      <c r="I68" t="inlineStr">
+        <is>
+          <t>Boston Red Sox</t>
+        </is>
+      </c>
+      <c r="J68" t="inlineStr">
+        <is>
+          <t>mlb3year</t>
+        </is>
+      </c>
+      <c r="K68" t="n">
+        <v>-112</v>
+      </c>
+      <c r="L68" t="inlineStr">
+        <is>
+          <t>WynnBET</t>
+        </is>
+      </c>
+      <c r="M68" t="n">
+        <v>109</v>
+      </c>
+      <c r="N68" t="inlineStr">
+        <is>
+          <t>BetUS</t>
+        </is>
+      </c>
+      <c r="O68" t="inlineStr"/>
+      <c r="P68" t="inlineStr"/>
+      <c r="Q68" t="inlineStr"/>
+      <c r="R68" t="inlineStr"/>
+      <c r="S68" t="n">
+        <v>0.02733988579617551</v>
+      </c>
+      <c r="T68" t="inlineStr">
+        <is>
+          <t>Fenway Park</t>
+        </is>
+      </c>
+      <c r="U68" t="inlineStr"/>
+      <c r="V68" t="inlineStr">
+        <is>
+          <t>['MLBN (out-of-market only)']</t>
+        </is>
+      </c>
+      <c r="W68" s="2" t="n">
+        <v>45128.41919939815</v>
+      </c>
+      <c r="X68" s="2" t="n">
+        <v>45128.41966820602</v>
+      </c>
+      <c r="Y68" t="inlineStr">
+        <is>
+          <t>2023-07-21T23:10:00Z</t>
+        </is>
+      </c>
+      <c r="Z68" t="n">
+        <v>717324</v>
+      </c>
+      <c r="AA68" t="inlineStr">
+        <is>
+          <t>2023-07-21 - New York Mets @ Boston Red Sox (Scheduled)</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>1</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>2023-07-21</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>07:10 pm</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>Cleveland Guardians</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>Gavin Williams</t>
+        </is>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>Philadelphia Phillies</t>
+        </is>
+      </c>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>Ranger Suarez</t>
+        </is>
+      </c>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>Cleveland Guardians</t>
+        </is>
+      </c>
+      <c r="I69" t="inlineStr">
+        <is>
+          <t>Philadelphia Phillies</t>
+        </is>
+      </c>
+      <c r="J69" t="inlineStr">
+        <is>
+          <t>mlb3year</t>
+        </is>
+      </c>
+      <c r="K69" t="n">
+        <v>109</v>
+      </c>
+      <c r="L69" t="inlineStr">
+        <is>
+          <t>LowVig.ag</t>
+        </is>
+      </c>
+      <c r="M69" t="n">
+        <v>-118</v>
+      </c>
+      <c r="N69" t="inlineStr">
+        <is>
+          <t>FanDuel</t>
+        </is>
+      </c>
+      <c r="O69" t="n">
+        <v>6</v>
+      </c>
+      <c r="P69" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q69" t="inlineStr">
+        <is>
+          <t>Trevor Stephan</t>
+        </is>
+      </c>
+      <c r="R69" t="inlineStr">
+        <is>
+          <t>Ranger Suarez</t>
+        </is>
+      </c>
+      <c r="S69" t="n">
+        <v>0.9784932878856787</v>
+      </c>
+      <c r="T69" t="inlineStr">
+        <is>
+          <t>Progressive Field</t>
+        </is>
+      </c>
+      <c r="U69" t="inlineStr"/>
+      <c r="V69" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="W69" s="2" t="n">
+        <v>45128.41919939815</v>
+      </c>
+      <c r="X69" s="2" t="n">
+        <v>45128.41972452546</v>
+      </c>
+      <c r="Y69" t="inlineStr">
+        <is>
+          <t>2023-07-21T23:10:00Z</t>
+        </is>
+      </c>
+      <c r="Z69" t="n">
+        <v>717315</v>
+      </c>
+      <c r="AA69" t="inlineStr">
+        <is>
+          <t>2023-07-21 - Philadelphia Phillies (5) @ Cleveland Guardians (6) (Final)</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr"/>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>2023-07-22</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>01:05 pm</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>New York Yankees</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>Gerrit Cole</t>
+        </is>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>Kansas City Royals</t>
+        </is>
+      </c>
+      <c r="G70" t="inlineStr">
+        <is>
+          <t>Brady Singer</t>
+        </is>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>New York Yankees</t>
+        </is>
+      </c>
+      <c r="I70" t="inlineStr">
+        <is>
+          <t>New York Yankees</t>
+        </is>
+      </c>
+      <c r="J70" t="inlineStr">
+        <is>
+          <t>mlb3year</t>
+        </is>
+      </c>
+      <c r="K70" t="inlineStr">
+        <is>
+          <t>-233</t>
+        </is>
+      </c>
+      <c r="L70" t="inlineStr">
+        <is>
+          <t>WynnBET</t>
+        </is>
+      </c>
+      <c r="M70" t="inlineStr">
+        <is>
+          <t>+212</t>
+        </is>
+      </c>
+      <c r="N70" t="inlineStr">
+        <is>
+          <t>LowVig.ag</t>
+        </is>
+      </c>
+      <c r="O70" t="inlineStr"/>
+      <c r="P70" t="inlineStr"/>
+      <c r="Q70" t="inlineStr"/>
+      <c r="R70" t="inlineStr"/>
+      <c r="S70" t="n">
+        <v>0.9172786768745543</v>
+      </c>
+      <c r="T70" t="inlineStr">
+        <is>
+          <t>Yankee Stadium</t>
+        </is>
+      </c>
+      <c r="U70" t="inlineStr"/>
+      <c r="V70" t="inlineStr">
+        <is>
+          <t>['MLBN (out-of-market only)']</t>
+        </is>
+      </c>
+      <c r="W70" s="2" t="n">
+        <v>45129.34648221559</v>
+      </c>
+      <c r="X70" s="2" t="n">
+        <v>45129.3465507333</v>
+      </c>
+      <c r="Y70" t="inlineStr">
+        <is>
+          <t>2023-07-22T17:05:00Z</t>
+        </is>
+      </c>
+      <c r="Z70" t="n">
+        <v>717304</v>
+      </c>
+      <c r="AA70" t="inlineStr">
+        <is>
+          <t>2023-07-22 - Kansas City Royals @ New York Yankees (Scheduled)</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr"/>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>2023-07-22</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>01:10 pm</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>Miami Marlins</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>Johnny Cueto</t>
+        </is>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>Colorado Rockies</t>
+        </is>
+      </c>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t>Chase Anderson</t>
+        </is>
+      </c>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>Colorado Rockies</t>
+        </is>
+      </c>
+      <c r="I71" t="inlineStr">
+        <is>
+          <t>Miami Marlins</t>
+        </is>
+      </c>
+      <c r="J71" t="inlineStr">
+        <is>
+          <t>mlb3year</t>
+        </is>
+      </c>
+      <c r="K71" t="inlineStr">
+        <is>
+          <t>-164</t>
+        </is>
+      </c>
+      <c r="L71" t="inlineStr">
+        <is>
+          <t>BetOnline.ag</t>
+        </is>
+      </c>
+      <c r="M71" t="inlineStr">
+        <is>
+          <t>+151</t>
+        </is>
+      </c>
+      <c r="N71" t="inlineStr">
+        <is>
+          <t>LowVig.ag</t>
+        </is>
+      </c>
+      <c r="O71" t="inlineStr"/>
+      <c r="P71" t="inlineStr"/>
+      <c r="Q71" t="inlineStr"/>
+      <c r="R71" t="inlineStr"/>
+      <c r="S71" t="n">
+        <v>0.03733136174875996</v>
+      </c>
+      <c r="T71" t="inlineStr">
+        <is>
+          <t>loanDepot park</t>
+        </is>
+      </c>
+      <c r="U71" t="inlineStr"/>
+      <c r="V71" t="inlineStr">
+        <is>
+          <t>['MLBN (out-of-market only)']</t>
+        </is>
+      </c>
+      <c r="W71" s="2" t="n">
+        <v>45129.34648221559</v>
+      </c>
+      <c r="X71" s="2" t="n">
+        <v>45129.34660605749</v>
+      </c>
+      <c r="Y71" t="inlineStr">
+        <is>
+          <t>2023-07-22T17:10:00Z</t>
+        </is>
+      </c>
+      <c r="Z71" t="n">
+        <v>717306</v>
+      </c>
+      <c r="AA71" t="inlineStr">
+        <is>
+          <t>2023-07-22 - Colorado Rockies @ Miami Marlins (Scheduled)</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr"/>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>2023-07-22</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>02:20 pm</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>Chicago Cubs</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>Michael Fulmer</t>
+        </is>
+      </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>St. Louis Cardinals</t>
+        </is>
+      </c>
+      <c r="G72" t="inlineStr">
+        <is>
+          <t>Miles Mikolas</t>
+        </is>
+      </c>
+      <c r="H72" t="inlineStr">
+        <is>
+          <t>St. Louis Cardinals</t>
+        </is>
+      </c>
+      <c r="I72" t="inlineStr">
+        <is>
+          <t>St. Louis Cardinals</t>
+        </is>
+      </c>
+      <c r="J72" t="inlineStr">
+        <is>
+          <t>mlb3year</t>
+        </is>
+      </c>
+      <c r="K72" t="inlineStr">
+        <is>
+          <t>+110</t>
+        </is>
+      </c>
+      <c r="L72" t="inlineStr">
+        <is>
+          <t>BetUS</t>
+        </is>
+      </c>
+      <c r="M72" t="inlineStr">
+        <is>
+          <t>-115</t>
+        </is>
+      </c>
+      <c r="N72" t="inlineStr">
+        <is>
+          <t>BetMGM</t>
+        </is>
+      </c>
+      <c r="O72" t="inlineStr"/>
+      <c r="P72" t="inlineStr"/>
+      <c r="Q72" t="inlineStr"/>
+      <c r="R72" t="inlineStr"/>
+      <c r="S72" t="n">
+        <v>0.1125441754735131</v>
+      </c>
+      <c r="T72" t="inlineStr">
+        <is>
+          <t>Wrigley Field</t>
+        </is>
+      </c>
+      <c r="U72" t="inlineStr">
+        <is>
+          <t>Series tied 1-1</t>
+        </is>
+      </c>
+      <c r="V72" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="W72" s="2" t="n">
+        <v>45129.34648221559</v>
+      </c>
+      <c r="X72" s="2" t="n">
+        <v>45129.34667830062</v>
+      </c>
+      <c r="Y72" t="inlineStr">
+        <is>
+          <t>2023-07-22T18:20:00Z</t>
+        </is>
+      </c>
+      <c r="Z72" t="n">
+        <v>717308</v>
+      </c>
+      <c r="AA72" t="inlineStr">
+        <is>
+          <t>2023-07-22 - St. Louis Cardinals @ Chicago Cubs (Scheduled)</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr"/>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>2023-07-22</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>04:05 pm</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>Texas Rangers</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>Dane Dunning</t>
+        </is>
+      </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>Los Angeles Dodgers</t>
+        </is>
+      </c>
+      <c r="G73" t="inlineStr">
+        <is>
+          <t>Bobby Miller</t>
+        </is>
+      </c>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t>Texas Rangers</t>
+        </is>
+      </c>
+      <c r="I73" t="inlineStr">
+        <is>
+          <t>Los Angeles Dodgers</t>
+        </is>
+      </c>
+      <c r="J73" t="inlineStr">
+        <is>
+          <t>mlb3year</t>
+        </is>
+      </c>
+      <c r="K73" t="inlineStr">
+        <is>
+          <t>+113</t>
+        </is>
+      </c>
+      <c r="L73" t="inlineStr">
+        <is>
+          <t>BetUS</t>
+        </is>
+      </c>
+      <c r="M73" t="inlineStr">
+        <is>
+          <t>-118</t>
+        </is>
+      </c>
+      <c r="N73" t="inlineStr">
+        <is>
+          <t>WynnBET</t>
+        </is>
+      </c>
+      <c r="O73" t="inlineStr"/>
+      <c r="P73" t="inlineStr"/>
+      <c r="Q73" t="inlineStr"/>
+      <c r="R73" t="inlineStr"/>
+      <c r="S73" t="n">
+        <v>0.7573945401129893</v>
+      </c>
+      <c r="T73" t="inlineStr">
+        <is>
+          <t>Globe Life Field</t>
+        </is>
+      </c>
+      <c r="U73" t="inlineStr"/>
+      <c r="V73" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="W73" s="2" t="n">
+        <v>45129.34648221559</v>
+      </c>
+      <c r="X73" s="2" t="n">
+        <v>45129.34673303444</v>
+      </c>
+      <c r="Y73" t="inlineStr">
+        <is>
+          <t>2023-07-22T20:05:00Z</t>
+        </is>
+      </c>
+      <c r="Z73" t="n">
+        <v>717305</v>
+      </c>
+      <c r="AA73" t="inlineStr">
+        <is>
+          <t>2023-07-22 - Los Angeles Dodgers @ Texas Rangers (Scheduled)</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr"/>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>2023-07-22</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>04:10 pm</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>Tampa Bay Rays</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>Shane McClanahan</t>
+        </is>
+      </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>Baltimore Orioles</t>
+        </is>
+      </c>
+      <c r="G74" t="inlineStr">
+        <is>
+          <t>Grayson Rodriguez</t>
+        </is>
+      </c>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t>Baltimore Orioles</t>
+        </is>
+      </c>
+      <c r="I74" t="inlineStr">
+        <is>
+          <t>Tampa Bay Rays</t>
+        </is>
+      </c>
+      <c r="J74" t="inlineStr">
+        <is>
+          <t>mlb3year</t>
+        </is>
+      </c>
+      <c r="K74" t="inlineStr">
+        <is>
+          <t>-175</t>
+        </is>
+      </c>
+      <c r="L74" t="inlineStr">
+        <is>
+          <t>WynnBET</t>
+        </is>
+      </c>
+      <c r="M74" t="inlineStr">
+        <is>
+          <t>+166</t>
+        </is>
+      </c>
+      <c r="N74" t="inlineStr">
+        <is>
+          <t>LowVig.ag</t>
+        </is>
+      </c>
+      <c r="O74" t="inlineStr"/>
+      <c r="P74" t="inlineStr"/>
+      <c r="Q74" t="inlineStr"/>
+      <c r="R74" t="inlineStr"/>
+      <c r="S74" t="n">
+        <v>0.01229636292900647</v>
+      </c>
+      <c r="T74" t="inlineStr">
+        <is>
+          <t>Tropicana Field</t>
+        </is>
+      </c>
+      <c r="U74" t="inlineStr"/>
+      <c r="V74" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="W74" s="2" t="n">
+        <v>45129.34648221559</v>
+      </c>
+      <c r="X74" s="2" t="n">
+        <v>45129.34678912203</v>
+      </c>
+      <c r="Y74" t="inlineStr">
+        <is>
+          <t>2023-07-22T20:10:00Z</t>
+        </is>
+      </c>
+      <c r="Z74" t="n">
+        <v>717300</v>
+      </c>
+      <c r="AA74" t="inlineStr">
+        <is>
+          <t>2023-07-22 - Baltimore Orioles @ Tampa Bay Rays (Scheduled)</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr"/>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>2023-07-22</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>04:10 pm</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>Seattle Mariners</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>Logan Gilbert</t>
+        </is>
+      </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>Toronto Blue Jays</t>
+        </is>
+      </c>
+      <c r="G75" t="inlineStr">
+        <is>
+          <t>Kevin Gausman</t>
+        </is>
+      </c>
+      <c r="H75" t="inlineStr">
+        <is>
+          <t>Seattle Mariners</t>
+        </is>
+      </c>
+      <c r="I75" t="inlineStr">
+        <is>
+          <t>Toronto Blue Jays</t>
+        </is>
+      </c>
+      <c r="J75" t="inlineStr">
+        <is>
+          <t>mlb3year</t>
+        </is>
+      </c>
+      <c r="K75" t="inlineStr">
+        <is>
+          <t>+125</t>
+        </is>
+      </c>
+      <c r="L75" t="inlineStr">
+        <is>
+          <t>BetUS</t>
+        </is>
+      </c>
+      <c r="M75" t="inlineStr">
+        <is>
+          <t>-133</t>
+        </is>
+      </c>
+      <c r="N75" t="inlineStr">
+        <is>
+          <t>BetOnline.ag</t>
+        </is>
+      </c>
+      <c r="O75" t="inlineStr"/>
+      <c r="P75" t="inlineStr"/>
+      <c r="Q75" t="inlineStr"/>
+      <c r="R75" t="inlineStr"/>
+      <c r="S75" t="n">
+        <v>0.8520667952673416</v>
+      </c>
+      <c r="T75" t="inlineStr">
+        <is>
+          <t>T-Mobile Park</t>
+        </is>
+      </c>
+      <c r="U75" t="inlineStr"/>
+      <c r="V75" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="W75" s="2" t="n">
+        <v>45129.34648221559</v>
+      </c>
+      <c r="X75" s="2" t="n">
+        <v>45129.34685949393</v>
+      </c>
+      <c r="Y75" t="inlineStr">
+        <is>
+          <t>2023-07-22T20:10:00Z</t>
+        </is>
+      </c>
+      <c r="Z75" t="n">
+        <v>717301</v>
+      </c>
+      <c r="AA75" t="inlineStr">
+        <is>
+          <t>2023-07-22 - Toronto Blue Jays @ Seattle Mariners (Scheduled)</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr"/>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>2023-07-22</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>06:10 pm</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>Detroit Tigers</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>Matt Manning</t>
+        </is>
+      </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>San Diego Padres</t>
+        </is>
+      </c>
+      <c r="G76" t="inlineStr"/>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>San Diego Padres</t>
+        </is>
+      </c>
+      <c r="I76" t="inlineStr">
+        <is>
+          <t>San Diego Padres</t>
+        </is>
+      </c>
+      <c r="J76" t="inlineStr">
+        <is>
+          <t>mlb3year</t>
+        </is>
+      </c>
+      <c r="K76" t="inlineStr">
+        <is>
+          <t>+125</t>
+        </is>
+      </c>
+      <c r="L76" t="inlineStr">
+        <is>
+          <t>BetUS</t>
+        </is>
+      </c>
+      <c r="M76" t="inlineStr">
+        <is>
+          <t>-130</t>
+        </is>
+      </c>
+      <c r="N76" t="inlineStr">
+        <is>
+          <t>LowVig.ag</t>
+        </is>
+      </c>
+      <c r="O76" t="inlineStr"/>
+      <c r="P76" t="inlineStr"/>
+      <c r="Q76" t="inlineStr"/>
+      <c r="R76" t="inlineStr"/>
+      <c r="S76" t="n">
+        <v>0.3239182628947005</v>
+      </c>
+      <c r="T76" t="inlineStr">
+        <is>
+          <t>Comerica Park</t>
+        </is>
+      </c>
+      <c r="U76" t="inlineStr"/>
+      <c r="V76" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="W76" s="2" t="n">
+        <v>45129.34648221559</v>
+      </c>
+      <c r="X76" s="2" t="n">
+        <v>45129.34691105314</v>
+      </c>
+      <c r="Y76" t="inlineStr">
+        <is>
+          <t>2023-07-22T22:10:00Z</t>
+        </is>
+      </c>
+      <c r="Z76" t="n">
+        <v>717299</v>
+      </c>
+      <c r="AA76" t="inlineStr">
+        <is>
+          <t>2023-07-22 - San Diego Padres @ Detroit Tigers (Scheduled)</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr"/>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>2023-07-22</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>07:05 pm</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>Washington Nationals</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>Josiah Gray</t>
+        </is>
+      </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>San Francisco Giants</t>
+        </is>
+      </c>
+      <c r="G77" t="inlineStr">
+        <is>
+          <t>Logan Webb</t>
+        </is>
+      </c>
+      <c r="H77" t="inlineStr">
+        <is>
+          <t>San Francisco Giants</t>
+        </is>
+      </c>
+      <c r="I77" t="inlineStr">
+        <is>
+          <t>San Francisco Giants</t>
+        </is>
+      </c>
+      <c r="J77" t="inlineStr">
+        <is>
+          <t>mlb3year</t>
+        </is>
+      </c>
+      <c r="K77" t="inlineStr">
+        <is>
+          <t>+168</t>
+        </is>
+      </c>
+      <c r="L77" t="inlineStr">
+        <is>
+          <t>WynnBET</t>
+        </is>
+      </c>
+      <c r="M77" t="inlineStr">
+        <is>
+          <t>-180</t>
+        </is>
+      </c>
+      <c r="N77" t="inlineStr">
+        <is>
+          <t>DraftKings</t>
+        </is>
+      </c>
+      <c r="O77" t="inlineStr"/>
+      <c r="P77" t="inlineStr"/>
+      <c r="Q77" t="inlineStr"/>
+      <c r="R77" t="inlineStr"/>
+      <c r="S77" t="n">
+        <v>0.4374312792395386</v>
+      </c>
+      <c r="T77" t="inlineStr">
+        <is>
+          <t>Nationals Park</t>
+        </is>
+      </c>
+      <c r="U77" t="inlineStr"/>
+      <c r="V77" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="W77" s="2" t="n">
+        <v>45129.34648221559</v>
+      </c>
+      <c r="X77" s="2" t="n">
+        <v>45129.34697167146</v>
+      </c>
+      <c r="Y77" t="inlineStr">
+        <is>
+          <t>2023-07-22T23:05:00Z</t>
+        </is>
+      </c>
+      <c r="Z77" t="n">
+        <v>717307</v>
+      </c>
+      <c r="AA77" t="inlineStr">
+        <is>
+          <t>2023-07-22 - San Francisco Giants @ Washington Nationals (Scheduled)</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr"/>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>2023-07-22</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>07:10 pm</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>Boston Red Sox</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>James Paxton</t>
+        </is>
+      </c>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>New York Mets</t>
+        </is>
+      </c>
+      <c r="G78" t="inlineStr">
+        <is>
+          <t>Max Scherzer</t>
+        </is>
+      </c>
+      <c r="H78" t="inlineStr">
+        <is>
+          <t>New York Mets</t>
+        </is>
+      </c>
+      <c r="I78" t="inlineStr">
+        <is>
+          <t>Boston Red Sox</t>
+        </is>
+      </c>
+      <c r="J78" t="inlineStr">
+        <is>
+          <t>mlb3year</t>
+        </is>
+      </c>
+      <c r="K78" t="inlineStr">
+        <is>
+          <t>-115</t>
+        </is>
+      </c>
+      <c r="L78" t="inlineStr">
+        <is>
+          <t>BetUS</t>
+        </is>
+      </c>
+      <c r="M78" t="inlineStr">
+        <is>
+          <t>+110</t>
+        </is>
+      </c>
+      <c r="N78" t="inlineStr">
+        <is>
+          <t>BetRivers</t>
+        </is>
+      </c>
+      <c r="O78" t="inlineStr"/>
+      <c r="P78" t="inlineStr"/>
+      <c r="Q78" t="inlineStr"/>
+      <c r="R78" t="inlineStr"/>
+      <c r="S78" t="n">
+        <v>0.01136361134537548</v>
+      </c>
+      <c r="T78" t="inlineStr">
+        <is>
+          <t>Fenway Park</t>
+        </is>
+      </c>
+      <c r="U78" t="inlineStr"/>
+      <c r="V78" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="W78" s="2" t="n">
+        <v>45129.34648221559</v>
+      </c>
+      <c r="X78" s="2" t="n">
+        <v>45129.34704088674</v>
+      </c>
+      <c r="Y78" t="inlineStr">
+        <is>
+          <t>2023-07-22T23:10:00Z</t>
+        </is>
+      </c>
+      <c r="Z78" t="n">
+        <v>717309</v>
+      </c>
+      <c r="AA78" t="inlineStr">
+        <is>
+          <t>2023-07-22 - New York Mets @ Boston Red Sox (Scheduled)</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr"/>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>2023-07-22</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>07:10 pm</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>Cleveland Guardians</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>Tanner Bibee</t>
+        </is>
+      </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>Philadelphia Phillies</t>
+        </is>
+      </c>
+      <c r="G79" t="inlineStr">
+        <is>
+          <t>Zack Wheeler</t>
+        </is>
+      </c>
+      <c r="H79" t="inlineStr">
+        <is>
+          <t>Philadelphia Phillies</t>
+        </is>
+      </c>
+      <c r="I79" t="inlineStr">
+        <is>
+          <t>Philadelphia Phillies</t>
+        </is>
+      </c>
+      <c r="J79" t="inlineStr">
+        <is>
+          <t>mlb3year</t>
+        </is>
+      </c>
+      <c r="K79" t="inlineStr">
+        <is>
+          <t>+110</t>
+        </is>
+      </c>
+      <c r="L79" t="inlineStr">
+        <is>
+          <t>WynnBET</t>
+        </is>
+      </c>
+      <c r="M79" t="inlineStr">
+        <is>
+          <t>-118</t>
+        </is>
+      </c>
+      <c r="N79" t="inlineStr">
+        <is>
+          <t>LowVig.ag</t>
+        </is>
+      </c>
+      <c r="O79" t="inlineStr"/>
+      <c r="P79" t="inlineStr"/>
+      <c r="Q79" t="inlineStr"/>
+      <c r="R79" t="inlineStr"/>
+      <c r="S79" t="n">
+        <v>0.3800097137373824</v>
+      </c>
+      <c r="T79" t="inlineStr">
+        <is>
+          <t>Progressive Field</t>
+        </is>
+      </c>
+      <c r="U79" t="inlineStr"/>
+      <c r="V79" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="W79" s="2" t="n">
+        <v>45129.34648221559</v>
+      </c>
+      <c r="X79" s="2" t="n">
+        <v>45129.34709737662</v>
+      </c>
+      <c r="Y79" t="inlineStr">
+        <is>
+          <t>2023-07-22T23:10:00Z</t>
+        </is>
+      </c>
+      <c r="Z79" t="n">
+        <v>717302</v>
+      </c>
+      <c r="AA79" t="inlineStr">
+        <is>
+          <t>2023-07-22 - Philadelphia Phillies @ Cleveland Guardians (Scheduled)</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr"/>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>2023-07-22</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>07:15 pm</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>Milwaukee Brewers</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>Adrian Houser</t>
+        </is>
+      </c>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>Atlanta Braves</t>
+        </is>
+      </c>
+      <c r="G80" t="inlineStr">
+        <is>
+          <t>Allan Winans</t>
+        </is>
+      </c>
+      <c r="H80" t="inlineStr">
+        <is>
+          <t>Atlanta Braves</t>
+        </is>
+      </c>
+      <c r="I80" t="inlineStr">
+        <is>
+          <t>Atlanta Braves</t>
+        </is>
+      </c>
+      <c r="J80" t="inlineStr">
+        <is>
+          <t>mlb3year</t>
+        </is>
+      </c>
+      <c r="K80" t="inlineStr">
+        <is>
+          <t>+123</t>
+        </is>
+      </c>
+      <c r="L80" t="inlineStr">
+        <is>
+          <t>BetUS</t>
+        </is>
+      </c>
+      <c r="M80" t="inlineStr">
+        <is>
+          <t>-133</t>
+        </is>
+      </c>
+      <c r="N80" t="inlineStr">
+        <is>
+          <t>BetOnline.ag</t>
+        </is>
+      </c>
+      <c r="O80" t="inlineStr"/>
+      <c r="P80" t="inlineStr"/>
+      <c r="Q80" t="inlineStr"/>
+      <c r="R80" t="inlineStr"/>
+      <c r="S80" t="n">
+        <v>0.008889384686767825</v>
+      </c>
+      <c r="T80" t="inlineStr">
+        <is>
+          <t>American Family Field</t>
+        </is>
+      </c>
+      <c r="U80" t="inlineStr">
+        <is>
+          <t>ATL leads 1-0</t>
+        </is>
+      </c>
+      <c r="V80" t="inlineStr">
+        <is>
+          <t>['FOX']</t>
+        </is>
+      </c>
+      <c r="W80" s="2" t="n">
+        <v>45129.34648221559</v>
+      </c>
+      <c r="X80" s="2" t="n">
+        <v>45129.34714766181</v>
+      </c>
+      <c r="Y80" t="inlineStr">
+        <is>
+          <t>2023-07-22T23:15:00Z</t>
+        </is>
+      </c>
+      <c r="Z80" t="n">
+        <v>717296</v>
+      </c>
+      <c r="AA80" t="inlineStr">
+        <is>
+          <t>2023-07-22 - Atlanta Braves @ Milwaukee Brewers (Scheduled)</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr"/>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>2023-07-22</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>07:15 pm</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>Minnesota Twins</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>Sonny Gray</t>
+        </is>
+      </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>Chicago White Sox</t>
+        </is>
+      </c>
+      <c r="G81" t="inlineStr">
+        <is>
+          <t>Dylan Cease</t>
+        </is>
+      </c>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>Chicago White Sox</t>
+        </is>
+      </c>
+      <c r="I81" t="inlineStr">
+        <is>
+          <t>Minnesota Twins</t>
+        </is>
+      </c>
+      <c r="J81" t="inlineStr">
+        <is>
+          <t>mlb3year</t>
+        </is>
+      </c>
+      <c r="K81" t="inlineStr">
+        <is>
+          <t>-133</t>
+        </is>
+      </c>
+      <c r="L81" t="inlineStr">
+        <is>
+          <t>WynnBET</t>
+        </is>
+      </c>
+      <c r="M81" t="inlineStr">
+        <is>
+          <t>+125</t>
+        </is>
+      </c>
+      <c r="N81" t="inlineStr">
+        <is>
+          <t>BetUS</t>
+        </is>
+      </c>
+      <c r="O81" t="inlineStr"/>
+      <c r="P81" t="inlineStr"/>
+      <c r="Q81" t="inlineStr"/>
+      <c r="R81" t="inlineStr"/>
+      <c r="S81" t="n">
+        <v>0.002727569814304598</v>
+      </c>
+      <c r="T81" t="inlineStr">
+        <is>
+          <t>Target Field</t>
+        </is>
+      </c>
+      <c r="U81" t="inlineStr"/>
+      <c r="V81" t="inlineStr">
+        <is>
+          <t>['FOX']</t>
+        </is>
+      </c>
+      <c r="W81" s="2" t="n">
+        <v>45129.34648221559</v>
+      </c>
+      <c r="X81" s="2" t="n">
+        <v>45129.34721555199</v>
+      </c>
+      <c r="Y81" t="inlineStr">
+        <is>
+          <t>2023-07-22T23:15:00Z</t>
+        </is>
+      </c>
+      <c r="Z81" t="n">
+        <v>717293</v>
+      </c>
+      <c r="AA81" t="inlineStr">
+        <is>
+          <t>2023-07-22 - Chicago White Sox @ Minnesota Twins (Scheduled)</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr"/>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>2023-07-22</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>09:07 pm</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>Oakland Athletics</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>Paul Blackburn</t>
+        </is>
+      </c>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>Houston Astros</t>
+        </is>
+      </c>
+      <c r="G82" t="inlineStr">
+        <is>
+          <t>Cristian Javier</t>
+        </is>
+      </c>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t>Oakland Athletics</t>
+        </is>
+      </c>
+      <c r="I82" t="inlineStr">
+        <is>
+          <t>Houston Astros</t>
+        </is>
+      </c>
+      <c r="J82" t="inlineStr">
+        <is>
+          <t>mlb3year</t>
+        </is>
+      </c>
+      <c r="K82" t="inlineStr">
+        <is>
+          <t>+176</t>
+        </is>
+      </c>
+      <c r="L82" t="inlineStr">
+        <is>
+          <t>LowVig.ag</t>
+        </is>
+      </c>
+      <c r="M82" t="inlineStr">
+        <is>
+          <t>-189</t>
+        </is>
+      </c>
+      <c r="N82" t="inlineStr">
+        <is>
+          <t>WynnBET</t>
+        </is>
+      </c>
+      <c r="O82" t="inlineStr"/>
+      <c r="P82" t="inlineStr"/>
+      <c r="Q82" t="inlineStr"/>
+      <c r="R82" t="inlineStr"/>
+      <c r="S82" t="n">
+        <v>0.9994406981813074</v>
+      </c>
+      <c r="T82" t="inlineStr">
+        <is>
+          <t>Oakland Coliseum</t>
+        </is>
+      </c>
+      <c r="U82" t="inlineStr"/>
+      <c r="V82" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="W82" s="2" t="n">
+        <v>45129.34648221559</v>
+      </c>
+      <c r="X82" s="2" t="n">
+        <v>45129.34727540473</v>
+      </c>
+      <c r="Y82" t="inlineStr">
+        <is>
+          <t>2023-07-23T01:07:00Z</t>
+        </is>
+      </c>
+      <c r="Z82" t="n">
+        <v>717295</v>
+      </c>
+      <c r="AA82" t="inlineStr">
+        <is>
+          <t>2023-07-22 - Houston Astros @ Oakland Athletics (Scheduled)</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr"/>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>2023-07-22</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>09:07 pm</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>Los Angeles Angels</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>Reid Detmers</t>
+        </is>
+      </c>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>Pittsburgh Pirates</t>
+        </is>
+      </c>
+      <c r="G83" t="inlineStr">
+        <is>
+          <t>Ryan Borucki</t>
+        </is>
+      </c>
+      <c r="H83" t="inlineStr">
+        <is>
+          <t>Pittsburgh Pirates</t>
+        </is>
+      </c>
+      <c r="I83" t="inlineStr">
+        <is>
+          <t>Los Angeles Angels</t>
+        </is>
+      </c>
+      <c r="J83" t="inlineStr">
+        <is>
+          <t>mlb3year</t>
+        </is>
+      </c>
+      <c r="K83" t="inlineStr">
+        <is>
+          <t>-178</t>
+        </is>
+      </c>
+      <c r="L83" t="inlineStr">
+        <is>
+          <t>LowVig.ag</t>
+        </is>
+      </c>
+      <c r="M83" t="inlineStr">
+        <is>
+          <t>+171</t>
+        </is>
+      </c>
+      <c r="N83" t="inlineStr">
+        <is>
+          <t>WynnBET</t>
+        </is>
+      </c>
+      <c r="O83" t="inlineStr"/>
+      <c r="P83" t="inlineStr"/>
+      <c r="Q83" t="inlineStr"/>
+      <c r="R83" t="inlineStr"/>
+      <c r="S83" t="n">
+        <v>0.001427805428936317</v>
+      </c>
+      <c r="T83" t="inlineStr">
+        <is>
+          <t>Angel Stadium</t>
+        </is>
+      </c>
+      <c r="U83" t="inlineStr">
+        <is>
+          <t>LAA leads 1-0</t>
+        </is>
+      </c>
+      <c r="V83" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="W83" s="2" t="n">
+        <v>45129.34648221559</v>
+      </c>
+      <c r="X83" s="2" t="n">
+        <v>45129.34732858533</v>
+      </c>
+      <c r="Y83" t="inlineStr">
+        <is>
+          <t>2023-07-23T01:07:00Z</t>
+        </is>
+      </c>
+      <c r="Z83" t="n">
+        <v>717297</v>
+      </c>
+      <c r="AA83" t="inlineStr">
+        <is>
+          <t>2023-07-22 - Pittsburgh Pirates @ Los Angeles Angels (Scheduled)</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
predictions for 07/23/2023 (53% yesterday)
</commit_message>
<xml_diff>
--- a/data/predictions.xlsx
+++ b/data/predictions.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA83"/>
+  <dimension ref="A1:AA96"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8241,7 +8241,9 @@
       </c>
     </row>
     <row r="68">
-      <c r="A68" t="inlineStr"/>
+      <c r="A68" t="n">
+        <v>1</v>
+      </c>
       <c r="B68" t="inlineStr">
         <is>
           <t>2023-07-21</t>
@@ -8303,10 +8305,22 @@
           <t>BetUS</t>
         </is>
       </c>
-      <c r="O68" t="inlineStr"/>
-      <c r="P68" t="inlineStr"/>
-      <c r="Q68" t="inlineStr"/>
-      <c r="R68" t="inlineStr"/>
+      <c r="O68" t="n">
+        <v>4</v>
+      </c>
+      <c r="P68" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q68" t="inlineStr">
+        <is>
+          <t>Grant Hartwig</t>
+        </is>
+      </c>
+      <c r="R68" t="inlineStr">
+        <is>
+          <t>Kutter Crawford</t>
+        </is>
+      </c>
       <c r="S68" t="n">
         <v>0.02733988579617551</v>
       </c>
@@ -8337,7 +8351,7 @@
       </c>
       <c r="AA68" t="inlineStr">
         <is>
-          <t>2023-07-21 - New York Mets @ Boston Red Sox (Scheduled)</t>
+          <t>2023-07-21 - New York Mets (5) @ Boston Red Sox (4) (Final)</t>
         </is>
       </c>
     </row>
@@ -8457,7 +8471,9 @@
       </c>
     </row>
     <row r="70">
-      <c r="A70" t="inlineStr"/>
+      <c r="A70" t="n">
+        <v>1</v>
+      </c>
       <c r="B70" t="inlineStr">
         <is>
           <t>2023-07-22</t>
@@ -8503,30 +8519,38 @@
           <t>mlb3year</t>
         </is>
       </c>
-      <c r="K70" t="inlineStr">
-        <is>
-          <t>-233</t>
-        </is>
+      <c r="K70" t="n">
+        <v>-233</v>
       </c>
       <c r="L70" t="inlineStr">
         <is>
           <t>WynnBET</t>
         </is>
       </c>
-      <c r="M70" t="inlineStr">
-        <is>
-          <t>+212</t>
-        </is>
+      <c r="M70" t="n">
+        <v>212</v>
       </c>
       <c r="N70" t="inlineStr">
         <is>
           <t>LowVig.ag</t>
         </is>
       </c>
-      <c r="O70" t="inlineStr"/>
-      <c r="P70" t="inlineStr"/>
-      <c r="Q70" t="inlineStr"/>
-      <c r="R70" t="inlineStr"/>
+      <c r="O70" t="n">
+        <v>5</v>
+      </c>
+      <c r="P70" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q70" t="inlineStr">
+        <is>
+          <t>Wandy Peralta</t>
+        </is>
+      </c>
+      <c r="R70" t="inlineStr">
+        <is>
+          <t>Carlos Hernandez</t>
+        </is>
+      </c>
       <c r="S70" t="n">
         <v>0.9172786768745543</v>
       </c>
@@ -8542,10 +8566,10 @@
         </is>
       </c>
       <c r="W70" s="2" t="n">
-        <v>45129.34648221559</v>
+        <v>45129.34648221065</v>
       </c>
       <c r="X70" s="2" t="n">
-        <v>45129.3465507333</v>
+        <v>45129.34655072917</v>
       </c>
       <c r="Y70" t="inlineStr">
         <is>
@@ -8557,12 +8581,14 @@
       </c>
       <c r="AA70" t="inlineStr">
         <is>
-          <t>2023-07-22 - Kansas City Royals @ New York Yankees (Scheduled)</t>
+          <t>2023-07-22 - Kansas City Royals (2) @ New York Yankees (5) (Final)</t>
         </is>
       </c>
     </row>
     <row r="71">
-      <c r="A71" t="inlineStr"/>
+      <c r="A71" t="n">
+        <v>1</v>
+      </c>
       <c r="B71" t="inlineStr">
         <is>
           <t>2023-07-22</t>
@@ -8608,30 +8634,38 @@
           <t>mlb3year</t>
         </is>
       </c>
-      <c r="K71" t="inlineStr">
-        <is>
-          <t>-164</t>
-        </is>
+      <c r="K71" t="n">
+        <v>-164</v>
       </c>
       <c r="L71" t="inlineStr">
         <is>
           <t>BetOnline.ag</t>
         </is>
       </c>
-      <c r="M71" t="inlineStr">
-        <is>
-          <t>+151</t>
-        </is>
+      <c r="M71" t="n">
+        <v>151</v>
       </c>
       <c r="N71" t="inlineStr">
         <is>
           <t>LowVig.ag</t>
         </is>
       </c>
-      <c r="O71" t="inlineStr"/>
-      <c r="P71" t="inlineStr"/>
-      <c r="Q71" t="inlineStr"/>
-      <c r="R71" t="inlineStr"/>
+      <c r="O71" t="n">
+        <v>3</v>
+      </c>
+      <c r="P71" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q71" t="inlineStr">
+        <is>
+          <t>Daniel Bard</t>
+        </is>
+      </c>
+      <c r="R71" t="inlineStr">
+        <is>
+          <t>Tanner Scott</t>
+        </is>
+      </c>
       <c r="S71" t="n">
         <v>0.03733136174875996</v>
       </c>
@@ -8647,10 +8681,10 @@
         </is>
       </c>
       <c r="W71" s="2" t="n">
-        <v>45129.34648221559</v>
+        <v>45129.34648221065</v>
       </c>
       <c r="X71" s="2" t="n">
-        <v>45129.34660605749</v>
+        <v>45129.34660605324</v>
       </c>
       <c r="Y71" t="inlineStr">
         <is>
@@ -8662,12 +8696,14 @@
       </c>
       <c r="AA71" t="inlineStr">
         <is>
-          <t>2023-07-22 - Colorado Rockies @ Miami Marlins (Scheduled)</t>
+          <t>2023-07-22 - Colorado Rockies (4) @ Miami Marlins (3) (Final)</t>
         </is>
       </c>
     </row>
     <row r="72">
-      <c r="A72" t="inlineStr"/>
+      <c r="A72" t="n">
+        <v>0</v>
+      </c>
       <c r="B72" t="inlineStr">
         <is>
           <t>2023-07-22</t>
@@ -8713,30 +8749,38 @@
           <t>mlb3year</t>
         </is>
       </c>
-      <c r="K72" t="inlineStr">
-        <is>
-          <t>+110</t>
-        </is>
+      <c r="K72" t="n">
+        <v>110</v>
       </c>
       <c r="L72" t="inlineStr">
         <is>
           <t>BetUS</t>
         </is>
       </c>
-      <c r="M72" t="inlineStr">
-        <is>
-          <t>-115</t>
-        </is>
+      <c r="M72" t="n">
+        <v>-115</v>
       </c>
       <c r="N72" t="inlineStr">
         <is>
           <t>BetMGM</t>
         </is>
       </c>
-      <c r="O72" t="inlineStr"/>
-      <c r="P72" t="inlineStr"/>
-      <c r="Q72" t="inlineStr"/>
-      <c r="R72" t="inlineStr"/>
+      <c r="O72" t="n">
+        <v>8</v>
+      </c>
+      <c r="P72" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q72" t="inlineStr">
+        <is>
+          <t>Daniel Palencia</t>
+        </is>
+      </c>
+      <c r="R72" t="inlineStr">
+        <is>
+          <t>Zack Thompson</t>
+        </is>
+      </c>
       <c r="S72" t="n">
         <v>0.1125441754735131</v>
       </c>
@@ -8756,10 +8800,10 @@
         </is>
       </c>
       <c r="W72" s="2" t="n">
-        <v>45129.34648221559</v>
+        <v>45129.34648221065</v>
       </c>
       <c r="X72" s="2" t="n">
-        <v>45129.34667830062</v>
+        <v>45129.34667829861</v>
       </c>
       <c r="Y72" t="inlineStr">
         <is>
@@ -8771,12 +8815,14 @@
       </c>
       <c r="AA72" t="inlineStr">
         <is>
-          <t>2023-07-22 - St. Louis Cardinals @ Chicago Cubs (Scheduled)</t>
+          <t>2023-07-22 - St. Louis Cardinals (6) @ Chicago Cubs (8) (Final)</t>
         </is>
       </c>
     </row>
     <row r="73">
-      <c r="A73" t="inlineStr"/>
+      <c r="A73" t="n">
+        <v>0</v>
+      </c>
       <c r="B73" t="inlineStr">
         <is>
           <t>2023-07-22</t>
@@ -8822,30 +8868,38 @@
           <t>mlb3year</t>
         </is>
       </c>
-      <c r="K73" t="inlineStr">
-        <is>
-          <t>+113</t>
-        </is>
+      <c r="K73" t="n">
+        <v>113</v>
       </c>
       <c r="L73" t="inlineStr">
         <is>
           <t>BetUS</t>
         </is>
       </c>
-      <c r="M73" t="inlineStr">
-        <is>
-          <t>-118</t>
-        </is>
+      <c r="M73" t="n">
+        <v>-118</v>
       </c>
       <c r="N73" t="inlineStr">
         <is>
           <t>WynnBET</t>
         </is>
       </c>
-      <c r="O73" t="inlineStr"/>
-      <c r="P73" t="inlineStr"/>
-      <c r="Q73" t="inlineStr"/>
-      <c r="R73" t="inlineStr"/>
+      <c r="O73" t="n">
+        <v>3</v>
+      </c>
+      <c r="P73" t="n">
+        <v>16</v>
+      </c>
+      <c r="Q73" t="inlineStr">
+        <is>
+          <t>Bobby Miller</t>
+        </is>
+      </c>
+      <c r="R73" t="inlineStr">
+        <is>
+          <t>Dane Dunning</t>
+        </is>
+      </c>
       <c r="S73" t="n">
         <v>0.7573945401129893</v>
       </c>
@@ -8861,10 +8915,10 @@
         </is>
       </c>
       <c r="W73" s="2" t="n">
-        <v>45129.34648221559</v>
+        <v>45129.34648221065</v>
       </c>
       <c r="X73" s="2" t="n">
-        <v>45129.34673303444</v>
+        <v>45129.34673303241</v>
       </c>
       <c r="Y73" t="inlineStr">
         <is>
@@ -8876,12 +8930,14 @@
       </c>
       <c r="AA73" t="inlineStr">
         <is>
-          <t>2023-07-22 - Los Angeles Dodgers @ Texas Rangers (Scheduled)</t>
+          <t>2023-07-22 - Los Angeles Dodgers (16) @ Texas Rangers (3) (Final)</t>
         </is>
       </c>
     </row>
     <row r="74">
-      <c r="A74" t="inlineStr"/>
+      <c r="A74" t="n">
+        <v>1</v>
+      </c>
       <c r="B74" t="inlineStr">
         <is>
           <t>2023-07-22</t>
@@ -8927,30 +8983,38 @@
           <t>mlb3year</t>
         </is>
       </c>
-      <c r="K74" t="inlineStr">
-        <is>
-          <t>-175</t>
-        </is>
+      <c r="K74" t="n">
+        <v>-175</v>
       </c>
       <c r="L74" t="inlineStr">
         <is>
           <t>WynnBET</t>
         </is>
       </c>
-      <c r="M74" t="inlineStr">
-        <is>
-          <t>+166</t>
-        </is>
+      <c r="M74" t="n">
+        <v>166</v>
       </c>
       <c r="N74" t="inlineStr">
         <is>
           <t>LowVig.ag</t>
         </is>
       </c>
-      <c r="O74" t="inlineStr"/>
-      <c r="P74" t="inlineStr"/>
-      <c r="Q74" t="inlineStr"/>
-      <c r="R74" t="inlineStr"/>
+      <c r="O74" t="n">
+        <v>5</v>
+      </c>
+      <c r="P74" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q74" t="inlineStr">
+        <is>
+          <t>Cionel Perez</t>
+        </is>
+      </c>
+      <c r="R74" t="inlineStr">
+        <is>
+          <t>Pete Fairbanks</t>
+        </is>
+      </c>
       <c r="S74" t="n">
         <v>0.01229636292900647</v>
       </c>
@@ -8966,10 +9030,10 @@
         </is>
       </c>
       <c r="W74" s="2" t="n">
-        <v>45129.34648221559</v>
+        <v>45129.34648221065</v>
       </c>
       <c r="X74" s="2" t="n">
-        <v>45129.34678912203</v>
+        <v>45129.34678912037</v>
       </c>
       <c r="Y74" t="inlineStr">
         <is>
@@ -8981,12 +9045,14 @@
       </c>
       <c r="AA74" t="inlineStr">
         <is>
-          <t>2023-07-22 - Baltimore Orioles @ Tampa Bay Rays (Scheduled)</t>
+          <t>2023-07-22 - Baltimore Orioles (6) @ Tampa Bay Rays (5) (Final)</t>
         </is>
       </c>
     </row>
     <row r="75">
-      <c r="A75" t="inlineStr"/>
+      <c r="A75" t="n">
+        <v>1</v>
+      </c>
       <c r="B75" t="inlineStr">
         <is>
           <t>2023-07-22</t>
@@ -9032,30 +9098,38 @@
           <t>mlb3year</t>
         </is>
       </c>
-      <c r="K75" t="inlineStr">
-        <is>
-          <t>+125</t>
-        </is>
+      <c r="K75" t="n">
+        <v>125</v>
       </c>
       <c r="L75" t="inlineStr">
         <is>
           <t>BetUS</t>
         </is>
       </c>
-      <c r="M75" t="inlineStr">
-        <is>
-          <t>-133</t>
-        </is>
+      <c r="M75" t="n">
+        <v>-133</v>
       </c>
       <c r="N75" t="inlineStr">
         <is>
           <t>BetOnline.ag</t>
         </is>
       </c>
-      <c r="O75" t="inlineStr"/>
-      <c r="P75" t="inlineStr"/>
-      <c r="Q75" t="inlineStr"/>
-      <c r="R75" t="inlineStr"/>
+      <c r="O75" t="n">
+        <v>9</v>
+      </c>
+      <c r="P75" t="n">
+        <v>8</v>
+      </c>
+      <c r="Q75" t="inlineStr">
+        <is>
+          <t>Isaiah Campbell</t>
+        </is>
+      </c>
+      <c r="R75" t="inlineStr">
+        <is>
+          <t>Nate Pearson</t>
+        </is>
+      </c>
       <c r="S75" t="n">
         <v>0.8520667952673416</v>
       </c>
@@ -9071,10 +9145,10 @@
         </is>
       </c>
       <c r="W75" s="2" t="n">
-        <v>45129.34648221559</v>
+        <v>45129.34648221065</v>
       </c>
       <c r="X75" s="2" t="n">
-        <v>45129.34685949393</v>
+        <v>45129.34685949074</v>
       </c>
       <c r="Y75" t="inlineStr">
         <is>
@@ -9086,12 +9160,14 @@
       </c>
       <c r="AA75" t="inlineStr">
         <is>
-          <t>2023-07-22 - Toronto Blue Jays @ Seattle Mariners (Scheduled)</t>
+          <t>2023-07-22 - Toronto Blue Jays (8) @ Seattle Mariners (9) (Final)</t>
         </is>
       </c>
     </row>
     <row r="76">
-      <c r="A76" t="inlineStr"/>
+      <c r="A76" t="n">
+        <v>1</v>
+      </c>
       <c r="B76" t="inlineStr">
         <is>
           <t>2023-07-22</t>
@@ -9133,30 +9209,38 @@
           <t>mlb3year</t>
         </is>
       </c>
-      <c r="K76" t="inlineStr">
-        <is>
-          <t>+125</t>
-        </is>
+      <c r="K76" t="n">
+        <v>125</v>
       </c>
       <c r="L76" t="inlineStr">
         <is>
           <t>BetUS</t>
         </is>
       </c>
-      <c r="M76" t="inlineStr">
-        <is>
-          <t>-130</t>
-        </is>
+      <c r="M76" t="n">
+        <v>-130</v>
       </c>
       <c r="N76" t="inlineStr">
         <is>
           <t>LowVig.ag</t>
         </is>
       </c>
-      <c r="O76" t="inlineStr"/>
-      <c r="P76" t="inlineStr"/>
-      <c r="Q76" t="inlineStr"/>
-      <c r="R76" t="inlineStr"/>
+      <c r="O76" t="n">
+        <v>3</v>
+      </c>
+      <c r="P76" t="n">
+        <v>14</v>
+      </c>
+      <c r="Q76" t="inlineStr">
+        <is>
+          <t>Jackson Wolf</t>
+        </is>
+      </c>
+      <c r="R76" t="inlineStr">
+        <is>
+          <t>Mason Englert</t>
+        </is>
+      </c>
       <c r="S76" t="n">
         <v>0.3239182628947005</v>
       </c>
@@ -9172,10 +9256,10 @@
         </is>
       </c>
       <c r="W76" s="2" t="n">
-        <v>45129.34648221559</v>
+        <v>45129.34648221065</v>
       </c>
       <c r="X76" s="2" t="n">
-        <v>45129.34691105314</v>
+        <v>45129.34691105324</v>
       </c>
       <c r="Y76" t="inlineStr">
         <is>
@@ -9187,12 +9271,14 @@
       </c>
       <c r="AA76" t="inlineStr">
         <is>
-          <t>2023-07-22 - San Diego Padres @ Detroit Tigers (Scheduled)</t>
+          <t>2023-07-22 - San Diego Padres (14) @ Detroit Tigers (3) (Final)</t>
         </is>
       </c>
     </row>
     <row r="77">
-      <c r="A77" t="inlineStr"/>
+      <c r="A77" t="n">
+        <v>0</v>
+      </c>
       <c r="B77" t="inlineStr">
         <is>
           <t>2023-07-22</t>
@@ -9238,30 +9324,38 @@
           <t>mlb3year</t>
         </is>
       </c>
-      <c r="K77" t="inlineStr">
-        <is>
-          <t>+168</t>
-        </is>
+      <c r="K77" t="n">
+        <v>168</v>
       </c>
       <c r="L77" t="inlineStr">
         <is>
           <t>WynnBET</t>
         </is>
       </c>
-      <c r="M77" t="inlineStr">
-        <is>
-          <t>-180</t>
-        </is>
+      <c r="M77" t="n">
+        <v>-180</v>
       </c>
       <c r="N77" t="inlineStr">
         <is>
           <t>DraftKings</t>
         </is>
       </c>
-      <c r="O77" t="inlineStr"/>
-      <c r="P77" t="inlineStr"/>
-      <c r="Q77" t="inlineStr"/>
-      <c r="R77" t="inlineStr"/>
+      <c r="O77" t="n">
+        <v>10</v>
+      </c>
+      <c r="P77" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q77" t="inlineStr">
+        <is>
+          <t>Josiah Gray</t>
+        </is>
+      </c>
+      <c r="R77" t="inlineStr">
+        <is>
+          <t>Logan Webb</t>
+        </is>
+      </c>
       <c r="S77" t="n">
         <v>0.4374312792395386</v>
       </c>
@@ -9277,10 +9371,10 @@
         </is>
       </c>
       <c r="W77" s="2" t="n">
-        <v>45129.34648221559</v>
+        <v>45129.34648221065</v>
       </c>
       <c r="X77" s="2" t="n">
-        <v>45129.34697167146</v>
+        <v>45129.34697166667</v>
       </c>
       <c r="Y77" t="inlineStr">
         <is>
@@ -9292,12 +9386,14 @@
       </c>
       <c r="AA77" t="inlineStr">
         <is>
-          <t>2023-07-22 - San Francisco Giants @ Washington Nationals (Scheduled)</t>
+          <t>2023-07-22 - San Francisco Giants (1) @ Washington Nationals (10) (Final)</t>
         </is>
       </c>
     </row>
     <row r="78">
-      <c r="A78" t="inlineStr"/>
+      <c r="A78" t="n">
+        <v>0</v>
+      </c>
       <c r="B78" t="inlineStr">
         <is>
           <t>2023-07-22</t>
@@ -9343,30 +9439,38 @@
           <t>mlb3year</t>
         </is>
       </c>
-      <c r="K78" t="inlineStr">
-        <is>
-          <t>-115</t>
-        </is>
+      <c r="K78" t="n">
+        <v>-115</v>
       </c>
       <c r="L78" t="inlineStr">
         <is>
           <t>BetUS</t>
         </is>
       </c>
-      <c r="M78" t="inlineStr">
-        <is>
-          <t>+110</t>
-        </is>
+      <c r="M78" t="n">
+        <v>110</v>
       </c>
       <c r="N78" t="inlineStr">
         <is>
           <t>BetRivers</t>
         </is>
       </c>
-      <c r="O78" t="inlineStr"/>
-      <c r="P78" t="inlineStr"/>
-      <c r="Q78" t="inlineStr"/>
-      <c r="R78" t="inlineStr"/>
+      <c r="O78" t="n">
+        <v>8</v>
+      </c>
+      <c r="P78" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q78" t="inlineStr">
+        <is>
+          <t>James Paxton</t>
+        </is>
+      </c>
+      <c r="R78" t="inlineStr">
+        <is>
+          <t>Max Scherzer</t>
+        </is>
+      </c>
       <c r="S78" t="n">
         <v>0.01136361134537548</v>
       </c>
@@ -9382,10 +9486,10 @@
         </is>
       </c>
       <c r="W78" s="2" t="n">
-        <v>45129.34648221559</v>
+        <v>45129.34648221065</v>
       </c>
       <c r="X78" s="2" t="n">
-        <v>45129.34704088674</v>
+        <v>45129.3470408912</v>
       </c>
       <c r="Y78" t="inlineStr">
         <is>
@@ -9397,12 +9501,14 @@
       </c>
       <c r="AA78" t="inlineStr">
         <is>
-          <t>2023-07-22 - New York Mets @ Boston Red Sox (Scheduled)</t>
+          <t>2023-07-22 - New York Mets (6) @ Boston Red Sox (8) (Final)</t>
         </is>
       </c>
     </row>
     <row r="79">
-      <c r="A79" t="inlineStr"/>
+      <c r="A79" t="n">
+        <v>0</v>
+      </c>
       <c r="B79" t="inlineStr">
         <is>
           <t>2023-07-22</t>
@@ -9448,30 +9554,38 @@
           <t>mlb3year</t>
         </is>
       </c>
-      <c r="K79" t="inlineStr">
-        <is>
-          <t>+110</t>
-        </is>
+      <c r="K79" t="n">
+        <v>110</v>
       </c>
       <c r="L79" t="inlineStr">
         <is>
           <t>WynnBET</t>
         </is>
       </c>
-      <c r="M79" t="inlineStr">
-        <is>
-          <t>-118</t>
-        </is>
+      <c r="M79" t="n">
+        <v>-118</v>
       </c>
       <c r="N79" t="inlineStr">
         <is>
           <t>LowVig.ag</t>
         </is>
       </c>
-      <c r="O79" t="inlineStr"/>
-      <c r="P79" t="inlineStr"/>
-      <c r="Q79" t="inlineStr"/>
-      <c r="R79" t="inlineStr"/>
+      <c r="O79" t="n">
+        <v>1</v>
+      </c>
+      <c r="P79" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q79" t="inlineStr">
+        <is>
+          <t>Tanner Bibee</t>
+        </is>
+      </c>
+      <c r="R79" t="inlineStr">
+        <is>
+          <t>Zack Wheeler</t>
+        </is>
+      </c>
       <c r="S79" t="n">
         <v>0.3800097137373824</v>
       </c>
@@ -9487,10 +9601,10 @@
         </is>
       </c>
       <c r="W79" s="2" t="n">
-        <v>45129.34648221559</v>
+        <v>45129.34648221065</v>
       </c>
       <c r="X79" s="2" t="n">
-        <v>45129.34709737662</v>
+        <v>45129.34709737269</v>
       </c>
       <c r="Y79" t="inlineStr">
         <is>
@@ -9502,12 +9616,14 @@
       </c>
       <c r="AA79" t="inlineStr">
         <is>
-          <t>2023-07-22 - Philadelphia Phillies @ Cleveland Guardians (Scheduled)</t>
+          <t>2023-07-22 - Philadelphia Phillies (0) @ Cleveland Guardians (1) (Final)</t>
         </is>
       </c>
     </row>
     <row r="80">
-      <c r="A80" t="inlineStr"/>
+      <c r="A80" t="n">
+        <v>0</v>
+      </c>
       <c r="B80" t="inlineStr">
         <is>
           <t>2023-07-22</t>
@@ -9553,30 +9669,38 @@
           <t>mlb3year</t>
         </is>
       </c>
-      <c r="K80" t="inlineStr">
-        <is>
-          <t>+123</t>
-        </is>
+      <c r="K80" t="n">
+        <v>123</v>
       </c>
       <c r="L80" t="inlineStr">
         <is>
           <t>BetUS</t>
         </is>
       </c>
-      <c r="M80" t="inlineStr">
-        <is>
-          <t>-133</t>
-        </is>
+      <c r="M80" t="n">
+        <v>-133</v>
       </c>
       <c r="N80" t="inlineStr">
         <is>
           <t>BetOnline.ag</t>
         </is>
       </c>
-      <c r="O80" t="inlineStr"/>
-      <c r="P80" t="inlineStr"/>
-      <c r="Q80" t="inlineStr"/>
-      <c r="R80" t="inlineStr"/>
+      <c r="O80" t="n">
+        <v>4</v>
+      </c>
+      <c r="P80" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q80" t="inlineStr">
+        <is>
+          <t>Joel Payamps</t>
+        </is>
+      </c>
+      <c r="R80" t="inlineStr">
+        <is>
+          <t>Joe Jimenez</t>
+        </is>
+      </c>
       <c r="S80" t="n">
         <v>0.008889384686767825</v>
       </c>
@@ -9596,10 +9720,10 @@
         </is>
       </c>
       <c r="W80" s="2" t="n">
-        <v>45129.34648221559</v>
+        <v>45129.34648221065</v>
       </c>
       <c r="X80" s="2" t="n">
-        <v>45129.34714766181</v>
+        <v>45129.34714766204</v>
       </c>
       <c r="Y80" t="inlineStr">
         <is>
@@ -9611,12 +9735,14 @@
       </c>
       <c r="AA80" t="inlineStr">
         <is>
-          <t>2023-07-22 - Atlanta Braves @ Milwaukee Brewers (Scheduled)</t>
+          <t>2023-07-22 - Atlanta Braves (3) @ Milwaukee Brewers (4) (Final)</t>
         </is>
       </c>
     </row>
     <row r="81">
-      <c r="A81" t="inlineStr"/>
+      <c r="A81" t="n">
+        <v>0</v>
+      </c>
       <c r="B81" t="inlineStr">
         <is>
           <t>2023-07-22</t>
@@ -9662,30 +9788,38 @@
           <t>mlb3year</t>
         </is>
       </c>
-      <c r="K81" t="inlineStr">
-        <is>
-          <t>-133</t>
-        </is>
+      <c r="K81" t="n">
+        <v>-133</v>
       </c>
       <c r="L81" t="inlineStr">
         <is>
           <t>WynnBET</t>
         </is>
       </c>
-      <c r="M81" t="inlineStr">
-        <is>
-          <t>+125</t>
-        </is>
+      <c r="M81" t="n">
+        <v>125</v>
       </c>
       <c r="N81" t="inlineStr">
         <is>
           <t>BetUS</t>
         </is>
       </c>
-      <c r="O81" t="inlineStr"/>
-      <c r="P81" t="inlineStr"/>
-      <c r="Q81" t="inlineStr"/>
-      <c r="R81" t="inlineStr"/>
+      <c r="O81" t="n">
+        <v>3</v>
+      </c>
+      <c r="P81" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q81" t="inlineStr">
+        <is>
+          <t>Jordan Balazovic</t>
+        </is>
+      </c>
+      <c r="R81" t="inlineStr">
+        <is>
+          <t>Keynan Middleton</t>
+        </is>
+      </c>
       <c r="S81" t="n">
         <v>0.002727569814304598</v>
       </c>
@@ -9701,10 +9835,10 @@
         </is>
       </c>
       <c r="W81" s="2" t="n">
-        <v>45129.34648221559</v>
+        <v>45129.34648221065</v>
       </c>
       <c r="X81" s="2" t="n">
-        <v>45129.34721555199</v>
+        <v>45129.34721555556</v>
       </c>
       <c r="Y81" t="inlineStr">
         <is>
@@ -9716,7 +9850,7 @@
       </c>
       <c r="AA81" t="inlineStr">
         <is>
-          <t>2023-07-22 - Chicago White Sox @ Minnesota Twins (Scheduled)</t>
+          <t>2023-07-22 - Chicago White Sox (2) @ Minnesota Twins (3) (Final)</t>
         </is>
       </c>
     </row>
@@ -9724,42 +9858,42 @@
       <c r="A82" t="inlineStr"/>
       <c r="B82" t="inlineStr">
         <is>
-          <t>2023-07-22</t>
+          <t>2023-07-23</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>09:07 pm</t>
+          <t>12:05 pm</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>Oakland Athletics</t>
+          <t>Detroit Tigers</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>Paul Blackburn</t>
+          <t>Alex Faedo</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>Houston Astros</t>
+          <t>San Diego Padres</t>
         </is>
       </c>
       <c r="G82" t="inlineStr">
         <is>
-          <t>Cristian Javier</t>
+          <t>Joe Musgrove</t>
         </is>
       </c>
       <c r="H82" t="inlineStr">
         <is>
-          <t>Oakland Athletics</t>
+          <t>San Diego Padres</t>
         </is>
       </c>
       <c r="I82" t="inlineStr">
         <is>
-          <t>Houston Astros</t>
+          <t>San Diego Padres</t>
         </is>
       </c>
       <c r="J82" t="inlineStr">
@@ -9769,22 +9903,22 @@
       </c>
       <c r="K82" t="inlineStr">
         <is>
-          <t>+176</t>
+          <t>+203</t>
         </is>
       </c>
       <c r="L82" t="inlineStr">
         <is>
+          <t>WynnBET</t>
+        </is>
+      </c>
+      <c r="M82" t="inlineStr">
+        <is>
+          <t>-225</t>
+        </is>
+      </c>
+      <c r="N82" t="inlineStr">
+        <is>
           <t>LowVig.ag</t>
-        </is>
-      </c>
-      <c r="M82" t="inlineStr">
-        <is>
-          <t>-189</t>
-        </is>
-      </c>
-      <c r="N82" t="inlineStr">
-        <is>
-          <t>WynnBET</t>
         </is>
       </c>
       <c r="O82" t="inlineStr"/>
@@ -9792,36 +9926,40 @@
       <c r="Q82" t="inlineStr"/>
       <c r="R82" t="inlineStr"/>
       <c r="S82" t="n">
-        <v>0.9994406981813074</v>
+        <v>0.08556238710565602</v>
       </c>
       <c r="T82" t="inlineStr">
         <is>
-          <t>Oakland Coliseum</t>
-        </is>
-      </c>
-      <c r="U82" t="inlineStr"/>
+          <t>Comerica Park</t>
+        </is>
+      </c>
+      <c r="U82" t="inlineStr">
+        <is>
+          <t>SD leads 2-0</t>
+        </is>
+      </c>
       <c r="V82" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>['Peacock']</t>
         </is>
       </c>
       <c r="W82" s="2" t="n">
-        <v>45129.34648221559</v>
+        <v>45130.30951167133</v>
       </c>
       <c r="X82" s="2" t="n">
-        <v>45129.34727540473</v>
+        <v>45130.3095808662</v>
       </c>
       <c r="Y82" t="inlineStr">
         <is>
-          <t>2023-07-23T01:07:00Z</t>
+          <t>2023-07-23T16:05:00Z</t>
         </is>
       </c>
       <c r="Z82" t="n">
-        <v>717295</v>
+        <v>717288</v>
       </c>
       <c r="AA82" t="inlineStr">
         <is>
-          <t>2023-07-22 - Houston Astros @ Oakland Athletics (Scheduled)</t>
+          <t>2023-07-23 - San Diego Padres @ Detroit Tigers (Scheduled)</t>
         </is>
       </c>
     </row>
@@ -9829,42 +9967,42 @@
       <c r="A83" t="inlineStr"/>
       <c r="B83" t="inlineStr">
         <is>
-          <t>2023-07-22</t>
+          <t>2023-07-23</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>09:07 pm</t>
+          <t>01:35 pm</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>Los Angeles Angels</t>
+          <t>New York Yankees</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>Reid Detmers</t>
+          <t>Luis Severino</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>Pittsburgh Pirates</t>
+          <t>Kansas City Royals</t>
         </is>
       </c>
       <c r="G83" t="inlineStr">
         <is>
-          <t>Ryan Borucki</t>
+          <t>Jordan Lyles</t>
         </is>
       </c>
       <c r="H83" t="inlineStr">
         <is>
-          <t>Pittsburgh Pirates</t>
+          <t>New York Yankees</t>
         </is>
       </c>
       <c r="I83" t="inlineStr">
         <is>
-          <t>Los Angeles Angels</t>
+          <t>New York Yankees</t>
         </is>
       </c>
       <c r="J83" t="inlineStr">
@@ -9874,22 +10012,22 @@
       </c>
       <c r="K83" t="inlineStr">
         <is>
-          <t>-178</t>
+          <t>-189</t>
         </is>
       </c>
       <c r="L83" t="inlineStr">
         <is>
-          <t>LowVig.ag</t>
+          <t>BetOnline.ag</t>
         </is>
       </c>
       <c r="M83" t="inlineStr">
         <is>
-          <t>+171</t>
+          <t>+175</t>
         </is>
       </c>
       <c r="N83" t="inlineStr">
         <is>
-          <t>WynnBET</t>
+          <t>Unibet</t>
         </is>
       </c>
       <c r="O83" t="inlineStr"/>
@@ -9897,40 +10035,1421 @@
       <c r="Q83" t="inlineStr"/>
       <c r="R83" t="inlineStr"/>
       <c r="S83" t="n">
-        <v>0.001427805428936317</v>
+        <v>0.7820568232615434</v>
       </c>
       <c r="T83" t="inlineStr">
         <is>
+          <t>Yankee Stadium</t>
+        </is>
+      </c>
+      <c r="U83" t="inlineStr"/>
+      <c r="V83" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="W83" s="2" t="n">
+        <v>45130.30951167133</v>
+      </c>
+      <c r="X83" s="2" t="n">
+        <v>45130.30964013565</v>
+      </c>
+      <c r="Y83" t="inlineStr">
+        <is>
+          <t>2023-07-23T17:35:00Z</t>
+        </is>
+      </c>
+      <c r="Z83" t="n">
+        <v>717294</v>
+      </c>
+      <c r="AA83" t="inlineStr">
+        <is>
+          <t>2023-07-23 - Kansas City Royals @ New York Yankees (Scheduled)</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr"/>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>2023-07-23</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>01:35 pm</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>Washington Nationals</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>MacKenzie Gore</t>
+        </is>
+      </c>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>San Francisco Giants</t>
+        </is>
+      </c>
+      <c r="G84" t="inlineStr"/>
+      <c r="H84" t="inlineStr">
+        <is>
+          <t>San Francisco Giants</t>
+        </is>
+      </c>
+      <c r="I84" t="inlineStr">
+        <is>
+          <t>San Francisco Giants</t>
+        </is>
+      </c>
+      <c r="J84" t="inlineStr">
+        <is>
+          <t>mlb3year</t>
+        </is>
+      </c>
+      <c r="K84" t="inlineStr">
+        <is>
+          <t>+110</t>
+        </is>
+      </c>
+      <c r="L84" t="inlineStr">
+        <is>
+          <t>BetUS</t>
+        </is>
+      </c>
+      <c r="M84" t="inlineStr">
+        <is>
+          <t>-115</t>
+        </is>
+      </c>
+      <c r="N84" t="inlineStr">
+        <is>
+          <t>DraftKings</t>
+        </is>
+      </c>
+      <c r="O84" t="inlineStr"/>
+      <c r="P84" t="inlineStr"/>
+      <c r="Q84" t="inlineStr"/>
+      <c r="R84" t="inlineStr"/>
+      <c r="S84" t="n">
+        <v>0.4061467604806184</v>
+      </c>
+      <c r="T84" t="inlineStr">
+        <is>
+          <t>Nationals Park</t>
+        </is>
+      </c>
+      <c r="U84" t="inlineStr"/>
+      <c r="V84" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="W84" s="2" t="n">
+        <v>45130.30951167133</v>
+      </c>
+      <c r="X84" s="2" t="n">
+        <v>45130.30970727849</v>
+      </c>
+      <c r="Y84" t="inlineStr">
+        <is>
+          <t>2023-07-23T17:35:00Z</t>
+        </is>
+      </c>
+      <c r="Z84" t="n">
+        <v>717290</v>
+      </c>
+      <c r="AA84" t="inlineStr">
+        <is>
+          <t>2023-07-23 - San Francisco Giants @ Washington Nationals (Scheduled)</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr"/>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>2023-07-23</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>01:40 pm</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>Cincinnati Reds</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>Luke Weaver</t>
+        </is>
+      </c>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>Arizona Diamondbacks</t>
+        </is>
+      </c>
+      <c r="G85" t="inlineStr">
+        <is>
+          <t>Jose Ruiz</t>
+        </is>
+      </c>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t>Arizona Diamondbacks</t>
+        </is>
+      </c>
+      <c r="I85" t="inlineStr">
+        <is>
+          <t>Arizona Diamondbacks</t>
+        </is>
+      </c>
+      <c r="J85" t="inlineStr">
+        <is>
+          <t>mlb3year</t>
+        </is>
+      </c>
+      <c r="K85" t="inlineStr">
+        <is>
+          <t>-103</t>
+        </is>
+      </c>
+      <c r="L85" t="inlineStr">
+        <is>
+          <t>BetOnline.ag</t>
+        </is>
+      </c>
+      <c r="M85" t="inlineStr">
+        <is>
+          <t>-103</t>
+        </is>
+      </c>
+      <c r="N85" t="inlineStr">
+        <is>
+          <t>WynnBET</t>
+        </is>
+      </c>
+      <c r="O85" t="inlineStr"/>
+      <c r="P85" t="inlineStr"/>
+      <c r="Q85" t="inlineStr"/>
+      <c r="R85" t="inlineStr"/>
+      <c r="S85" t="n">
+        <v>0.04959668005893381</v>
+      </c>
+      <c r="T85" t="inlineStr">
+        <is>
+          <t>Great American Ball Park</t>
+        </is>
+      </c>
+      <c r="U85" t="inlineStr">
+        <is>
+          <t>CIN leads 2-0</t>
+        </is>
+      </c>
+      <c r="V85" t="inlineStr">
+        <is>
+          <t>['MLB.tv Free Game']</t>
+        </is>
+      </c>
+      <c r="W85" s="2" t="n">
+        <v>45130.30951167133</v>
+      </c>
+      <c r="X85" s="2" t="n">
+        <v>45130.30976610965</v>
+      </c>
+      <c r="Y85" t="inlineStr">
+        <is>
+          <t>2023-07-23T17:40:00Z</t>
+        </is>
+      </c>
+      <c r="Z85" t="n">
+        <v>717289</v>
+      </c>
+      <c r="AA85" t="inlineStr">
+        <is>
+          <t>2023-07-23 - Arizona Diamondbacks @ Cincinnati Reds (Scheduled)</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr"/>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>2023-07-23</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>01:40 pm</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>Tampa Bay Rays</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>Taj Bradley</t>
+        </is>
+      </c>
+      <c r="F86" t="inlineStr">
+        <is>
+          <t>Baltimore Orioles</t>
+        </is>
+      </c>
+      <c r="G86" t="inlineStr">
+        <is>
+          <t>Tyler Wells</t>
+        </is>
+      </c>
+      <c r="H86" t="inlineStr">
+        <is>
+          <t>Baltimore Orioles</t>
+        </is>
+      </c>
+      <c r="I86" t="inlineStr">
+        <is>
+          <t>Tampa Bay Rays</t>
+        </is>
+      </c>
+      <c r="J86" t="inlineStr">
+        <is>
+          <t>mlb3year</t>
+        </is>
+      </c>
+      <c r="K86" t="inlineStr">
+        <is>
+          <t>-130</t>
+        </is>
+      </c>
+      <c r="L86" t="inlineStr">
+        <is>
+          <t>WynnBET</t>
+        </is>
+      </c>
+      <c r="M86" t="inlineStr">
+        <is>
+          <t>+126</t>
+        </is>
+      </c>
+      <c r="N86" t="inlineStr">
+        <is>
+          <t>FanDuel</t>
+        </is>
+      </c>
+      <c r="O86" t="inlineStr"/>
+      <c r="P86" t="inlineStr"/>
+      <c r="Q86" t="inlineStr"/>
+      <c r="R86" t="inlineStr"/>
+      <c r="S86" t="n">
+        <v>0.001216818941118575</v>
+      </c>
+      <c r="T86" t="inlineStr">
+        <is>
+          <t>Tropicana Field</t>
+        </is>
+      </c>
+      <c r="U86" t="inlineStr"/>
+      <c r="V86" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="W86" s="2" t="n">
+        <v>45130.30951167133</v>
+      </c>
+      <c r="X86" s="2" t="n">
+        <v>45130.3098271456</v>
+      </c>
+      <c r="Y86" t="inlineStr">
+        <is>
+          <t>2023-07-23T17:40:00Z</t>
+        </is>
+      </c>
+      <c r="Z86" t="n">
+        <v>717291</v>
+      </c>
+      <c r="AA86" t="inlineStr">
+        <is>
+          <t>2023-07-23 - Baltimore Orioles @ Tampa Bay Rays (Scheduled)</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr"/>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>2023-07-23</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>01:40 pm</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>Cleveland Guardians</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>Xzavion Curry</t>
+        </is>
+      </c>
+      <c r="F87" t="inlineStr">
+        <is>
+          <t>Philadelphia Phillies</t>
+        </is>
+      </c>
+      <c r="G87" t="inlineStr">
+        <is>
+          <t>Aaron Nola</t>
+        </is>
+      </c>
+      <c r="H87" t="inlineStr">
+        <is>
+          <t>Cleveland Guardians</t>
+        </is>
+      </c>
+      <c r="I87" t="inlineStr">
+        <is>
+          <t>Philadelphia Phillies</t>
+        </is>
+      </c>
+      <c r="J87" t="inlineStr">
+        <is>
+          <t>mlb3year</t>
+        </is>
+      </c>
+      <c r="K87" t="inlineStr">
+        <is>
+          <t>+131</t>
+        </is>
+      </c>
+      <c r="L87" t="inlineStr">
+        <is>
+          <t>LowVig.ag</t>
+        </is>
+      </c>
+      <c r="M87" t="inlineStr">
+        <is>
+          <t>-137</t>
+        </is>
+      </c>
+      <c r="N87" t="inlineStr">
+        <is>
+          <t>BetRivers</t>
+        </is>
+      </c>
+      <c r="O87" t="inlineStr"/>
+      <c r="P87" t="inlineStr"/>
+      <c r="Q87" t="inlineStr"/>
+      <c r="R87" t="inlineStr"/>
+      <c r="S87" t="n">
+        <v>0.5495487940049334</v>
+      </c>
+      <c r="T87" t="inlineStr">
+        <is>
+          <t>Progressive Field</t>
+        </is>
+      </c>
+      <c r="U87" t="inlineStr">
+        <is>
+          <t>CLE leads 2-0</t>
+        </is>
+      </c>
+      <c r="V87" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="W87" s="2" t="n">
+        <v>45130.30951167133</v>
+      </c>
+      <c r="X87" s="2" t="n">
+        <v>45130.30989982719</v>
+      </c>
+      <c r="Y87" t="inlineStr">
+        <is>
+          <t>2023-07-23T17:40:00Z</t>
+        </is>
+      </c>
+      <c r="Z87" t="n">
+        <v>717283</v>
+      </c>
+      <c r="AA87" t="inlineStr">
+        <is>
+          <t>2023-07-23 - Philadelphia Phillies @ Cleveland Guardians (Scheduled)</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr"/>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>2023-07-23</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>01:40 pm</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>Miami Marlins</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>Jesus Luzardo</t>
+        </is>
+      </c>
+      <c r="F88" t="inlineStr">
+        <is>
+          <t>Colorado Rockies</t>
+        </is>
+      </c>
+      <c r="G88" t="inlineStr">
+        <is>
+          <t>Ty Blach</t>
+        </is>
+      </c>
+      <c r="H88" t="inlineStr">
+        <is>
+          <t>Colorado Rockies</t>
+        </is>
+      </c>
+      <c r="I88" t="inlineStr">
+        <is>
+          <t>Miami Marlins</t>
+        </is>
+      </c>
+      <c r="J88" t="inlineStr">
+        <is>
+          <t>mlb3year</t>
+        </is>
+      </c>
+      <c r="K88" t="inlineStr">
+        <is>
+          <t>-250</t>
+        </is>
+      </c>
+      <c r="L88" t="inlineStr">
+        <is>
+          <t>BetMGM</t>
+        </is>
+      </c>
+      <c r="M88" t="inlineStr">
+        <is>
+          <t>+240</t>
+        </is>
+      </c>
+      <c r="N88" t="inlineStr">
+        <is>
+          <t>FanDuel</t>
+        </is>
+      </c>
+      <c r="O88" t="inlineStr"/>
+      <c r="P88" t="inlineStr"/>
+      <c r="Q88" t="inlineStr"/>
+      <c r="R88" t="inlineStr"/>
+      <c r="S88" t="n">
+        <v>0.0004062770097038835</v>
+      </c>
+      <c r="T88" t="inlineStr">
+        <is>
+          <t>loanDepot park</t>
+        </is>
+      </c>
+      <c r="U88" t="inlineStr">
+        <is>
+          <t>COL leads 2-0</t>
+        </is>
+      </c>
+      <c r="V88" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="W88" s="2" t="n">
+        <v>45130.30951167133</v>
+      </c>
+      <c r="X88" s="2" t="n">
+        <v>45130.30995271856</v>
+      </c>
+      <c r="Y88" t="inlineStr">
+        <is>
+          <t>2023-07-23T17:40:00Z</t>
+        </is>
+      </c>
+      <c r="Z88" t="n">
+        <v>717292</v>
+      </c>
+      <c r="AA88" t="inlineStr">
+        <is>
+          <t>2023-07-23 - Colorado Rockies @ Miami Marlins (Scheduled)</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr"/>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>2023-07-23</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>02:10 pm</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>Milwaukee Brewers</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>Julio Teheran</t>
+        </is>
+      </c>
+      <c r="F89" t="inlineStr">
+        <is>
+          <t>Atlanta Braves</t>
+        </is>
+      </c>
+      <c r="G89" t="inlineStr">
+        <is>
+          <t>Bryce Elder</t>
+        </is>
+      </c>
+      <c r="H89" t="inlineStr">
+        <is>
+          <t>Atlanta Braves</t>
+        </is>
+      </c>
+      <c r="I89" t="inlineStr">
+        <is>
+          <t>Atlanta Braves</t>
+        </is>
+      </c>
+      <c r="J89" t="inlineStr">
+        <is>
+          <t>mlb3year</t>
+        </is>
+      </c>
+      <c r="K89" t="inlineStr">
+        <is>
+          <t>+154</t>
+        </is>
+      </c>
+      <c r="L89" t="inlineStr">
+        <is>
+          <t>LowVig.ag</t>
+        </is>
+      </c>
+      <c r="M89" t="inlineStr">
+        <is>
+          <t>-164</t>
+        </is>
+      </c>
+      <c r="N89" t="inlineStr">
+        <is>
+          <t>WynnBET</t>
+        </is>
+      </c>
+      <c r="O89" t="inlineStr"/>
+      <c r="P89" t="inlineStr"/>
+      <c r="Q89" t="inlineStr"/>
+      <c r="R89" t="inlineStr"/>
+      <c r="S89" t="n">
+        <v>0.004875185181505377</v>
+      </c>
+      <c r="T89" t="inlineStr">
+        <is>
+          <t>American Family Field</t>
+        </is>
+      </c>
+      <c r="U89" t="inlineStr"/>
+      <c r="V89" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="W89" s="2" t="n">
+        <v>45130.30951167133</v>
+      </c>
+      <c r="X89" s="2" t="n">
+        <v>45130.310021755</v>
+      </c>
+      <c r="Y89" t="inlineStr">
+        <is>
+          <t>2023-07-23T18:10:00Z</t>
+        </is>
+      </c>
+      <c r="Z89" t="n">
+        <v>717287</v>
+      </c>
+      <c r="AA89" t="inlineStr">
+        <is>
+          <t>2023-07-23 - Atlanta Braves @ Milwaukee Brewers (Scheduled)</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr"/>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>2023-07-23</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>02:10 pm</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>Minnesota Twins</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>Bailey Ober</t>
+        </is>
+      </c>
+      <c r="F90" t="inlineStr">
+        <is>
+          <t>Chicago White Sox</t>
+        </is>
+      </c>
+      <c r="G90" t="inlineStr">
+        <is>
+          <t>Lucas Giolito</t>
+        </is>
+      </c>
+      <c r="H90" t="inlineStr">
+        <is>
+          <t>Chicago White Sox</t>
+        </is>
+      </c>
+      <c r="I90" t="inlineStr">
+        <is>
+          <t>Minnesota Twins</t>
+        </is>
+      </c>
+      <c r="J90" t="inlineStr">
+        <is>
+          <t>mlb3year</t>
+        </is>
+      </c>
+      <c r="K90" t="inlineStr">
+        <is>
+          <t>-141</t>
+        </is>
+      </c>
+      <c r="L90" t="inlineStr">
+        <is>
+          <t>WynnBET</t>
+        </is>
+      </c>
+      <c r="M90" t="inlineStr">
+        <is>
+          <t>+132</t>
+        </is>
+      </c>
+      <c r="N90" t="inlineStr">
+        <is>
+          <t>LowVig.ag</t>
+        </is>
+      </c>
+      <c r="O90" t="inlineStr"/>
+      <c r="P90" t="inlineStr"/>
+      <c r="Q90" t="inlineStr"/>
+      <c r="R90" t="inlineStr"/>
+      <c r="S90" t="n">
+        <v>0.004405682690476807</v>
+      </c>
+      <c r="T90" t="inlineStr">
+        <is>
+          <t>Target Field</t>
+        </is>
+      </c>
+      <c r="U90" t="inlineStr"/>
+      <c r="V90" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="W90" s="2" t="n">
+        <v>45130.30951167133</v>
+      </c>
+      <c r="X90" s="2" t="n">
+        <v>45130.31007831867</v>
+      </c>
+      <c r="Y90" t="inlineStr">
+        <is>
+          <t>2023-07-23T18:10:00Z</t>
+        </is>
+      </c>
+      <c r="Z90" t="n">
+        <v>717285</v>
+      </c>
+      <c r="AA90" t="inlineStr">
+        <is>
+          <t>2023-07-23 - Chicago White Sox @ Minnesota Twins (Scheduled)</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr"/>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>2023-07-23</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>02:20 pm</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>Chicago Cubs</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>Jameson Taillon</t>
+        </is>
+      </c>
+      <c r="F91" t="inlineStr">
+        <is>
+          <t>St. Louis Cardinals</t>
+        </is>
+      </c>
+      <c r="G91" t="inlineStr">
+        <is>
+          <t>Jordan Montgomery</t>
+        </is>
+      </c>
+      <c r="H91" t="inlineStr">
+        <is>
+          <t>Chicago Cubs</t>
+        </is>
+      </c>
+      <c r="I91" t="inlineStr">
+        <is>
+          <t>St. Louis Cardinals</t>
+        </is>
+      </c>
+      <c r="J91" t="inlineStr">
+        <is>
+          <t>mlb3year</t>
+        </is>
+      </c>
+      <c r="K91" t="inlineStr">
+        <is>
+          <t>+128</t>
+        </is>
+      </c>
+      <c r="L91" t="inlineStr">
+        <is>
+          <t>BetRivers</t>
+        </is>
+      </c>
+      <c r="M91" t="inlineStr">
+        <is>
+          <t>-135</t>
+        </is>
+      </c>
+      <c r="N91" t="inlineStr">
+        <is>
+          <t>WynnBET</t>
+        </is>
+      </c>
+      <c r="O91" t="inlineStr"/>
+      <c r="P91" t="inlineStr"/>
+      <c r="Q91" t="inlineStr"/>
+      <c r="R91" t="inlineStr"/>
+      <c r="S91" t="n">
+        <v>0.9834489797455822</v>
+      </c>
+      <c r="T91" t="inlineStr">
+        <is>
+          <t>Wrigley Field</t>
+        </is>
+      </c>
+      <c r="U91" t="inlineStr">
+        <is>
+          <t>CHC leads 2-1</t>
+        </is>
+      </c>
+      <c r="V91" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="W91" s="2" t="n">
+        <v>45130.30951167133</v>
+      </c>
+      <c r="X91" s="2" t="n">
+        <v>45130.31014128128</v>
+      </c>
+      <c r="Y91" t="inlineStr">
+        <is>
+          <t>2023-07-23T18:20:00Z</t>
+        </is>
+      </c>
+      <c r="Z91" t="n">
+        <v>717286</v>
+      </c>
+      <c r="AA91" t="inlineStr">
+        <is>
+          <t>2023-07-23 - St. Louis Cardinals @ Chicago Cubs (Scheduled)</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr"/>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>2023-07-23</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>02:35 pm</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>Texas Rangers</t>
+        </is>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>Martin Perez</t>
+        </is>
+      </c>
+      <c r="F92" t="inlineStr">
+        <is>
+          <t>Los Angeles Dodgers</t>
+        </is>
+      </c>
+      <c r="G92" t="inlineStr">
+        <is>
+          <t>Emmet Sheehan</t>
+        </is>
+      </c>
+      <c r="H92" t="inlineStr">
+        <is>
+          <t>Los Angeles Dodgers</t>
+        </is>
+      </c>
+      <c r="I92" t="inlineStr">
+        <is>
+          <t>Los Angeles Dodgers</t>
+        </is>
+      </c>
+      <c r="J92" t="inlineStr">
+        <is>
+          <t>mlb3year</t>
+        </is>
+      </c>
+      <c r="K92" t="inlineStr">
+        <is>
+          <t>+117</t>
+        </is>
+      </c>
+      <c r="L92" t="inlineStr">
+        <is>
+          <t>Unibet</t>
+        </is>
+      </c>
+      <c r="M92" t="inlineStr">
+        <is>
+          <t>-112</t>
+        </is>
+      </c>
+      <c r="N92" t="inlineStr">
+        <is>
+          <t>BetUS</t>
+        </is>
+      </c>
+      <c r="O92" t="inlineStr"/>
+      <c r="P92" t="inlineStr"/>
+      <c r="Q92" t="inlineStr"/>
+      <c r="R92" t="inlineStr"/>
+      <c r="S92" t="n">
+        <v>0.2194162234360617</v>
+      </c>
+      <c r="T92" t="inlineStr">
+        <is>
+          <t>Globe Life Field</t>
+        </is>
+      </c>
+      <c r="U92" t="inlineStr"/>
+      <c r="V92" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="W92" s="2" t="n">
+        <v>45130.30951167133</v>
+      </c>
+      <c r="X92" s="2" t="n">
+        <v>45130.31021316792</v>
+      </c>
+      <c r="Y92" t="inlineStr">
+        <is>
+          <t>2023-07-23T18:35:00Z</t>
+        </is>
+      </c>
+      <c r="Z92" t="n">
+        <v>717284</v>
+      </c>
+      <c r="AA92" t="inlineStr">
+        <is>
+          <t>2023-07-23 - Los Angeles Dodgers @ Texas Rangers (Scheduled)</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr"/>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>2023-07-23</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>04:07 pm</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>Oakland Athletics</t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>Luis Medina</t>
+        </is>
+      </c>
+      <c r="F93" t="inlineStr">
+        <is>
+          <t>Houston Astros</t>
+        </is>
+      </c>
+      <c r="G93" t="inlineStr">
+        <is>
+          <t>Hunter Brown</t>
+        </is>
+      </c>
+      <c r="H93" t="inlineStr">
+        <is>
+          <t>Oakland Athletics</t>
+        </is>
+      </c>
+      <c r="I93" t="inlineStr">
+        <is>
+          <t>Houston Astros</t>
+        </is>
+      </c>
+      <c r="J93" t="inlineStr">
+        <is>
+          <t>mlb3year</t>
+        </is>
+      </c>
+      <c r="K93" t="inlineStr">
+        <is>
+          <t>+203</t>
+        </is>
+      </c>
+      <c r="L93" t="inlineStr">
+        <is>
+          <t>WynnBET</t>
+        </is>
+      </c>
+      <c r="M93" t="inlineStr">
+        <is>
+          <t>-220</t>
+        </is>
+      </c>
+      <c r="N93" t="inlineStr">
+        <is>
+          <t>Barstool Sportsbook</t>
+        </is>
+      </c>
+      <c r="O93" t="inlineStr"/>
+      <c r="P93" t="inlineStr"/>
+      <c r="Q93" t="inlineStr"/>
+      <c r="R93" t="inlineStr"/>
+      <c r="S93" t="n">
+        <v>0.9994069968108991</v>
+      </c>
+      <c r="T93" t="inlineStr">
+        <is>
+          <t>Oakland Coliseum</t>
+        </is>
+      </c>
+      <c r="U93" t="inlineStr">
+        <is>
+          <t>HOU leads 1-0</t>
+        </is>
+      </c>
+      <c r="V93" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="W93" s="2" t="n">
+        <v>45130.30951167133</v>
+      </c>
+      <c r="X93" s="2" t="n">
+        <v>45130.31027692462</v>
+      </c>
+      <c r="Y93" t="inlineStr">
+        <is>
+          <t>2023-07-23T20:07:00Z</t>
+        </is>
+      </c>
+      <c r="Z93" t="n">
+        <v>717279</v>
+      </c>
+      <c r="AA93" t="inlineStr">
+        <is>
+          <t>2023-07-23 - Houston Astros @ Oakland Athletics (Scheduled)</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr"/>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>2023-07-23</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>04:07 pm</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>Los Angeles Angels</t>
+        </is>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>Tyler Anderson</t>
+        </is>
+      </c>
+      <c r="F94" t="inlineStr">
+        <is>
+          <t>Pittsburgh Pirates</t>
+        </is>
+      </c>
+      <c r="G94" t="inlineStr">
+        <is>
+          <t>Mitch Keller</t>
+        </is>
+      </c>
+      <c r="H94" t="inlineStr">
+        <is>
+          <t>Pittsburgh Pirates</t>
+        </is>
+      </c>
+      <c r="I94" t="inlineStr">
+        <is>
+          <t>Los Angeles Angels</t>
+        </is>
+      </c>
+      <c r="J94" t="inlineStr">
+        <is>
+          <t>mlb3year</t>
+        </is>
+      </c>
+      <c r="K94" t="inlineStr">
+        <is>
+          <t>-118</t>
+        </is>
+      </c>
+      <c r="L94" t="inlineStr">
+        <is>
+          <t>FanDuel</t>
+        </is>
+      </c>
+      <c r="M94" t="inlineStr">
+        <is>
+          <t>+112</t>
+        </is>
+      </c>
+      <c r="N94" t="inlineStr">
+        <is>
+          <t>BetUS</t>
+        </is>
+      </c>
+      <c r="O94" t="inlineStr"/>
+      <c r="P94" t="inlineStr"/>
+      <c r="Q94" t="inlineStr"/>
+      <c r="R94" t="inlineStr"/>
+      <c r="S94" t="n">
+        <v>0.1899544495023527</v>
+      </c>
+      <c r="T94" t="inlineStr">
+        <is>
           <t>Angel Stadium</t>
         </is>
       </c>
-      <c r="U83" t="inlineStr">
-        <is>
-          <t>LAA leads 1-0</t>
-        </is>
-      </c>
-      <c r="V83" t="inlineStr">
+      <c r="U94" t="inlineStr"/>
+      <c r="V94" t="inlineStr">
+        <is>
+          <t>['MLB.tv Free Game']</t>
+        </is>
+      </c>
+      <c r="W94" s="2" t="n">
+        <v>45130.30951167133</v>
+      </c>
+      <c r="X94" s="2" t="n">
+        <v>45130.31033271937</v>
+      </c>
+      <c r="Y94" t="inlineStr">
+        <is>
+          <t>2023-07-23T20:07:00Z</t>
+        </is>
+      </c>
+      <c r="Z94" t="n">
+        <v>717278</v>
+      </c>
+      <c r="AA94" t="inlineStr">
+        <is>
+          <t>2023-07-23 - Pittsburgh Pirates @ Los Angeles Angels (Scheduled)</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr"/>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>2023-07-23</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>04:10 pm</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>Seattle Mariners</t>
+        </is>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>Bryan Woo</t>
+        </is>
+      </c>
+      <c r="F95" t="inlineStr">
+        <is>
+          <t>Toronto Blue Jays</t>
+        </is>
+      </c>
+      <c r="G95" t="inlineStr">
+        <is>
+          <t>Alek Manoah</t>
+        </is>
+      </c>
+      <c r="H95" t="inlineStr">
+        <is>
+          <t>Seattle Mariners</t>
+        </is>
+      </c>
+      <c r="I95" t="inlineStr">
+        <is>
+          <t>Seattle Mariners</t>
+        </is>
+      </c>
+      <c r="J95" t="inlineStr">
+        <is>
+          <t>mlb3year</t>
+        </is>
+      </c>
+      <c r="K95" t="inlineStr">
+        <is>
+          <t>-128</t>
+        </is>
+      </c>
+      <c r="L95" t="inlineStr">
+        <is>
+          <t>BetOnline.ag</t>
+        </is>
+      </c>
+      <c r="M95" t="inlineStr">
+        <is>
+          <t>+125</t>
+        </is>
+      </c>
+      <c r="N95" t="inlineStr">
+        <is>
+          <t>BetUS</t>
+        </is>
+      </c>
+      <c r="O95" t="inlineStr"/>
+      <c r="P95" t="inlineStr"/>
+      <c r="Q95" t="inlineStr"/>
+      <c r="R95" t="inlineStr"/>
+      <c r="S95" t="n">
+        <v>0.9993995314244155</v>
+      </c>
+      <c r="T95" t="inlineStr">
+        <is>
+          <t>T-Mobile Park</t>
+        </is>
+      </c>
+      <c r="U95" t="inlineStr"/>
+      <c r="V95" t="inlineStr">
         <is>
           <t>[]</t>
         </is>
       </c>
-      <c r="W83" s="2" t="n">
-        <v>45129.34648221559</v>
-      </c>
-      <c r="X83" s="2" t="n">
-        <v>45129.34732858533</v>
-      </c>
-      <c r="Y83" t="inlineStr">
-        <is>
-          <t>2023-07-23T01:07:00Z</t>
-        </is>
-      </c>
-      <c r="Z83" t="n">
-        <v>717297</v>
-      </c>
-      <c r="AA83" t="inlineStr">
-        <is>
-          <t>2023-07-22 - Pittsburgh Pirates @ Los Angeles Angels (Scheduled)</t>
+      <c r="W95" s="2" t="n">
+        <v>45130.30951167133</v>
+      </c>
+      <c r="X95" s="2" t="n">
+        <v>45130.31041051487</v>
+      </c>
+      <c r="Y95" t="inlineStr">
+        <is>
+          <t>2023-07-23T20:10:00Z</t>
+        </is>
+      </c>
+      <c r="Z95" t="n">
+        <v>717281</v>
+      </c>
+      <c r="AA95" t="inlineStr">
+        <is>
+          <t>2023-07-23 - Toronto Blue Jays @ Seattle Mariners (Scheduled)</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr"/>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>2023-07-23</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>07:10 pm</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>Boston Red Sox</t>
+        </is>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>Brennan Bernardino</t>
+        </is>
+      </c>
+      <c r="F96" t="inlineStr">
+        <is>
+          <t>New York Mets</t>
+        </is>
+      </c>
+      <c r="G96" t="inlineStr">
+        <is>
+          <t>Carlos Carrasco</t>
+        </is>
+      </c>
+      <c r="H96" t="inlineStr">
+        <is>
+          <t>New York Mets</t>
+        </is>
+      </c>
+      <c r="I96" t="inlineStr">
+        <is>
+          <t>Boston Red Sox</t>
+        </is>
+      </c>
+      <c r="J96" t="inlineStr">
+        <is>
+          <t>mlb3year</t>
+        </is>
+      </c>
+      <c r="K96" t="inlineStr">
+        <is>
+          <t>-142</t>
+        </is>
+      </c>
+      <c r="L96" t="inlineStr">
+        <is>
+          <t>BetUS</t>
+        </is>
+      </c>
+      <c r="M96" t="inlineStr">
+        <is>
+          <t>+130</t>
+        </is>
+      </c>
+      <c r="N96" t="inlineStr">
+        <is>
+          <t>LowVig.ag</t>
+        </is>
+      </c>
+      <c r="O96" t="inlineStr"/>
+      <c r="P96" t="inlineStr"/>
+      <c r="Q96" t="inlineStr"/>
+      <c r="R96" t="inlineStr"/>
+      <c r="S96" t="n">
+        <v>0.03620456554568066</v>
+      </c>
+      <c r="T96" t="inlineStr">
+        <is>
+          <t>Fenway Park</t>
+        </is>
+      </c>
+      <c r="U96" t="inlineStr">
+        <is>
+          <t>Series tied 1-1</t>
+        </is>
+      </c>
+      <c r="V96" t="inlineStr">
+        <is>
+          <t>['ESPN']</t>
+        </is>
+      </c>
+      <c r="W96" s="2" t="n">
+        <v>45130.30951167133</v>
+      </c>
+      <c r="X96" s="2" t="n">
+        <v>45130.31047776365</v>
+      </c>
+      <c r="Y96" t="inlineStr">
+        <is>
+          <t>2023-07-23T23:10:00Z</t>
+        </is>
+      </c>
+      <c r="Z96" t="n">
+        <v>717298</v>
+      </c>
+      <c r="AA96" t="inlineStr">
+        <is>
+          <t>2023-07-23 - New York Mets @ Boston Red Sox (Scheduled)</t>
         </is>
       </c>
     </row>

</xml_diff>